<commit_message>
Fix renal substance request types
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -4799,10 +4799,10 @@
   </sheetPr>
   <dimension ref="A1:Q105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B28" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
-      <selection pane="topRight" activeCell="A88" activeCellId="0" sqref="A88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="E40" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+      <selection pane="topRight" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8904,10 +8904,10 @@
   </sheetPr>
   <dimension ref="A1:Q92"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="0" topLeftCell="M73" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A73" activeCellId="0" sqref="A73"/>
-      <selection pane="topRight" activeCell="M73" activeCellId="0" sqref="M73"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="0" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27036,10 +27036,10 @@
   </sheetPr>
   <dimension ref="A1:Q157"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="0" topLeftCell="N103" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A103" activeCellId="0" sqref="A103"/>
-      <selection pane="topRight" activeCell="S140" activeCellId="0" sqref="S140"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="0" topLeftCell="M109" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A109" activeCellId="0" sqref="A109"/>
+      <selection pane="topRight" activeCell="S144" activeCellId="0" sqref="S144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -31403,7 +31403,7 @@
       </c>
       <c r="P109" s="15"/>
       <c r="Q109" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31446,7 +31446,7 @@
       </c>
       <c r="P110" s="15"/>
       <c r="Q110" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31483,7 +31483,7 @@
       </c>
       <c r="P111" s="15"/>
       <c r="Q111" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31526,7 +31526,7 @@
       </c>
       <c r="P112" s="15"/>
       <c r="Q112" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31567,7 +31567,7 @@
       </c>
       <c r="P113" s="15"/>
       <c r="Q113" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31608,7 +31608,7 @@
       </c>
       <c r="P114" s="15"/>
       <c r="Q114" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31649,7 +31649,7 @@
       </c>
       <c r="P115" s="15"/>
       <c r="Q115" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31690,7 +31690,7 @@
       </c>
       <c r="P116" s="15"/>
       <c r="Q116" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31731,7 +31731,7 @@
       </c>
       <c r="P117" s="15"/>
       <c r="Q117" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31772,7 +31772,7 @@
       </c>
       <c r="P118" s="15"/>
       <c r="Q118" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31813,7 +31813,7 @@
       </c>
       <c r="P119" s="15"/>
       <c r="Q119" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31854,7 +31854,7 @@
       </c>
       <c r="P120" s="15"/>
       <c r="Q120" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31895,7 +31895,7 @@
       </c>
       <c r="P121" s="15"/>
       <c r="Q121" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31936,7 +31936,7 @@
       </c>
       <c r="P122" s="15"/>
       <c r="Q122" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -31977,7 +31977,7 @@
       </c>
       <c r="P123" s="15"/>
       <c r="Q123" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="43.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32018,7 +32018,7 @@
       </c>
       <c r="P124" s="15"/>
       <c r="Q124" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32059,7 +32059,7 @@
       </c>
       <c r="P125" s="15"/>
       <c r="Q125" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32100,7 +32100,7 @@
       </c>
       <c r="P126" s="15"/>
       <c r="Q126" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32137,7 +32137,7 @@
       </c>
       <c r="P127" s="15"/>
       <c r="Q127" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32178,7 +32178,7 @@
       </c>
       <c r="P128" s="15"/>
       <c r="Q128" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32217,7 +32217,7 @@
       </c>
       <c r="P129" s="15"/>
       <c r="Q129" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32256,7 +32256,7 @@
       </c>
       <c r="P130" s="15"/>
       <c r="Q130" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32297,7 +32297,7 @@
       </c>
       <c r="P131" s="15"/>
       <c r="Q131" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32338,7 +32338,7 @@
       </c>
       <c r="P132" s="15"/>
       <c r="Q132" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32379,7 +32379,7 @@
       </c>
       <c r="P133" s="15"/>
       <c r="Q133" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32416,7 +32416,7 @@
       </c>
       <c r="P134" s="15"/>
       <c r="Q134" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32457,7 +32457,7 @@
       </c>
       <c r="P135" s="15"/>
       <c r="Q135" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32498,7 +32498,7 @@
       </c>
       <c r="P136" s="15"/>
       <c r="Q136" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32539,7 +32539,7 @@
       </c>
       <c r="P137" s="15"/>
       <c r="Q137" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32580,7 +32580,7 @@
       </c>
       <c r="P138" s="15"/>
       <c r="Q138" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32617,7 +32617,7 @@
       </c>
       <c r="P139" s="15"/>
       <c r="Q139" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32658,7 +32658,7 @@
       </c>
       <c r="P140" s="15"/>
       <c r="Q140" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32699,7 +32699,7 @@
       </c>
       <c r="P141" s="15"/>
       <c r="Q141" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32738,7 +32738,7 @@
       </c>
       <c r="P142" s="15"/>
       <c r="Q142" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32777,7 +32777,7 @@
       </c>
       <c r="P143" s="15"/>
       <c r="Q143" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -32818,7 +32818,7 @@
       </c>
       <c r="P144" s="15"/>
       <c r="Q144" s="15" t="s">
-        <v>359</v>
+        <v>133</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Add PPI back it from conflicts
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F3CB3B-D758-4925-A3D5-8A588D974F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9434C2C0-836B-4550-82C0-CEDE3A926AFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="28800" windowHeight="16920" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6662" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6670" uniqueCount="1193">
   <si>
     <t>Patient Inputs</t>
   </si>
@@ -3746,6 +3746,15 @@
   </si>
   <si>
     <t>Urea-IntracellularMolarity*</t>
+  </si>
+  <si>
+    <t>PeripheralPerfusionIndex</t>
+  </si>
+  <si>
+    <t>[0.029,0.062]</t>
+  </si>
+  <si>
+    <t>savastano2021post</t>
   </si>
 </sst>
 </file>
@@ -16714,11 +16723,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AMJ111"/>
+  <dimension ref="A1:AMJ112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -17012,7 +17021,7 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="20">
-        <f>F42*60</f>
+        <f>F43*60</f>
         <v>672</v>
       </c>
       <c r="G7" s="17" t="s">
@@ -17592,7 +17601,7 @@
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="52">
-        <f>F103</f>
+        <f>F104</f>
         <v>4.666666666666667</v>
       </c>
       <c r="G22" s="8" t="s">
@@ -17619,83 +17628,77 @@
       </c>
       <c r="R22" s="32"/>
     </row>
-    <row r="23" spans="1:18" ht="24">
-      <c r="A23" s="48" t="s">
-        <v>316</v>
+    <row r="23" spans="1:18" s="1" customFormat="1" ht="12">
+      <c r="A23" s="11" t="s">
+        <v>1190</v>
       </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="F23" s="52" t="s">
+        <v>1191</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>1192</v>
+      </c>
       <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="26" t="s">
-        <v>263</v>
-      </c>
+      <c r="I23" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J23" s="4"/>
       <c r="K23" s="8"/>
       <c r="L23" s="49"/>
       <c r="M23" s="5" t="s">
         <v>264</v>
       </c>
       <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
+      <c r="O23" s="5" t="s">
+        <v>142</v>
+      </c>
       <c r="P23" s="4"/>
       <c r="Q23" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="R23" s="32"/>
-    </row>
-    <row r="24" spans="1:18" ht="41.25" customHeight="1">
-      <c r="A24" s="11" t="s">
-        <v>317</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="R23" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="24">
+      <c r="A24" s="48" t="s">
+        <v>316</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17" t="s">
-        <v>318</v>
-      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="K24" s="8"/>
       <c r="L24" s="49"/>
       <c r="M24" s="5" t="s">
         <v>264</v>
       </c>
       <c r="N24" s="5"/>
-      <c r="O24" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="O24" s="5"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="R24" s="32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="24">
+      <c r="R24" s="32"/>
+    </row>
+    <row r="25" spans="1:18" ht="41.25" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>319</v>
-      </c>
-      <c r="B25" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>202</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -17703,21 +17706,21 @@
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="8" t="s">
-        <v>320</v>
+      <c r="F25" s="17" t="s">
+        <v>286</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>322</v>
+        <v>93</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>272</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8" t="s">
-        <v>284</v>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17" t="s">
+        <v>318</v>
       </c>
       <c r="L25" s="49"/>
       <c r="M25" s="5" t="s">
@@ -17731,11 +17734,13 @@
       <c r="Q25" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="R25" s="32"/>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="R25" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="24">
       <c r="A26" s="11" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>202</v>
@@ -17746,17 +17751,21 @@
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="H26" s="8"/>
+        <v>320</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>322</v>
+      </c>
       <c r="I26" s="8" t="s">
         <v>51</v>
       </c>
       <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
+      <c r="K26" s="8" t="s">
+        <v>284</v>
+      </c>
       <c r="L26" s="49"/>
       <c r="M26" s="5" t="s">
         <v>264</v>
@@ -17772,27 +17781,37 @@
       <c r="R26" s="32"/>
     </row>
     <row r="27" spans="1:18">
-      <c r="A27" s="48" t="s">
-        <v>325</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
+      <c r="A27" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
+      <c r="F27" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>287</v>
+      </c>
       <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
+      <c r="I27" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="J27" s="8"/>
-      <c r="K27" s="8" t="s">
-        <v>326</v>
-      </c>
+      <c r="K27" s="8"/>
       <c r="L27" s="49"/>
       <c r="M27" s="5" t="s">
         <v>264</v>
       </c>
       <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
+      <c r="O27" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="32" t="s">
         <v>54</v>
@@ -17801,13 +17820,13 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="48" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="53"/>
+      <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
@@ -17828,95 +17847,81 @@
       <c r="R28" s="32"/>
     </row>
     <row r="29" spans="1:18">
-      <c r="A29" s="11" t="s">
-        <v>328</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="A29" s="48" t="s">
+        <v>327</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H29" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="F29" s="53"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8" t="s">
-        <v>284</v>
+        <v>326</v>
       </c>
       <c r="L29" s="49"/>
       <c r="M29" s="5" t="s">
         <v>264</v>
       </c>
       <c r="N29" s="5"/>
-      <c r="O29" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="O29" s="5"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="32" t="s">
         <v>54</v>
       </c>
       <c r="R29" s="32"/>
     </row>
-    <row r="30" spans="1:18" ht="24">
+    <row r="30" spans="1:18">
       <c r="A30" s="11" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>331</v>
+        <v>202</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="8"/>
-      <c r="F30" s="8">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>15</v>
+      <c r="F30" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="G30" s="17" t="s">
+        <v>93</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>332</v>
+        <v>272</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>51</v>
       </c>
       <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
+      <c r="K30" s="8" t="s">
+        <v>284</v>
+      </c>
       <c r="L30" s="49"/>
       <c r="M30" s="5" t="s">
         <v>264</v>
       </c>
       <c r="N30" s="5"/>
       <c r="O30" s="5" t="s">
-        <v>142</v>
+        <v>73</v>
       </c>
       <c r="P30" s="4"/>
       <c r="Q30" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="R30" s="32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" s="1" customFormat="1" ht="36">
+      <c r="R30" s="32"/>
+    </row>
+    <row r="31" spans="1:18" ht="24">
       <c r="A31" s="11" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>48</v>
@@ -17924,20 +17929,19 @@
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8">
-        <v>0.24</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="I31" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="J31" s="8" t="s">
-        <v>336</v>
-      </c>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
       <c r="L31" s="49"/>
       <c r="M31" s="5" t="s">
         <v>264</v>
@@ -17954,33 +17958,32 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:18" ht="24">
+    <row r="32" spans="1:18" s="1" customFormat="1" ht="36">
       <c r="A32" s="11" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>202</v>
+        <v>334</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
-      <c r="F32" s="8" t="s">
-        <v>338</v>
+      <c r="F32" s="8">
+        <v>0.24</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>339</v>
-      </c>
-      <c r="H32" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>335</v>
+      </c>
       <c r="I32" s="8" t="s">
         <v>51</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>340</v>
-      </c>
-      <c r="K32" s="8" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="L32" s="49"/>
       <c r="M32" s="5" t="s">
@@ -17988,41 +17991,43 @@
       </c>
       <c r="N32" s="5"/>
       <c r="O32" s="5" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="P32" s="4"/>
       <c r="Q32" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="R32" s="32"/>
-    </row>
-    <row r="33" spans="1:18" ht="24" customHeight="1">
+      <c r="R32" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="24">
       <c r="A33" s="11" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>331</v>
+        <v>202</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="52">
-        <v>1</v>
+      <c r="F33" s="8" t="s">
+        <v>338</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>343</v>
-      </c>
+        <v>339</v>
+      </c>
+      <c r="H33" s="8"/>
       <c r="I33" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="J33" s="8"/>
+      <c r="J33" s="8" t="s">
+        <v>340</v>
+      </c>
       <c r="K33" s="8" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="L33" s="49"/>
       <c r="M33" s="5" t="s">
@@ -18036,37 +18041,35 @@
       <c r="Q33" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="R33" s="32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" ht="44.25" customHeight="1">
+      <c r="R33" s="32"/>
+    </row>
+    <row r="34" spans="1:18" ht="24" customHeight="1">
       <c r="A34" s="11" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>202</v>
+        <v>331</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8"/>
-      <c r="F34" s="20" t="s">
-        <v>346</v>
-      </c>
-      <c r="G34" s="17" t="s">
-        <v>93</v>
+      <c r="F34" s="52">
+        <v>1</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>272</v>
+        <v>343</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>51</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="8" t="s">
-        <v>284</v>
+        <v>344</v>
       </c>
       <c r="L34" s="49"/>
       <c r="M34" s="5" t="s">
@@ -18081,12 +18084,12 @@
         <v>54</v>
       </c>
       <c r="R34" s="32">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="44.25" customHeight="1">
       <c r="A35" s="11" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>202</v>
@@ -18096,21 +18099,21 @@
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="20" t="s">
         <v>346</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>348</v>
-      </c>
-      <c r="H35" s="17" t="s">
-        <v>349</v>
+        <v>93</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>272</v>
       </c>
       <c r="I35" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="J35" s="51"/>
-      <c r="K35" s="25" t="s">
-        <v>350</v>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8" t="s">
+        <v>284</v>
       </c>
       <c r="L35" s="49"/>
       <c r="M35" s="5" t="s">
@@ -18130,7 +18133,7 @@
     </row>
     <row r="36" spans="1:18" ht="44.25" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>202</v>
@@ -18141,17 +18144,21 @@
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8" t="s">
-        <v>329</v>
+        <v>346</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>287</v>
-      </c>
-      <c r="H36" s="8"/>
+        <v>348</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>349</v>
+      </c>
       <c r="I36" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="25" t="s">
+        <v>350</v>
+      </c>
       <c r="L36" s="49"/>
       <c r="M36" s="5" t="s">
         <v>264</v>
@@ -18170,29 +18177,27 @@
     </row>
     <row r="37" spans="1:18" ht="44.25" customHeight="1">
       <c r="A37" s="11" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>14</v>
+        <v>202</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
-      <c r="F37" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>15</v>
+      <c r="F37" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>287</v>
       </c>
       <c r="H37" s="8"/>
       <c r="I37" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="J37" s="8" t="s">
-        <v>354</v>
-      </c>
+      <c r="J37" s="8"/>
       <c r="K37" s="8"/>
       <c r="L37" s="49"/>
       <c r="M37" s="5" t="s">
@@ -18206,130 +18211,125 @@
       <c r="Q37" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="R37" s="32"/>
-    </row>
-    <row r="38" spans="1:18">
-      <c r="A38" s="28" t="s">
+      <c r="R37" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="44.25" customHeight="1">
+      <c r="A38" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="K38" s="8"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="R38" s="32"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="28" t="s">
         <v>355</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D39" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E39" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F39" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="G38" s="29" t="s">
+      <c r="G39" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="H38" s="29" t="s">
+      <c r="H39" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="I38" s="9" t="s">
+      <c r="I39" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J39" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="K39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L38" s="29" t="s">
+      <c r="L39" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="M38" s="9" t="s">
+      <c r="M39" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N38" s="9" t="s">
+      <c r="N39" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="O38" s="9" t="s">
+      <c r="O39" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P38" s="9" t="s">
+      <c r="P39" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="Q38" s="9" t="s">
+      <c r="Q39" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="R38" s="9" t="s">
+      <c r="R39" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="24.75">
-      <c r="A39" s="11" t="s">
+    <row r="40" spans="1:18" ht="24.75">
+      <c r="A40" s="11" t="s">
         <v>356</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B40" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" s="8">
+      <c r="C40" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="8">
         <v>0.05</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E40" s="8">
         <v>0.05</v>
       </c>
-      <c r="F39" s="52">
-        <f>Patient!C7*IF(Patient!C2="Male",D39,E39)</f>
+      <c r="F40" s="52">
+        <f>Patient!C7*IF(Patient!C2="Male",D40,E40)</f>
         <v>275.48273332896093</v>
-      </c>
-      <c r="G39" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J39" s="51"/>
-      <c r="K39" s="47" t="s">
-        <v>357</v>
-      </c>
-      <c r="L39" s="49"/>
-      <c r="M39" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="P39" s="32" t="s">
-        <v>359</v>
-      </c>
-      <c r="Q39" s="32" t="s">
-        <v>360</v>
-      </c>
-      <c r="R39" s="32"/>
-    </row>
-    <row r="40" spans="1:18" ht="36.75">
-      <c r="A40" s="11" t="s">
-        <v>361</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="8">
-        <v>1</v>
-      </c>
-      <c r="E40" s="8">
-        <v>1</v>
-      </c>
-      <c r="F40" s="52">
-        <f>Patient!C6*IF(Patient!C2="Male",D40,E40)/60</f>
-        <v>93.333333333333329</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>275</v>
@@ -18339,8 +18339,8 @@
         <v>51</v>
       </c>
       <c r="J40" s="51"/>
-      <c r="K40" s="25" t="s">
-        <v>362</v>
+      <c r="K40" s="47" t="s">
+        <v>357</v>
       </c>
       <c r="L40" s="49"/>
       <c r="M40" s="5" t="s">
@@ -18358,25 +18358,25 @@
       </c>
       <c r="R40" s="32"/>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" ht="36.75">
       <c r="A41" s="11" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D41" s="8">
-        <v>1.2E-2</v>
+        <v>1</v>
       </c>
       <c r="E41" s="8">
-        <v>1.2E-2</v>
+        <v>1</v>
       </c>
       <c r="F41" s="52">
-        <f>Patient!C7*IF(Patient!C2="Male",D41,E41)</f>
-        <v>66.115855998950622</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D41,E41)/60</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>275</v>
@@ -18385,8 +18385,10 @@
       <c r="I41" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J41" s="17"/>
-      <c r="K41" s="25"/>
+      <c r="J41" s="51"/>
+      <c r="K41" s="25" t="s">
+        <v>362</v>
+      </c>
       <c r="L41" s="49"/>
       <c r="M41" s="5" t="s">
         <v>358</v>
@@ -18405,23 +18407,23 @@
     </row>
     <row r="42" spans="1:18">
       <c r="A42" s="11" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D42" s="8">
-        <v>0.12</v>
+        <v>1.2E-2</v>
       </c>
       <c r="E42" s="8">
-        <v>0.12</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F42" s="52">
-        <f>Patient!C6*IF(Patient!C2="Male",D42,E42)/60</f>
-        <v>11.2</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D42,E42)</f>
+        <v>66.115855998950622</v>
       </c>
       <c r="G42" s="17" t="s">
         <v>275</v>
@@ -18450,30 +18452,33 @@
     </row>
     <row r="43" spans="1:18">
       <c r="A43" s="11" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>202</v>
+        <v>314</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="20">
-        <v>40</v>
+      <c r="D43" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="E43" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="F43" s="52">
+        <f>Patient!C6*IF(Patient!C2="Male",D43,E43)/60</f>
+        <v>11.2</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>366</v>
-      </c>
-      <c r="H43" s="17">
-        <v>409</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="H43" s="17"/>
       <c r="I43" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J43" s="17"/>
-      <c r="K43" s="54"/>
+      <c r="K43" s="25"/>
       <c r="L43" s="49"/>
       <c r="M43" s="5" t="s">
         <v>358</v>
@@ -18488,41 +18493,34 @@
       <c r="Q43" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R43" s="32">
-        <v>2</v>
-      </c>
+      <c r="R43" s="32"/>
     </row>
     <row r="44" spans="1:18">
       <c r="A44" s="11" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>17</v>
+        <v>202</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="8">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E44" s="8">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F44" s="50">
-        <f>Patient!C7*IF(Patient!C2="Male",D44,E44)</f>
-        <v>385.67582666054534</v>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="20">
+        <v>40</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="H44" s="17"/>
+        <v>366</v>
+      </c>
+      <c r="H44" s="17">
+        <v>409</v>
+      </c>
       <c r="I44" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J44" s="17"/>
-      <c r="K44" s="47" t="s">
-        <v>368</v>
-      </c>
+      <c r="K44" s="54"/>
       <c r="L44" s="49"/>
       <c r="M44" s="5" t="s">
         <v>358</v>
@@ -18537,27 +18535,29 @@
       <c r="Q44" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R44" s="32"/>
+      <c r="R44" s="32">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="1:18">
       <c r="A45" s="11" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="8">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E45" s="8">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F45" s="50">
-        <f>Patient!C6*IF(Patient!C2="Male",D45,E45)/60</f>
-        <v>4.666666666666667</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D45,E45)</f>
+        <v>385.67582666054534</v>
       </c>
       <c r="G45" s="17" t="s">
         <v>275</v>
@@ -18567,7 +18567,9 @@
         <v>51</v>
       </c>
       <c r="J45" s="17"/>
-      <c r="K45" s="25"/>
+      <c r="K45" s="47" t="s">
+        <v>368</v>
+      </c>
       <c r="L45" s="49"/>
       <c r="M45" s="5" t="s">
         <v>358</v>
@@ -18586,10 +18588,10 @@
     </row>
     <row r="46" spans="1:18">
       <c r="A46" s="11" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>48</v>
@@ -18598,20 +18600,20 @@
         <v>0.05</v>
       </c>
       <c r="E46" s="8">
-        <v>8.5000000000000006E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F46" s="50">
-        <f>Patient!C7*IF(Patient!C2="Male",D46,E46)</f>
-        <v>275.48273332896093</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D46,E46)/60</f>
+        <v>4.666666666666667</v>
       </c>
       <c r="G46" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="H46" s="8"/>
+      <c r="H46" s="17"/>
       <c r="I46" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J46" s="8"/>
+      <c r="J46" s="17"/>
       <c r="K46" s="25"/>
       <c r="L46" s="49"/>
       <c r="M46" s="5" t="s">
@@ -18631,10 +18633,10 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" s="11" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>48</v>
@@ -18646,17 +18648,17 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="F47" s="50">
-        <f>Patient!C6*IF(Patient!C2="Male",D47,E47)/60</f>
-        <v>4.666666666666667</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D47,E47)</f>
+        <v>275.48273332896093</v>
       </c>
       <c r="G47" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="H47" s="17"/>
+      <c r="H47" s="8"/>
       <c r="I47" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J47" s="17"/>
+      <c r="J47" s="8"/>
       <c r="K47" s="25"/>
       <c r="L47" s="49"/>
       <c r="M47" s="5" t="s">
@@ -18676,32 +18678,32 @@
     </row>
     <row r="48" spans="1:18">
       <c r="A48" s="11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D48" s="8">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E48" s="8">
-        <v>0.02</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="F48" s="50">
-        <f>Patient!C7*IF(Patient!C2="Male",D48,E48)</f>
-        <v>110.19309333158436</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D48,E48)/60</f>
+        <v>4.666666666666667</v>
       </c>
       <c r="G48" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="H48" s="55"/>
+      <c r="H48" s="17"/>
       <c r="I48" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J48" s="55"/>
+      <c r="J48" s="17"/>
       <c r="K48" s="25"/>
       <c r="L48" s="49"/>
       <c r="M48" s="5" t="s">
@@ -18721,32 +18723,32 @@
     </row>
     <row r="49" spans="1:18">
       <c r="A49" s="11" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D49" s="8">
-        <v>0.19</v>
+        <v>0.02</v>
       </c>
       <c r="E49" s="8">
-        <v>0.17</v>
+        <v>0.02</v>
       </c>
       <c r="F49" s="50">
-        <f>Patient!C6*IF(Patient!C2="Male",D49,E49)/60</f>
-        <v>17.733333333333334</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D49,E49)</f>
+        <v>110.19309333158436</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="H49" s="17"/>
+      <c r="H49" s="55"/>
       <c r="I49" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J49" s="17"/>
+      <c r="J49" s="55"/>
       <c r="K49" s="25"/>
       <c r="L49" s="49"/>
       <c r="M49" s="5" t="s">
@@ -18764,25 +18766,25 @@
       </c>
       <c r="R49" s="32"/>
     </row>
-    <row r="50" spans="1:18" ht="24.75">
+    <row r="50" spans="1:18">
       <c r="A50" s="11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D50" s="8">
-        <v>2.1999999999999999E-2</v>
+        <v>0.19</v>
       </c>
       <c r="E50" s="8">
-        <v>2.1999999999999999E-2</v>
+        <v>0.17</v>
       </c>
       <c r="F50" s="50">
-        <f>Patient!C7*IF(Patient!C2="Male",D50,E50)</f>
-        <v>121.2124026647428</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D50,E50)/60</f>
+        <v>17.733333333333334</v>
       </c>
       <c r="G50" s="17" t="s">
         <v>275</v>
@@ -18792,9 +18794,7 @@
         <v>51</v>
       </c>
       <c r="J50" s="17"/>
-      <c r="K50" s="47" t="s">
-        <v>375</v>
-      </c>
+      <c r="K50" s="25"/>
       <c r="L50" s="49"/>
       <c r="M50" s="5" t="s">
         <v>358</v>
@@ -18811,25 +18811,25 @@
       </c>
       <c r="R50" s="32"/>
     </row>
-    <row r="51" spans="1:18">
+    <row r="51" spans="1:18" ht="24.75">
       <c r="A51" s="11" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D51" s="8">
-        <v>0.04</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E51" s="8">
-        <v>0.05</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="F51" s="50">
-        <f>Patient!C6*IF(Patient!C2="Male",D51,E51)/60</f>
-        <v>3.7333333333333334</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D51,E51)</f>
+        <v>121.2124026647428</v>
       </c>
       <c r="G51" s="17" t="s">
         <v>275</v>
@@ -18839,7 +18839,9 @@
         <v>51</v>
       </c>
       <c r="J51" s="17"/>
-      <c r="K51" s="25"/>
+      <c r="K51" s="47" t="s">
+        <v>375</v>
+      </c>
       <c r="L51" s="49"/>
       <c r="M51" s="5" t="s">
         <v>358</v>
@@ -18856,25 +18858,25 @@
       </c>
       <c r="R51" s="32"/>
     </row>
-    <row r="52" spans="1:18" ht="36.75">
+    <row r="52" spans="1:18">
       <c r="A52" s="11" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D52" s="8">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E52" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F52" s="52">
-        <f>Patient!C7*IF(Patient!C2="Male",D52,E52)</f>
-        <v>110.19309333158436</v>
+        <v>0.05</v>
+      </c>
+      <c r="F52" s="50">
+        <f>Patient!C6*IF(Patient!C2="Male",D52,E52)/60</f>
+        <v>3.7333333333333334</v>
       </c>
       <c r="G52" s="17" t="s">
         <v>275</v>
@@ -18883,10 +18885,8 @@
       <c r="I52" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J52" s="51"/>
-      <c r="K52" s="47" t="s">
-        <v>378</v>
-      </c>
+      <c r="J52" s="17"/>
+      <c r="K52" s="25"/>
       <c r="L52" s="49"/>
       <c r="M52" s="5" t="s">
         <v>358</v>
@@ -18903,25 +18903,25 @@
       </c>
       <c r="R52" s="32"/>
     </row>
-    <row r="53" spans="1:18">
+    <row r="53" spans="1:18" ht="36.75">
       <c r="A53" s="11" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D53" s="8">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E53" s="8">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F53" s="52">
-        <f>Patient!C6*IF(Patient!C2="Male",D53,E53)/60</f>
-        <v>1.4</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D53,E53)</f>
+        <v>110.19309333158436</v>
       </c>
       <c r="G53" s="17" t="s">
         <v>275</v>
@@ -18932,14 +18932,16 @@
       </c>
       <c r="J53" s="51"/>
       <c r="K53" s="47" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L53" s="49"/>
       <c r="M53" s="5" t="s">
         <v>358</v>
       </c>
       <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
+      <c r="O53" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="P53" s="32" t="s">
         <v>359</v>
       </c>
@@ -18950,45 +18952,48 @@
     </row>
     <row r="54" spans="1:18">
       <c r="A54" s="11" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C54" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="8" t="s">
-        <v>383</v>
+        <v>314</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D54" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E54" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F54" s="52">
+        <f>Patient!C6*IF(Patient!C2="Male",D54,E54)/60</f>
+        <v>1.4</v>
       </c>
       <c r="G54" s="17" t="s">
-        <v>384</v>
+        <v>275</v>
       </c>
       <c r="H54" s="17"/>
       <c r="I54" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J54" s="51"/>
-      <c r="K54" s="25"/>
+      <c r="K54" s="47" t="s">
+        <v>380</v>
+      </c>
       <c r="L54" s="49"/>
       <c r="M54" s="5" t="s">
         <v>358</v>
       </c>
       <c r="N54" s="5"/>
-      <c r="O54" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="O54" s="5"/>
       <c r="P54" s="32" t="s">
         <v>359</v>
       </c>
       <c r="Q54" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R54" s="32">
-        <v>6</v>
-      </c>
+      <c r="R54" s="32"/>
     </row>
     <row r="55" spans="1:18">
       <c r="A55" s="11" t="s">
@@ -18998,12 +19003,12 @@
         <v>17</v>
       </c>
       <c r="C55" s="20" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D55" s="20"/>
       <c r="E55" s="20"/>
       <c r="F55" s="8" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G55" s="17" t="s">
         <v>384</v>
@@ -19034,21 +19039,21 @@
     </row>
     <row r="56" spans="1:18">
       <c r="A56" s="11" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>202</v>
+        <v>17</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="20"/>
       <c r="F56" s="8" t="s">
-        <v>286</v>
+        <v>386</v>
       </c>
       <c r="G56" s="17" t="s">
-        <v>287</v>
+        <v>384</v>
       </c>
       <c r="H56" s="17"/>
       <c r="I56" s="17" t="s">
@@ -19074,7 +19079,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="48.75">
+    <row r="57" spans="1:18">
       <c r="A57" s="11" t="s">
         <v>387</v>
       </c>
@@ -19082,26 +19087,22 @@
         <v>202</v>
       </c>
       <c r="C57" s="20" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="20"/>
       <c r="F57" s="8" t="s">
-        <v>346</v>
+        <v>286</v>
       </c>
       <c r="G57" s="17" t="s">
-        <v>348</v>
-      </c>
-      <c r="H57" s="17" t="s">
-        <v>349</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="H57" s="17"/>
       <c r="I57" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J57" s="51"/>
-      <c r="K57" s="25" t="s">
-        <v>350</v>
-      </c>
+      <c r="K57" s="25"/>
       <c r="L57" s="49"/>
       <c r="M57" s="5" t="s">
         <v>358</v>
@@ -19120,34 +19121,34 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:18">
+    <row r="58" spans="1:18" ht="48.75">
       <c r="A58" s="11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D58" s="8">
-        <v>1</v>
-      </c>
-      <c r="E58" s="8">
-        <v>1</v>
-      </c>
-      <c r="F58" s="8">
-        <v>94.7</v>
+        <v>202</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="8" t="s">
+        <v>346</v>
       </c>
       <c r="G58" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="H58" s="17"/>
+        <v>348</v>
+      </c>
+      <c r="H58" s="17" t="s">
+        <v>349</v>
+      </c>
       <c r="I58" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J58" s="51"/>
-      <c r="K58" s="25"/>
+      <c r="K58" s="25" t="s">
+        <v>350</v>
+      </c>
       <c r="L58" s="49"/>
       <c r="M58" s="5" t="s">
         <v>358</v>
@@ -19162,35 +19163,38 @@
       <c r="Q58" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R58" s="32"/>
-    </row>
-    <row r="59" spans="1:18" ht="24.75">
+      <c r="R58" s="32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
       <c r="A59" s="11" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="7">
-        <f>F48*0.5</f>
-        <v>55.096546665792182</v>
-      </c>
-      <c r="G59" s="26" t="s">
-        <v>390</v>
+      <c r="D59" s="8">
+        <v>1</v>
+      </c>
+      <c r="E59" s="8">
+        <v>1</v>
+      </c>
+      <c r="F59" s="8">
+        <v>94.7</v>
+      </c>
+      <c r="G59" s="17" t="s">
+        <v>275</v>
       </c>
       <c r="H59" s="17"/>
       <c r="I59" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J59" s="51"/>
-      <c r="K59" s="47" t="s">
-        <v>391</v>
-      </c>
+      <c r="K59" s="25"/>
       <c r="L59" s="49"/>
       <c r="M59" s="5" t="s">
         <v>358</v>
@@ -19209,30 +19213,30 @@
     </row>
     <row r="60" spans="1:18" ht="24.75">
       <c r="A60" s="11" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B60" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D60" s="8"/>
       <c r="E60" s="8"/>
-      <c r="F60" s="50">
+      <c r="F60" s="7">
         <f>F49*0.5</f>
-        <v>8.8666666666666671</v>
-      </c>
-      <c r="G60" s="17" t="s">
-        <v>275</v>
+        <v>55.096546665792182</v>
+      </c>
+      <c r="G60" s="26" t="s">
+        <v>390</v>
       </c>
       <c r="H60" s="17"/>
       <c r="I60" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J60" s="51"/>
-      <c r="K60" s="25" t="s">
-        <v>393</v>
+      <c r="K60" s="47" t="s">
+        <v>391</v>
       </c>
       <c r="L60" s="49"/>
       <c r="M60" s="5" t="s">
@@ -19250,25 +19254,21 @@
       </c>
       <c r="R60" s="32"/>
     </row>
-    <row r="61" spans="1:18" ht="36.75">
+    <row r="61" spans="1:18" ht="24.75">
       <c r="A61" s="11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D61" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="E61" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="F61" s="52">
-        <f>Patient!C7*IF(Patient!C2="Male",D61,E61)</f>
-        <v>220.38618666316873</v>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="50">
+        <f>F50*0.5</f>
+        <v>8.8666666666666671</v>
       </c>
       <c r="G61" s="17" t="s">
         <v>275</v>
@@ -19278,8 +19278,8 @@
         <v>51</v>
       </c>
       <c r="J61" s="51"/>
-      <c r="K61" s="47" t="s">
-        <v>378</v>
+      <c r="K61" s="25" t="s">
+        <v>393</v>
       </c>
       <c r="L61" s="49"/>
       <c r="M61" s="5" t="s">
@@ -19297,28 +19297,28 @@
       </c>
       <c r="R61" s="32"/>
     </row>
-    <row r="62" spans="1:18">
+    <row r="62" spans="1:18" ht="36.75">
       <c r="A62" s="11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D62" s="8">
-        <v>5.2499999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E62" s="8">
-        <v>5.2499999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F62" s="52">
-        <f>Patient!C6*IF(Patient!C2="Male",D62,E62)/60</f>
-        <v>4.9000000000000004</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D62,E62)</f>
+        <v>220.38618666316873</v>
       </c>
       <c r="G62" s="17" t="s">
-        <v>396</v>
+        <v>275</v>
       </c>
       <c r="H62" s="17"/>
       <c r="I62" s="17" t="s">
@@ -19326,14 +19326,16 @@
       </c>
       <c r="J62" s="51"/>
       <c r="K62" s="47" t="s">
-        <v>397</v>
+        <v>378</v>
       </c>
       <c r="L62" s="49"/>
       <c r="M62" s="5" t="s">
         <v>358</v>
       </c>
       <c r="N62" s="5"/>
-      <c r="O62" s="5"/>
+      <c r="O62" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="P62" s="32" t="s">
         <v>359</v>
       </c>
@@ -19342,28 +19344,28 @@
       </c>
       <c r="R62" s="32"/>
     </row>
-    <row r="63" spans="1:18" ht="24.75">
+    <row r="63" spans="1:18">
       <c r="A63" s="11" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D63" s="8">
-        <v>0.03</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="E63" s="8">
-        <v>0.03</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="F63" s="52">
-        <f>Patient!C10*Patient!C7*IF(Patient!C2="Male",D63,E63)</f>
-        <v>66.115855998950622</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D63,E63)/60</f>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>275</v>
+        <v>396</v>
       </c>
       <c r="H63" s="17"/>
       <c r="I63" s="17" t="s">
@@ -19371,45 +19373,41 @@
       </c>
       <c r="J63" s="51"/>
       <c r="K63" s="47" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L63" s="49"/>
       <c r="M63" s="5" t="s">
         <v>358</v>
       </c>
       <c r="N63" s="5"/>
-      <c r="O63" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="O63" s="5"/>
       <c r="P63" s="32" t="s">
         <v>359</v>
       </c>
       <c r="Q63" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R63" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18">
+      <c r="R63" s="32"/>
+    </row>
+    <row r="64" spans="1:18" ht="24.75">
       <c r="A64" s="11" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B64" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D64" s="8">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E64" s="8">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="F64" s="52">
-        <f>Patient!C10*Patient!C6*IF(Patient!C3="Male",D64,E64)/60</f>
-        <v>37.333333333333336</v>
+        <f>Patient!C10*Patient!C7*IF(Patient!C2="Male",D64,E64)</f>
+        <v>66.115855998950622</v>
       </c>
       <c r="G64" s="17" t="s">
         <v>275</v>
@@ -19419,7 +19417,9 @@
         <v>51</v>
       </c>
       <c r="J64" s="51"/>
-      <c r="K64" s="25"/>
+      <c r="K64" s="47" t="s">
+        <v>399</v>
+      </c>
       <c r="L64" s="49"/>
       <c r="M64" s="5" t="s">
         <v>358</v>
@@ -19434,27 +19434,29 @@
       <c r="Q64" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R64" s="32"/>
-    </row>
-    <row r="65" spans="1:18" ht="24.75">
+      <c r="R64" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18">
       <c r="A65" s="11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D65" s="8">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="E65" s="8">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="F65" s="52">
-        <f>Patient!C10*Patient!C7*IF(Patient!C4="Male",D65,E65)</f>
-        <v>44.07723733263375</v>
+        <f>Patient!C10*Patient!C6*IF(Patient!C3="Male",D65,E65)/60</f>
+        <v>37.333333333333336</v>
       </c>
       <c r="G65" s="17" t="s">
         <v>275</v>
@@ -19464,9 +19466,7 @@
         <v>51</v>
       </c>
       <c r="J65" s="51"/>
-      <c r="K65" s="47" t="s">
-        <v>399</v>
-      </c>
+      <c r="K65" s="25"/>
       <c r="L65" s="49"/>
       <c r="M65" s="5" t="s">
         <v>358</v>
@@ -19481,29 +19481,27 @@
       <c r="Q65" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R65" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18">
+      <c r="R65" s="32"/>
+    </row>
+    <row r="66" spans="1:18" ht="24.75">
       <c r="A66" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D66" s="8">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="E66" s="8">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="F66" s="52">
-        <f>Patient!C10*Patient!C6*IF(Patient!C5="Male",D66,E66)/60</f>
-        <v>37.333333333333336</v>
+        <f>Patient!C10*Patient!C7*IF(Patient!C4="Male",D66,E66)</f>
+        <v>44.07723733263375</v>
       </c>
       <c r="G66" s="17" t="s">
         <v>275</v>
@@ -19513,7 +19511,9 @@
         <v>51</v>
       </c>
       <c r="J66" s="51"/>
-      <c r="K66" s="25"/>
+      <c r="K66" s="47" t="s">
+        <v>399</v>
+      </c>
       <c r="L66" s="49"/>
       <c r="M66" s="5" t="s">
         <v>358</v>
@@ -19528,27 +19528,29 @@
       <c r="Q66" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R66" s="32"/>
-    </row>
-    <row r="67" spans="1:18" ht="24.75">
+      <c r="R66" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18">
       <c r="A67" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D67" s="8">
-        <v>5.5E-2</v>
+        <v>1</v>
       </c>
       <c r="E67" s="8">
-        <v>5.5E-2</v>
+        <v>1</v>
       </c>
       <c r="F67" s="52">
-        <f>Patient!C10*Patient!C7*IF(Patient!C6="Male",D67,E67)</f>
-        <v>121.21240266474281</v>
+        <f>Patient!C10*Patient!C6*IF(Patient!C5="Male",D67,E67)/60</f>
+        <v>37.333333333333336</v>
       </c>
       <c r="G67" s="17" t="s">
         <v>275</v>
@@ -19558,9 +19560,7 @@
         <v>51</v>
       </c>
       <c r="J67" s="51"/>
-      <c r="K67" s="47" t="s">
-        <v>399</v>
-      </c>
+      <c r="K67" s="25"/>
       <c r="L67" s="49"/>
       <c r="M67" s="5" t="s">
         <v>358</v>
@@ -19575,29 +19575,27 @@
       <c r="Q67" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R67" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18">
+      <c r="R67" s="32"/>
+    </row>
+    <row r="68" spans="1:18" ht="24.75">
       <c r="A68" s="11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D68" s="8">
-        <v>1</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E68" s="8">
-        <v>1</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F68" s="52">
-        <f>Patient!C10*Patient!C6*IF(Patient!C7="Male",D68,E68)/60</f>
-        <v>37.333333333333336</v>
+        <f>Patient!C10*Patient!C7*IF(Patient!C6="Male",D68,E68)</f>
+        <v>121.21240266474281</v>
       </c>
       <c r="G68" s="17" t="s">
         <v>275</v>
@@ -19607,7 +19605,9 @@
         <v>51</v>
       </c>
       <c r="J68" s="51"/>
-      <c r="K68" s="25"/>
+      <c r="K68" s="47" t="s">
+        <v>399</v>
+      </c>
       <c r="L68" s="49"/>
       <c r="M68" s="5" t="s">
         <v>358</v>
@@ -19622,27 +19622,29 @@
       <c r="Q68" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R68" s="32"/>
-    </row>
-    <row r="69" spans="1:18" ht="24.75">
+      <c r="R68" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18">
       <c r="A69" s="11" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D69" s="8">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="E69" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="F69" s="50">
-        <f>Patient!C7*IF(Patient!C2="Male",D69,E69)</f>
-        <v>550.96546665792187</v>
+        <v>1</v>
+      </c>
+      <c r="F69" s="52">
+        <f>Patient!C10*Patient!C6*IF(Patient!C7="Male",D69,E69)/60</f>
+        <v>37.333333333333336</v>
       </c>
       <c r="G69" s="17" t="s">
         <v>275</v>
@@ -19651,10 +19653,8 @@
       <c r="I69" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J69" s="17"/>
-      <c r="K69" s="47" t="s">
-        <v>406</v>
-      </c>
+      <c r="J69" s="51"/>
+      <c r="K69" s="25"/>
       <c r="L69" s="49"/>
       <c r="M69" s="5" t="s">
         <v>358</v>
@@ -19671,38 +19671,36 @@
       </c>
       <c r="R69" s="32"/>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" ht="24.75">
       <c r="A70" s="11" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D70" s="8">
-        <v>0.255</v>
+        <v>0.1</v>
       </c>
       <c r="E70" s="8">
-        <v>0.27</v>
+        <v>0.1</v>
       </c>
       <c r="F70" s="50">
-        <f>Patient!C6*IF(Patient!C2="Male",D70,E70)/60</f>
-        <v>23.8</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D70,E70)</f>
+        <v>550.96546665792187</v>
       </c>
       <c r="G70" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H70" s="17" t="s">
-        <v>408</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="H70" s="17"/>
       <c r="I70" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J70" s="17"/>
-      <c r="K70" s="25" t="s">
-        <v>409</v>
+      <c r="K70" s="47" t="s">
+        <v>406</v>
       </c>
       <c r="L70" s="49"/>
       <c r="M70" s="5" t="s">
@@ -19722,34 +19720,36 @@
     </row>
     <row r="71" spans="1:18">
       <c r="A71" s="11" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D71" s="8">
-        <v>0.14000000000000001</v>
+        <v>0.255</v>
       </c>
       <c r="E71" s="8">
-        <v>0.105</v>
-      </c>
-      <c r="F71" s="52">
-        <f>Patient!C7*IF(Patient!C2="Male",D71,E71)</f>
-        <v>771.35165332109068</v>
+        <v>0.27</v>
+      </c>
+      <c r="F71" s="50">
+        <f>Patient!C6*IF(Patient!C2="Male",D71,E71)/60</f>
+        <v>23.8</v>
       </c>
       <c r="G71" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="H71" s="17"/>
+        <v>15</v>
+      </c>
+      <c r="H71" s="17" t="s">
+        <v>408</v>
+      </c>
       <c r="I71" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J71" s="17"/>
-      <c r="K71" s="47" t="s">
-        <v>411</v>
+      <c r="K71" s="25" t="s">
+        <v>409</v>
       </c>
       <c r="L71" s="49"/>
       <c r="M71" s="5" t="s">
@@ -19769,23 +19769,23 @@
     </row>
     <row r="72" spans="1:18">
       <c r="A72" s="11" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D72" s="8">
-        <v>0.17</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E72" s="8">
-        <v>0.12</v>
+        <v>0.105</v>
       </c>
       <c r="F72" s="52">
-        <f>Patient!C6*IF(Patient!C2="Male",D72,E72)/60</f>
-        <v>15.866666666666669</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D72,E72)</f>
+        <v>771.35165332109068</v>
       </c>
       <c r="G72" s="17" t="s">
         <v>275</v>
@@ -19795,7 +19795,9 @@
         <v>51</v>
       </c>
       <c r="J72" s="17"/>
-      <c r="K72" s="25"/>
+      <c r="K72" s="47" t="s">
+        <v>411</v>
+      </c>
       <c r="L72" s="49"/>
       <c r="M72" s="5" t="s">
         <v>358</v>
@@ -19814,23 +19816,23 @@
     </row>
     <row r="73" spans="1:18">
       <c r="A73" s="11" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D73" s="8">
-        <v>0.01</v>
+        <v>0.17</v>
       </c>
       <c r="E73" s="8">
-        <v>0.01</v>
+        <v>0.12</v>
       </c>
       <c r="F73" s="52">
-        <f>Patient!C7*IF(Patient!C2="Male",D73,E73)</f>
-        <v>55.096546665792182</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D73,E73)/60</f>
+        <v>15.866666666666669</v>
       </c>
       <c r="G73" s="17" t="s">
         <v>275</v>
@@ -19839,10 +19841,8 @@
       <c r="I73" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J73" s="51"/>
-      <c r="K73" s="47" t="s">
-        <v>414</v>
-      </c>
+      <c r="J73" s="17"/>
+      <c r="K73" s="25"/>
       <c r="L73" s="49"/>
       <c r="M73" s="5" t="s">
         <v>358</v>
@@ -19861,23 +19861,23 @@
     </row>
     <row r="74" spans="1:18">
       <c r="A74" s="11" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D74" s="8">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="E74" s="8">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F74" s="52">
-        <f>Patient!C6*IF(Patient!C2="Male",D74,E74)/60</f>
-        <v>3.7333333333333334</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D74,E74)</f>
+        <v>55.096546665792182</v>
       </c>
       <c r="G74" s="17" t="s">
         <v>275</v>
@@ -19887,7 +19887,9 @@
         <v>51</v>
       </c>
       <c r="J74" s="51"/>
-      <c r="K74" s="25"/>
+      <c r="K74" s="47" t="s">
+        <v>414</v>
+      </c>
       <c r="L74" s="49"/>
       <c r="M74" s="5" t="s">
         <v>358</v>
@@ -19904,25 +19906,25 @@
       </c>
       <c r="R74" s="32"/>
     </row>
-    <row r="75" spans="1:18" ht="24.75">
+    <row r="75" spans="1:18">
       <c r="A75" s="11" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D75" s="8">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E75" s="8">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="F75" s="52">
-        <f>Patient!C7*IF(Patient!C19="Male",D75,E75)</f>
-        <v>165.28963999737655</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D75,E75)/60</f>
+        <v>3.7333333333333334</v>
       </c>
       <c r="G75" s="17" t="s">
         <v>275</v>
@@ -19932,9 +19934,7 @@
         <v>51</v>
       </c>
       <c r="J75" s="51"/>
-      <c r="K75" s="47" t="s">
-        <v>399</v>
-      </c>
+      <c r="K75" s="25"/>
       <c r="L75" s="49"/>
       <c r="M75" s="5" t="s">
         <v>358</v>
@@ -19951,25 +19951,25 @@
       </c>
       <c r="R75" s="32"/>
     </row>
-    <row r="76" spans="1:18">
+    <row r="76" spans="1:18" ht="24.75">
       <c r="A76" s="11" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D76" s="8">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E76" s="8">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="F76" s="52">
-        <f>Patient!C6*IF(Patient!C2="Male",D76,E76)/60</f>
-        <v>93.333333333333329</v>
+        <f>Patient!C7*IF(Patient!C19="Male",D76,E76)</f>
+        <v>165.28963999737655</v>
       </c>
       <c r="G76" s="17" t="s">
         <v>275</v>
@@ -19979,7 +19979,9 @@
         <v>51</v>
       </c>
       <c r="J76" s="51"/>
-      <c r="K76" s="25"/>
+      <c r="K76" s="47" t="s">
+        <v>399</v>
+      </c>
       <c r="L76" s="49"/>
       <c r="M76" s="5" t="s">
         <v>358</v>
@@ -19998,25 +20000,28 @@
     </row>
     <row r="77" spans="1:18">
       <c r="A77" s="11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C77" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="8" t="s">
-        <v>286</v>
+        <v>314</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D77" s="8">
+        <v>1</v>
+      </c>
+      <c r="E77" s="8">
+        <v>1</v>
+      </c>
+      <c r="F77" s="52">
+        <f>Patient!C6*IF(Patient!C2="Male",D77,E77)/60</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="G77" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H77" s="17" t="s">
-        <v>272</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="H77" s="17"/>
       <c r="I77" s="17" t="s">
         <v>51</v>
       </c>
@@ -20046,12 +20051,12 @@
         <v>202</v>
       </c>
       <c r="C78" s="20" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
       <c r="F78" s="8" t="s">
-        <v>329</v>
+        <v>286</v>
       </c>
       <c r="G78" s="17" t="s">
         <v>93</v>
@@ -20080,37 +20085,32 @@
       </c>
       <c r="R78" s="32"/>
     </row>
-    <row r="79" spans="1:18" ht="24.75">
+    <row r="79" spans="1:18">
       <c r="A79" s="11" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C79" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D79" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="E79" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F79" s="52">
-        <f>Patient!C7*IF(Patient!C2="Male",D79,E79)</f>
-        <v>110.19309333158436</v>
+        <v>202</v>
+      </c>
+      <c r="C79" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="8" t="s">
+        <v>329</v>
       </c>
       <c r="G79" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="H79" s="17"/>
+        <v>93</v>
+      </c>
+      <c r="H79" s="17" t="s">
+        <v>272</v>
+      </c>
       <c r="I79" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J79" s="51"/>
-      <c r="K79" s="47" t="s">
-        <v>399</v>
-      </c>
+      <c r="K79" s="25"/>
       <c r="L79" s="49"/>
       <c r="M79" s="5" t="s">
         <v>358</v>
@@ -20127,25 +20127,25 @@
       </c>
       <c r="R79" s="32"/>
     </row>
-    <row r="80" spans="1:18">
+    <row r="80" spans="1:18" ht="24.75">
       <c r="A80" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D80" s="8">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="E80" s="8">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="F80" s="52">
-        <f>Patient!C6*IF(Patient!C20="Male",D80,E80)/60</f>
-        <v>93.333333333333329</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D80,E80)</f>
+        <v>110.19309333158436</v>
       </c>
       <c r="G80" s="17" t="s">
         <v>275</v>
@@ -20155,7 +20155,9 @@
         <v>51</v>
       </c>
       <c r="J80" s="51"/>
-      <c r="K80" s="25"/>
+      <c r="K80" s="47" t="s">
+        <v>399</v>
+      </c>
       <c r="L80" s="49"/>
       <c r="M80" s="5" t="s">
         <v>358</v>
@@ -20174,32 +20176,33 @@
     </row>
     <row r="81" spans="1:18">
       <c r="A81" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C81" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="8" t="s">
-        <v>286</v>
+        <v>314</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D81" s="8">
+        <v>1</v>
+      </c>
+      <c r="E81" s="8">
+        <v>1</v>
+      </c>
+      <c r="F81" s="52">
+        <f>Patient!C6*IF(Patient!C20="Male",D81,E81)/60</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="G81" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H81" s="17" t="s">
-        <v>272</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="H81" s="17"/>
       <c r="I81" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J81" s="51"/>
-      <c r="K81" s="25" t="s">
-        <v>422</v>
-      </c>
+      <c r="K81" s="25"/>
       <c r="L81" s="49"/>
       <c r="M81" s="5" t="s">
         <v>358</v>
@@ -20214,40 +20217,35 @@
       <c r="Q81" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R81" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:18" ht="24.75">
+      <c r="R81" s="32"/>
+    </row>
+    <row r="82" spans="1:18">
       <c r="A82" s="11" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D82" s="8">
-        <v>5.5E-2</v>
-      </c>
-      <c r="E82" s="8">
-        <v>5.5E-2</v>
-      </c>
-      <c r="F82" s="52">
-        <f>Patient!C7*IF(Patient!C22="Male",D82,E82)</f>
-        <v>303.03100666185702</v>
+        <v>202</v>
+      </c>
+      <c r="C82" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D82" s="5"/>
+      <c r="E82" s="5"/>
+      <c r="F82" s="8" t="s">
+        <v>286</v>
       </c>
       <c r="G82" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="H82" s="17"/>
+        <v>93</v>
+      </c>
+      <c r="H82" s="17" t="s">
+        <v>272</v>
+      </c>
       <c r="I82" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J82" s="51"/>
-      <c r="K82" s="47" t="s">
-        <v>399</v>
+      <c r="K82" s="25" t="s">
+        <v>422</v>
       </c>
       <c r="L82" s="49"/>
       <c r="M82" s="5" t="s">
@@ -20263,27 +20261,29 @@
       <c r="Q82" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R82" s="32"/>
-    </row>
-    <row r="83" spans="1:18">
+      <c r="R82" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" ht="24.75">
       <c r="A83" s="11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B83" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D83" s="8">
-        <v>1</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E83" s="8">
-        <v>1</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F83" s="52">
-        <f>Patient!C6*IF(Patient!C23="Male",D83,E83)/60</f>
-        <v>93.333333333333329</v>
+        <f>Patient!C7*IF(Patient!C22="Male",D83,E83)</f>
+        <v>303.03100666185702</v>
       </c>
       <c r="G83" s="17" t="s">
         <v>275</v>
@@ -20293,7 +20293,9 @@
         <v>51</v>
       </c>
       <c r="J83" s="51"/>
-      <c r="K83" s="25"/>
+      <c r="K83" s="47" t="s">
+        <v>399</v>
+      </c>
       <c r="L83" s="49"/>
       <c r="M83" s="5" t="s">
         <v>358</v>
@@ -20310,34 +20312,35 @@
       </c>
       <c r="R83" s="32"/>
     </row>
-    <row r="84" spans="1:18" ht="36.75">
+    <row r="84" spans="1:18">
       <c r="A84" s="11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C84" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D84" s="20"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="8" t="s">
-        <v>286</v>
+        <v>314</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D84" s="8">
+        <v>1</v>
+      </c>
+      <c r="E84" s="8">
+        <v>1</v>
+      </c>
+      <c r="F84" s="52">
+        <f>Patient!C6*IF(Patient!C23="Male",D84,E84)/60</f>
+        <v>93.333333333333329</v>
       </c>
       <c r="G84" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H84" s="17" t="s">
-        <v>272</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="H84" s="17"/>
       <c r="I84" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J84" s="51"/>
-      <c r="K84" s="25" t="s">
-        <v>426</v>
-      </c>
+      <c r="K84" s="25"/>
       <c r="L84" s="49"/>
       <c r="M84" s="5" t="s">
         <v>358</v>
@@ -20352,40 +20355,35 @@
       <c r="Q84" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R84" s="32">
-        <v>1</v>
-      </c>
+      <c r="R84" s="32"/>
     </row>
     <row r="85" spans="1:18" ht="36.75">
       <c r="A85" s="11" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D85" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="E85" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F85" s="52">
-        <f>Patient!C7*IF(Patient!C2="Male",D85,E85)</f>
-        <v>110.19309333158436</v>
+        <v>202</v>
+      </c>
+      <c r="C85" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D85" s="20"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="8" t="s">
+        <v>286</v>
       </c>
       <c r="G85" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="H85" s="17"/>
+        <v>93</v>
+      </c>
+      <c r="H85" s="17" t="s">
+        <v>272</v>
+      </c>
       <c r="I85" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J85" s="51"/>
-      <c r="K85" s="47" t="s">
-        <v>378</v>
+      <c r="K85" s="25" t="s">
+        <v>426</v>
       </c>
       <c r="L85" s="49"/>
       <c r="M85" s="5" t="s">
@@ -20401,30 +20399,32 @@
       <c r="Q85" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R85" s="32"/>
-    </row>
-    <row r="86" spans="1:18">
+      <c r="R85" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" ht="36.75">
       <c r="A86" s="11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C86" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D86" s="8">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E86" s="8">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F86" s="52">
-        <f>Patient!C6*IF(Patient!C2="Male",D86,E86)/60</f>
-        <v>1.4</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D86,E86)</f>
+        <v>110.19309333158436</v>
       </c>
       <c r="G86" s="17" t="s">
-        <v>429</v>
+        <v>275</v>
       </c>
       <c r="H86" s="17"/>
       <c r="I86" s="17" t="s">
@@ -20432,14 +20432,16 @@
       </c>
       <c r="J86" s="51"/>
       <c r="K86" s="47" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="L86" s="49"/>
       <c r="M86" s="5" t="s">
         <v>358</v>
       </c>
       <c r="N86" s="5"/>
-      <c r="O86" s="5"/>
+      <c r="O86" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="P86" s="32" t="s">
         <v>359</v>
       </c>
@@ -20448,23 +20450,28 @@
       </c>
       <c r="R86" s="32"/>
     </row>
-    <row r="87" spans="1:18" ht="60.75">
+    <row r="87" spans="1:18">
       <c r="A87" s="11" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B87" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C87" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="D87" s="20"/>
-      <c r="E87" s="20"/>
-      <c r="F87" s="8" t="s">
-        <v>431</v>
+        <v>314</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D87" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E87" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F87" s="52">
+        <f>Patient!C6*IF(Patient!C2="Male",D87,E87)/60</f>
+        <v>1.4</v>
       </c>
       <c r="G87" s="17" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H87" s="17"/>
       <c r="I87" s="17" t="s">
@@ -20472,16 +20479,14 @@
       </c>
       <c r="J87" s="51"/>
       <c r="K87" s="47" t="s">
-        <v>433</v>
+        <v>380</v>
       </c>
       <c r="L87" s="49"/>
       <c r="M87" s="5" t="s">
         <v>358</v>
       </c>
       <c r="N87" s="5"/>
-      <c r="O87" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="O87" s="5"/>
       <c r="P87" s="32" t="s">
         <v>359</v>
       </c>
@@ -20490,7 +20495,7 @@
       </c>
       <c r="R87" s="32"/>
     </row>
-    <row r="88" spans="1:18" ht="24">
+    <row r="88" spans="1:18" ht="60.75">
       <c r="A88" s="11" t="s">
         <v>430</v>
       </c>
@@ -20498,12 +20503,12 @@
         <v>17</v>
       </c>
       <c r="C88" s="20" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D88" s="20"/>
       <c r="E88" s="20"/>
       <c r="F88" s="8" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G88" s="17" t="s">
         <v>432</v>
@@ -20513,7 +20518,9 @@
         <v>51</v>
       </c>
       <c r="J88" s="51"/>
-      <c r="K88" s="25"/>
+      <c r="K88" s="47" t="s">
+        <v>433</v>
+      </c>
       <c r="L88" s="49"/>
       <c r="M88" s="5" t="s">
         <v>358</v>
@@ -20530,32 +20537,30 @@
       </c>
       <c r="R88" s="32"/>
     </row>
-    <row r="89" spans="1:18" ht="36.75">
+    <row r="89" spans="1:18" ht="24">
       <c r="A89" s="11" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B89" s="17" t="s">
-        <v>202</v>
+        <v>17</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D89" s="20"/>
       <c r="E89" s="20"/>
       <c r="F89" s="8" t="s">
-        <v>289</v>
+        <v>434</v>
       </c>
       <c r="G89" s="17" t="s">
-        <v>287</v>
+        <v>432</v>
       </c>
       <c r="H89" s="17"/>
       <c r="I89" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J89" s="51"/>
-      <c r="K89" s="25" t="s">
-        <v>290</v>
-      </c>
+      <c r="K89" s="25"/>
       <c r="L89" s="49"/>
       <c r="M89" s="5" t="s">
         <v>358</v>
@@ -20572,7 +20577,7 @@
       </c>
       <c r="R89" s="32"/>
     </row>
-    <row r="90" spans="1:18">
+    <row r="90" spans="1:18" ht="36.75">
       <c r="A90" s="11" t="s">
         <v>435</v>
       </c>
@@ -20580,12 +20585,12 @@
         <v>202</v>
       </c>
       <c r="C90" s="20" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D90" s="20"/>
       <c r="E90" s="20"/>
       <c r="F90" s="8" t="s">
-        <v>329</v>
+        <v>289</v>
       </c>
       <c r="G90" s="17" t="s">
         <v>287</v>
@@ -20595,7 +20600,9 @@
         <v>51</v>
       </c>
       <c r="J90" s="51"/>
-      <c r="K90" s="25"/>
+      <c r="K90" s="25" t="s">
+        <v>290</v>
+      </c>
       <c r="L90" s="49"/>
       <c r="M90" s="5" t="s">
         <v>358</v>
@@ -20614,21 +20621,21 @@
     </row>
     <row r="91" spans="1:18">
       <c r="A91" s="11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B91" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8">
-        <v>94.7</v>
+        <v>202</v>
+      </c>
+      <c r="C91" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="D91" s="20"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="8" t="s">
+        <v>329</v>
       </c>
       <c r="G91" s="17" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="H91" s="17"/>
       <c r="I91" s="17" t="s">
@@ -20652,33 +20659,30 @@
       </c>
       <c r="R91" s="32"/>
     </row>
-    <row r="92" spans="1:18" ht="24.75">
+    <row r="92" spans="1:18">
       <c r="A92" s="11" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B92" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D92" s="8"/>
       <c r="E92" s="8"/>
-      <c r="F92" s="7">
-        <f>F48*0.5</f>
-        <v>55.096546665792182</v>
-      </c>
-      <c r="G92" s="26" t="s">
-        <v>390</v>
+      <c r="F92" s="8">
+        <v>94.7</v>
+      </c>
+      <c r="G92" s="17" t="s">
+        <v>275</v>
       </c>
       <c r="H92" s="17"/>
       <c r="I92" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J92" s="51"/>
-      <c r="K92" s="47" t="s">
-        <v>391</v>
-      </c>
+      <c r="K92" s="25"/>
       <c r="L92" s="49"/>
       <c r="M92" s="5" t="s">
         <v>358</v>
@@ -20697,30 +20701,30 @@
     </row>
     <row r="93" spans="1:18" ht="24.75">
       <c r="A93" s="11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B93" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D93" s="8"/>
       <c r="E93" s="8"/>
-      <c r="F93" s="50">
+      <c r="F93" s="7">
         <f>F49*0.5</f>
-        <v>8.8666666666666671</v>
-      </c>
-      <c r="G93" s="17" t="s">
-        <v>275</v>
+        <v>55.096546665792182</v>
+      </c>
+      <c r="G93" s="26" t="s">
+        <v>390</v>
       </c>
       <c r="H93" s="17"/>
       <c r="I93" s="17" t="s">
         <v>51</v>
       </c>
       <c r="J93" s="51"/>
-      <c r="K93" s="25" t="s">
-        <v>393</v>
+      <c r="K93" s="47" t="s">
+        <v>391</v>
       </c>
       <c r="L93" s="49"/>
       <c r="M93" s="5" t="s">
@@ -20738,25 +20742,21 @@
       </c>
       <c r="R93" s="32"/>
     </row>
-    <row r="94" spans="1:18" ht="36.75">
+    <row r="94" spans="1:18" ht="24.75">
       <c r="A94" s="11" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D94" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="E94" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="F94" s="52">
-        <f>Patient!C7*IF(Patient!C2="Male",D94,E94)</f>
-        <v>220.38618666316873</v>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="50">
+        <f>F50*0.5</f>
+        <v>8.8666666666666671</v>
       </c>
       <c r="G94" s="17" t="s">
         <v>275</v>
@@ -20766,8 +20766,8 @@
         <v>51</v>
       </c>
       <c r="J94" s="51"/>
-      <c r="K94" s="47" t="s">
-        <v>378</v>
+      <c r="K94" s="25" t="s">
+        <v>393</v>
       </c>
       <c r="L94" s="49"/>
       <c r="M94" s="5" t="s">
@@ -20785,28 +20785,28 @@
       </c>
       <c r="R94" s="32"/>
     </row>
-    <row r="95" spans="1:18">
+    <row r="95" spans="1:18" ht="36.75">
       <c r="A95" s="11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B95" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D95" s="8">
-        <v>5.2499999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E95" s="8">
-        <v>5.2499999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F95" s="52">
-        <f>Patient!C6*IF(Patient!C2="Male",D95,E95)/60</f>
-        <v>4.9000000000000004</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D95,E95)</f>
+        <v>220.38618666316873</v>
       </c>
       <c r="G95" s="17" t="s">
-        <v>396</v>
+        <v>275</v>
       </c>
       <c r="H95" s="17"/>
       <c r="I95" s="17" t="s">
@@ -20814,14 +20814,16 @@
       </c>
       <c r="J95" s="51"/>
       <c r="K95" s="47" t="s">
-        <v>397</v>
+        <v>378</v>
       </c>
       <c r="L95" s="49"/>
       <c r="M95" s="5" t="s">
         <v>358</v>
       </c>
       <c r="N95" s="5"/>
-      <c r="O95" s="5"/>
+      <c r="O95" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="P95" s="32" t="s">
         <v>359</v>
       </c>
@@ -20830,28 +20832,28 @@
       </c>
       <c r="R95" s="32"/>
     </row>
-    <row r="96" spans="1:18" ht="24.75">
+    <row r="96" spans="1:18">
       <c r="A96" s="11" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B96" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D96" s="8">
-        <v>0.03</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="E96" s="8">
-        <v>0.03</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="F96" s="52">
-        <f>Patient!C9*Patient!C7*IF(Patient!C2="Male",D96,E96)</f>
-        <v>99.173783998425932</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D96,E96)/60</f>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G96" s="17" t="s">
-        <v>275</v>
+        <v>396</v>
       </c>
       <c r="H96" s="17"/>
       <c r="I96" s="17" t="s">
@@ -20859,45 +20861,41 @@
       </c>
       <c r="J96" s="51"/>
       <c r="K96" s="47" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L96" s="49"/>
       <c r="M96" s="5" t="s">
         <v>358</v>
       </c>
       <c r="N96" s="5"/>
-      <c r="O96" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="O96" s="5"/>
       <c r="P96" s="32" t="s">
         <v>359</v>
       </c>
       <c r="Q96" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R96" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:18">
+      <c r="R96" s="32"/>
+    </row>
+    <row r="97" spans="1:18" ht="24.75">
       <c r="A97" s="11" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D97" s="8">
-        <v>1</v>
+        <v>0.03</v>
       </c>
       <c r="E97" s="8">
-        <v>1</v>
-      </c>
-      <c r="F97" s="8">
-        <f>Patient!C9*Patient!C6*IF(Patient!C2="Male",D97,E97)/60</f>
-        <v>56</v>
+        <v>0.03</v>
+      </c>
+      <c r="F97" s="52">
+        <f>Patient!C9*Patient!C7*IF(Patient!C2="Male",D97,E97)</f>
+        <v>99.173783998425932</v>
       </c>
       <c r="G97" s="17" t="s">
         <v>275</v>
@@ -20907,7 +20905,9 @@
         <v>51</v>
       </c>
       <c r="J97" s="51"/>
-      <c r="K97" s="25"/>
+      <c r="K97" s="47" t="s">
+        <v>399</v>
+      </c>
       <c r="L97" s="49"/>
       <c r="M97" s="5" t="s">
         <v>358</v>
@@ -20922,27 +20922,29 @@
       <c r="Q97" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R97" s="32"/>
-    </row>
-    <row r="98" spans="1:18" ht="24.75">
+      <c r="R97" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:18">
       <c r="A98" s="11" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B98" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D98" s="8">
-        <v>0.02</v>
+        <v>1</v>
       </c>
       <c r="E98" s="8">
-        <v>0.02</v>
-      </c>
-      <c r="F98" s="52">
-        <f>Patient!C9*Patient!C7*IF(Patient!C2="Male",D98,E98)</f>
-        <v>66.115855998950622</v>
+        <v>1</v>
+      </c>
+      <c r="F98" s="8">
+        <f>Patient!C9*Patient!C6*IF(Patient!C2="Male",D98,E98)/60</f>
+        <v>56</v>
       </c>
       <c r="G98" s="17" t="s">
         <v>275</v>
@@ -20952,9 +20954,7 @@
         <v>51</v>
       </c>
       <c r="J98" s="51"/>
-      <c r="K98" s="47" t="s">
-        <v>399</v>
-      </c>
+      <c r="K98" s="25"/>
       <c r="L98" s="49"/>
       <c r="M98" s="5" t="s">
         <v>358</v>
@@ -20969,29 +20969,27 @@
       <c r="Q98" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R98" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:18">
+      <c r="R98" s="32"/>
+    </row>
+    <row r="99" spans="1:18" ht="24.75">
       <c r="A99" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B99" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D99" s="8">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="E99" s="8">
-        <v>1</v>
-      </c>
-      <c r="F99" s="8">
-        <f>Patient!C9*Patient!C6*IF(Patient!C2="Male",D99,E99)/60</f>
-        <v>56</v>
+        <v>0.02</v>
+      </c>
+      <c r="F99" s="52">
+        <f>Patient!C9*Patient!C7*IF(Patient!C2="Male",D99,E99)</f>
+        <v>66.115855998950622</v>
       </c>
       <c r="G99" s="17" t="s">
         <v>275</v>
@@ -21001,7 +20999,9 @@
         <v>51</v>
       </c>
       <c r="J99" s="51"/>
-      <c r="K99" s="25"/>
+      <c r="K99" s="47" t="s">
+        <v>399</v>
+      </c>
       <c r="L99" s="49"/>
       <c r="M99" s="5" t="s">
         <v>358</v>
@@ -21016,27 +21016,29 @@
       <c r="Q99" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R99" s="32"/>
-    </row>
-    <row r="100" spans="1:18" ht="24.75">
+      <c r="R99" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18">
       <c r="A100" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B100" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D100" s="8">
-        <v>5.5E-2</v>
+        <v>1</v>
       </c>
       <c r="E100" s="8">
-        <v>5.5E-2</v>
-      </c>
-      <c r="F100" s="52">
-        <f>Patient!C9*Patient!C7*IF(Patient!C2="Male",D100,E100)</f>
-        <v>181.8186039971142</v>
+        <v>1</v>
+      </c>
+      <c r="F100" s="8">
+        <f>Patient!C9*Patient!C6*IF(Patient!C2="Male",D100,E100)/60</f>
+        <v>56</v>
       </c>
       <c r="G100" s="17" t="s">
         <v>275</v>
@@ -21045,10 +21047,8 @@
       <c r="I100" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J100" s="17"/>
-      <c r="K100" s="47" t="s">
-        <v>399</v>
-      </c>
+      <c r="J100" s="51"/>
+      <c r="K100" s="25"/>
       <c r="L100" s="49"/>
       <c r="M100" s="5" t="s">
         <v>358</v>
@@ -21063,29 +21063,27 @@
       <c r="Q100" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R100" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:18">
+      <c r="R100" s="32"/>
+    </row>
+    <row r="101" spans="1:18" ht="24.75">
       <c r="A101" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B101" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D101" s="8">
-        <v>1</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E101" s="8">
-        <v>1</v>
-      </c>
-      <c r="F101" s="8">
-        <f>Patient!C9*Patient!C6*IF(Patient!C2="Male",D101,E101)/60</f>
-        <v>56</v>
+        <v>5.5E-2</v>
+      </c>
+      <c r="F101" s="52">
+        <f>Patient!C9*Patient!C7*IF(Patient!C2="Male",D101,E101)</f>
+        <v>181.8186039971142</v>
       </c>
       <c r="G101" s="17" t="s">
         <v>275</v>
@@ -21095,7 +21093,9 @@
         <v>51</v>
       </c>
       <c r="J101" s="17"/>
-      <c r="K101" s="25"/>
+      <c r="K101" s="47" t="s">
+        <v>399</v>
+      </c>
       <c r="L101" s="49"/>
       <c r="M101" s="5" t="s">
         <v>358</v>
@@ -21110,27 +21110,29 @@
       <c r="Q101" s="32" t="s">
         <v>360</v>
       </c>
-      <c r="R101" s="32"/>
-    </row>
-    <row r="102" spans="1:18" ht="24.75">
+      <c r="R101" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18">
       <c r="A102" s="11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B102" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D102" s="8">
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="E102" s="8">
-        <v>0.03</v>
-      </c>
-      <c r="F102" s="52">
-        <f>Patient!C7*IF(Patient!C2="Male",D102,E102)</f>
-        <v>165.28963999737655</v>
+        <v>1</v>
+      </c>
+      <c r="F102" s="8">
+        <f>Patient!C9*Patient!C6*IF(Patient!C2="Male",D102,E102)/60</f>
+        <v>56</v>
       </c>
       <c r="G102" s="17" t="s">
         <v>275</v>
@@ -21140,9 +21142,7 @@
         <v>51</v>
       </c>
       <c r="J102" s="17"/>
-      <c r="K102" s="47" t="s">
-        <v>406</v>
-      </c>
+      <c r="K102" s="25"/>
       <c r="L102" s="49"/>
       <c r="M102" s="5" t="s">
         <v>358</v>
@@ -21159,25 +21159,25 @@
       </c>
       <c r="R102" s="32"/>
     </row>
-    <row r="103" spans="1:18">
+    <row r="103" spans="1:18" ht="24.75">
       <c r="A103" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B103" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D103" s="8">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="E103" s="8">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F103" s="52">
-        <f>Patient!C6*IF(Patient!C2="Male",D103,E103)/60</f>
-        <v>4.666666666666667</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D103,E103)</f>
+        <v>165.28963999737655</v>
       </c>
       <c r="G103" s="17" t="s">
         <v>275</v>
@@ -21187,7 +21187,9 @@
         <v>51</v>
       </c>
       <c r="J103" s="17"/>
-      <c r="K103" s="25"/>
+      <c r="K103" s="47" t="s">
+        <v>406</v>
+      </c>
       <c r="L103" s="49"/>
       <c r="M103" s="5" t="s">
         <v>358</v>
@@ -21206,23 +21208,23 @@
     </row>
     <row r="104" spans="1:18">
       <c r="A104" s="11" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B104" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D104" s="8">
-        <v>3.7999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="E104" s="8">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="F104" s="50">
-        <f>Patient!C7*IF(Patient!C2="Male",D104,E104)</f>
-        <v>209.36687733001028</v>
+        <v>0.05</v>
+      </c>
+      <c r="F104" s="52">
+        <f>Patient!C6*IF(Patient!C2="Male",D104,E104)/60</f>
+        <v>4.666666666666667</v>
       </c>
       <c r="G104" s="17" t="s">
         <v>275</v>
@@ -21251,23 +21253,23 @@
     </row>
     <row r="105" spans="1:18">
       <c r="A105" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B105" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D105" s="8">
-        <v>0.1</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E105" s="8">
-        <v>0.11</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="F105" s="50">
-        <f>Patient!C6*IF(Patient!C2="Male",D105,E105)/60</f>
-        <v>9.3333333333333339</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D105,E105)</f>
+        <v>209.36687733001028</v>
       </c>
       <c r="G105" s="17" t="s">
         <v>275</v>
@@ -21296,23 +21298,23 @@
     </row>
     <row r="106" spans="1:18">
       <c r="A106" s="11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B106" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D106" s="8">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="E106" s="8">
-        <v>0.01</v>
+        <v>0.11</v>
       </c>
       <c r="F106" s="50">
-        <f>Patient!C7*IF(Patient!C2="Male",D106,E106)</f>
-        <v>55.096546665792182</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D106,E106)/60</f>
+        <v>9.3333333333333339</v>
       </c>
       <c r="G106" s="17" t="s">
         <v>275</v>
@@ -21341,10 +21343,10 @@
     </row>
     <row r="107" spans="1:18">
       <c r="A107" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B107" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>48</v>
@@ -21356,20 +21358,18 @@
         <v>0.01</v>
       </c>
       <c r="F107" s="50">
-        <f>Patient!C6*IF(Patient!C2="Male",D107,E107)/60</f>
-        <v>0.93333333333333335</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D107,E107)</f>
+        <v>55.096546665792182</v>
       </c>
       <c r="G107" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="H107" s="8"/>
+      <c r="H107" s="17"/>
       <c r="I107" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J107" s="8"/>
-      <c r="K107" s="47" t="s">
-        <v>453</v>
-      </c>
+      <c r="J107" s="17"/>
+      <c r="K107" s="25"/>
       <c r="L107" s="49"/>
       <c r="M107" s="5" t="s">
         <v>358</v>
@@ -21388,33 +21388,35 @@
     </row>
     <row r="108" spans="1:18">
       <c r="A108" s="11" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B108" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D108" s="8">
-        <v>1.4E-2</v>
+        <v>0.01</v>
       </c>
       <c r="E108" s="8">
-        <v>1.4E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F108" s="50">
-        <f>Patient!C7*IF(Patient!C2="Male",D108,E108)</f>
-        <v>77.135165332109054</v>
+        <f>Patient!C6*IF(Patient!C2="Male",D108,E108)/60</f>
+        <v>0.93333333333333335</v>
       </c>
       <c r="G108" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="H108" s="17"/>
+      <c r="H108" s="8"/>
       <c r="I108" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J108" s="51"/>
-      <c r="K108" s="25"/>
+      <c r="J108" s="8"/>
+      <c r="K108" s="47" t="s">
+        <v>453</v>
+      </c>
       <c r="L108" s="49"/>
       <c r="M108" s="5" t="s">
         <v>358</v>
@@ -21433,23 +21435,23 @@
     </row>
     <row r="109" spans="1:18">
       <c r="A109" s="11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B109" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D109" s="8">
-        <v>0.03</v>
+        <v>1.4E-2</v>
       </c>
       <c r="E109" s="8">
-        <v>0.03</v>
+        <v>1.4E-2</v>
       </c>
       <c r="F109" s="50">
-        <f>Patient!C6*IF(Patient!C2="Male",D109,E109)/60</f>
-        <v>2.8</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D109,E109)</f>
+        <v>77.135165332109054</v>
       </c>
       <c r="G109" s="17" t="s">
         <v>275</v>
@@ -21476,38 +21478,36 @@
       </c>
       <c r="R109" s="32"/>
     </row>
-    <row r="110" spans="1:18" ht="24.75">
+    <row r="110" spans="1:18">
       <c r="A110" s="11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B110" s="17" t="s">
-        <v>17</v>
+        <v>314</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D110" s="8">
-        <v>0.17499999999999999</v>
+        <v>0.03</v>
       </c>
       <c r="E110" s="8">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="F110" s="52">
-        <f>Patient!C7*IF(Patient!C2="Male",D110,E110)</f>
-        <v>964.18956665136318</v>
+        <v>0.03</v>
+      </c>
+      <c r="F110" s="50">
+        <f>Patient!C6*IF(Patient!C2="Male",D110,E110)/60</f>
+        <v>2.8</v>
       </c>
       <c r="G110" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="H110" s="26"/>
+      <c r="H110" s="17"/>
       <c r="I110" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J110" s="5"/>
-      <c r="K110" s="47" t="s">
-        <v>406</v>
-      </c>
-      <c r="L110" s="56"/>
+      <c r="J110" s="51"/>
+      <c r="K110" s="25"/>
+      <c r="L110" s="49"/>
       <c r="M110" s="5" t="s">
         <v>358</v>
       </c>
@@ -21523,25 +21523,25 @@
       </c>
       <c r="R110" s="32"/>
     </row>
-    <row r="111" spans="1:18">
+    <row r="111" spans="1:18" ht="24.75">
       <c r="A111" s="11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B111" s="17" t="s">
-        <v>314</v>
+        <v>17</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D111" s="8">
-        <v>1</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="E111" s="8">
-        <v>1</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="F111" s="52">
-        <f>Patient!C6*IF(Patient!C2="Male",D111,E111)/60</f>
-        <v>93.333333333333329</v>
+        <f>Patient!C7*IF(Patient!C2="Male",D111,E111)</f>
+        <v>964.18956665136318</v>
       </c>
       <c r="G111" s="17" t="s">
         <v>275</v>
@@ -21551,7 +21551,9 @@
         <v>51</v>
       </c>
       <c r="J111" s="5"/>
-      <c r="K111" s="33"/>
+      <c r="K111" s="47" t="s">
+        <v>406</v>
+      </c>
       <c r="L111" s="56"/>
       <c r="M111" s="5" t="s">
         <v>358</v>
@@ -21567,6 +21569,51 @@
         <v>360</v>
       </c>
       <c r="R111" s="32"/>
+    </row>
+    <row r="112" spans="1:18">
+      <c r="A112" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="B112" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="C112" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D112" s="8">
+        <v>1</v>
+      </c>
+      <c r="E112" s="8">
+        <v>1</v>
+      </c>
+      <c r="F112" s="52">
+        <f>Patient!C6*IF(Patient!C2="Male",D112,E112)/60</f>
+        <v>93.333333333333329</v>
+      </c>
+      <c r="G112" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="H112" s="26"/>
+      <c r="I112" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J112" s="5"/>
+      <c r="K112" s="33"/>
+      <c r="L112" s="56"/>
+      <c r="M112" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="N112" s="5"/>
+      <c r="O112" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="P112" s="32" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q112" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="R112" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -28407,7 +28454,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="52">
-        <f>Cardiovascular!F49*60</f>
+        <f>Cardiovascular!F50*60</f>
         <v>1064</v>
       </c>
       <c r="G4" s="18" t="s">

</xml_diff>

<commit_message>
Add total fluid volume to Tissue validation spreadsheet.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\dehydration\source\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435855C0-84E9-4079-A5F4-BAFC757C25BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC967D77-C265-4B64-B878-DCF809F2D993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23610" yWindow="825" windowWidth="28800" windowHeight="17235" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28770" yWindow="6540" windowWidth="27825" windowHeight="23535" tabRatio="500" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6590" uniqueCount="1193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6598" uniqueCount="1194">
   <si>
     <t>Patient Inputs</t>
   </si>
@@ -3755,6 +3755,9 @@
   </si>
   <si>
     <t>marriott1993water</t>
+  </si>
+  <si>
+    <t>TotalFluidVolume</t>
   </si>
 </sst>
 </file>
@@ -4026,7 +4029,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4361,6 +4364,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9178,12 +9184,12 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:P92"/>
+  <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A67" sqref="A67"/>
-      <selection pane="topRight" activeCell="D21" sqref="D21"/>
+      <selection pane="topRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9303,7 +9309,7 @@
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
       <c r="F3" s="52">
-        <f>SUM(F14,F17,F20,F23,F26,F29,F32,F35,F38,F41,F46,F49,F52)</f>
+        <f>SUM(F15,F18,F21,F24,F27,F30,F33,F36,F39,F42,F47,F50,F53)</f>
         <v>8751.6116205773851</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -9346,7 +9352,7 @@
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
       <c r="F4" s="8">
-        <f>SUM(F13:F42,F46:F53)</f>
+        <f>SUM(F14:F43,F47:F54)</f>
         <v>34084.065120622952</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -9429,7 +9435,7 @@
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="52">
-        <f>SUM(F15+F18+F21+F24+F27+F30+F33+F36+F39+F42+F47+F50+F53)</f>
+        <f>SUM(F16+F19+F22+F25+F28+F31+F34+F37+F40+F43+F48+F51+F54)</f>
         <v>25271.303751033935</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -9535,101 +9541,97 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:16">
+      <c r="A9" s="120" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>937</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="110">
+        <v>42</v>
+      </c>
+      <c r="G9" s="111" t="s">
+        <v>1044</v>
+      </c>
+      <c r="H9" s="111"/>
+      <c r="I9" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="112"/>
+      <c r="K9" s="110"/>
+      <c r="L9" s="110">
+        <v>37</v>
+      </c>
+      <c r="M9" s="66" t="s">
+        <v>1045</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="P9" s="69"/>
+    </row>
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A10" s="28" t="s">
         <v>1064</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K9" s="3" t="s">
+      <c r="K10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L10" s="3" t="s">
         <v>1042</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N9" s="9" t="s">
+      <c r="N10" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="O9" s="9" t="s">
+      <c r="O10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P9" s="9" t="s">
+      <c r="P10" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="67" t="s">
+    <row r="11" spans="1:16">
+      <c r="A11" s="67" t="s">
         <v>1065</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14">
-        <v>-250</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>1066</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14">
-        <v>250</v>
-      </c>
-      <c r="M10" s="66" t="s">
-        <v>1045</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="O10" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="P10" s="66">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="1" customFormat="1">
-      <c r="A11" s="67" t="s">
-        <v>1067</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>14</v>
@@ -9639,8 +9641,8 @@
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
-      <c r="F11" s="17">
-        <v>300</v>
+      <c r="F11" s="14">
+        <v>-250</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>104</v>
@@ -9651,10 +9653,10 @@
       <c r="I11" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17">
-        <v>300</v>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14">
+        <v>250</v>
       </c>
       <c r="M11" s="66" t="s">
         <v>1045</v>
@@ -9662,128 +9664,127 @@
       <c r="N11" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="O11" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="66">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A12" s="28" t="s">
+    <row r="12" spans="1:16" s="1" customFormat="1">
+      <c r="A12" s="67" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="17">
+        <v>300</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17">
+        <v>300</v>
+      </c>
+      <c r="M12" s="66" t="s">
+        <v>1045</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="P12" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A13" s="28" t="s">
         <v>1068</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="L13" s="3" t="s">
         <v>1042</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="M13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N12" s="9" t="s">
+      <c r="N13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="O12" s="9" t="s">
+      <c r="O13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P12" s="9" t="s">
+      <c r="P13" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" ht="12">
-      <c r="A13" s="30" t="s">
+    <row r="14" spans="1:16" s="1" customFormat="1" ht="12">
+      <c r="A14" s="30" t="s">
         <v>1069</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>937</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="14">
+      <c r="C14" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="14">
         <v>14.5</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E14" s="14">
         <v>19</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F14" s="7">
         <f>Patient!C12*Patient!C4/1.03</f>
         <v>15.69902912621359</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G14" s="17" t="s">
         <v>273</v>
-      </c>
-      <c r="H13" s="26" t="s">
-        <v>1070</v>
-      </c>
-      <c r="I13" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="J13" s="17"/>
-      <c r="K13" s="33" t="s">
-        <v>1071</v>
-      </c>
-      <c r="L13" s="5">
-        <v>3140</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>1072</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="O13" s="14" t="s">
-        <v>1073</v>
-      </c>
-      <c r="P13" s="14"/>
-    </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" ht="12">
-      <c r="A14" s="30" t="s">
-        <v>1074</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="7">
-        <f>F13*0.135*1000</f>
-        <v>2119.3689320388348</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>1047</v>
       </c>
       <c r="H14" s="26" t="s">
         <v>1070</v>
@@ -9802,16 +9803,16 @@
         <v>1072</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P14" s="14"/>
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A15" s="30" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>17</v>
@@ -9822,8 +9823,8 @@
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="7">
-        <f>F13*0.017*1000</f>
-        <v>266.88349514563106</v>
+        <f>F14*0.135*1000</f>
+        <v>2119.3689320388348</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>1047</v>
@@ -9854,26 +9855,22 @@
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A16" s="30" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>937</v>
+        <v>17</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="14">
-        <v>10.5</v>
-      </c>
-      <c r="E16" s="14">
-        <v>7.8</v>
-      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="7">
-        <f>(IF(Patient!C2="Male",D16,E16)/1.3)*(Patient!C13/Patient!C17)</f>
-        <v>8.0769230769230766</v>
+        <f>F14*0.017*1000</f>
+        <v>266.88349514563106</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>273</v>
+        <v>1047</v>
       </c>
       <c r="H16" s="26" t="s">
         <v>1070</v>
@@ -9883,40 +9880,44 @@
       </c>
       <c r="J16" s="17"/>
       <c r="K16" s="33" t="s">
-        <v>1077</v>
+        <v>1071</v>
       </c>
       <c r="L16" s="5">
-        <v>2680</v>
+        <v>3140</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>1072</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O16" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P16" s="14"/>
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A17" s="30" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+      <c r="D17" s="14">
+        <v>10.5</v>
+      </c>
+      <c r="E17" s="14">
+        <v>7.8</v>
+      </c>
       <c r="F17" s="7">
-        <f>F16*0.1*1000</f>
-        <v>807.69230769230774</v>
+        <f>(IF(Patient!C2="Male",D17,E17)/1.3)*(Patient!C13/Patient!C17)</f>
+        <v>8.0769230769230766</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H17" s="26" t="s">
         <v>1070</v>
@@ -9935,16 +9936,16 @@
         <v>1072</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P17" s="14"/>
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A18" s="30" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>17</v>
@@ -9955,8 +9956,8 @@
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="7">
-        <f>F16*0.346*1000</f>
-        <v>2794.6153846153843</v>
+        <f>F17*0.1*1000</f>
+        <v>807.69230769230774</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>1047</v>
@@ -9987,26 +9988,22 @@
     </row>
     <row r="19" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A19" s="30" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>937</v>
+        <v>17</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="14">
-        <v>1.45</v>
-      </c>
-      <c r="E19" s="14">
-        <v>1.3</v>
-      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="7">
-        <f>(IF(Patient!C2="Male",D19,E19)/1)*(Patient!C13/Patient!C17)</f>
-        <v>1.45</v>
+        <f>F17*0.346*1000</f>
+        <v>2794.6153846153843</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>273</v>
+        <v>1047</v>
       </c>
       <c r="H19" s="26" t="s">
         <v>1070</v>
@@ -10016,40 +10013,44 @@
       </c>
       <c r="J19" s="17"/>
       <c r="K19" s="33" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="L19" s="5">
-        <v>1020</v>
+        <v>2680</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>1072</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P19" s="14"/>
     </row>
     <row r="20" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A20" s="30" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+      <c r="D20" s="14">
+        <v>1.45</v>
+      </c>
+      <c r="E20" s="14">
+        <v>1.3</v>
+      </c>
       <c r="F20" s="7">
-        <f>F19*0.162*1000</f>
-        <v>234.9</v>
+        <f>(IF(Patient!C2="Male",D20,E20)/1)*(Patient!C13/Patient!C17)</f>
+        <v>1.45</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H20" s="26" t="s">
         <v>1070</v>
@@ -10068,16 +10069,16 @@
         <v>1072</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P20" s="14"/>
     </row>
     <row r="21" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A21" s="30" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>17</v>
@@ -10088,8 +10089,8 @@
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="7">
-        <f>F19*0.62*1000</f>
-        <v>899</v>
+        <f>F20*0.162*1000</f>
+        <v>234.9</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>1047</v>
@@ -10120,26 +10121,22 @@
     </row>
     <row r="22" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A22" s="30" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>937</v>
+        <v>17</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="14">
-        <v>1.02</v>
-      </c>
-      <c r="E22" s="14">
-        <v>0.96</v>
-      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="7">
-        <f>(IF(Patient!C2="Male",D22,E22)/1)*(Patient!C13/Patient!C17)</f>
-        <v>1.02</v>
+        <f>F20*0.62*1000</f>
+        <v>899</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>273</v>
+        <v>1047</v>
       </c>
       <c r="H22" s="26" t="s">
         <v>1070</v>
@@ -10152,37 +10149,41 @@
         <v>1081</v>
       </c>
       <c r="L22" s="5">
-        <v>730</v>
+        <v>1020</v>
       </c>
       <c r="M22" s="5" t="s">
         <v>1072</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O22" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P22" s="14"/>
     </row>
     <row r="23" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A23" s="30" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+      <c r="D23" s="14">
+        <v>1.02</v>
+      </c>
+      <c r="E23" s="14">
+        <v>0.96</v>
+      </c>
       <c r="F23" s="7">
-        <f>F22*0.282*1000</f>
-        <v>287.63999999999993</v>
+        <f>(IF(Patient!C2="Male",D23,E23)/1)*(Patient!C13/Patient!C17)</f>
+        <v>1.02</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H23" s="26" t="s">
         <v>1070</v>
@@ -10201,16 +10202,16 @@
         <v>1072</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P23" s="14"/>
     </row>
     <row r="24" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A24" s="30" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>17</v>
@@ -10221,8 +10222,8 @@
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="7">
-        <f>F22*0.475*1000</f>
-        <v>484.5</v>
+        <f>F23*0.282*1000</f>
+        <v>287.63999999999993</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>1047</v>
@@ -10253,26 +10254,22 @@
     </row>
     <row r="25" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A25" s="30" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>937</v>
+        <v>17</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="14">
-        <v>0.155</v>
-      </c>
-      <c r="E25" s="14">
-        <v>0.13750000000000001</v>
-      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="7">
-        <f>(IF(Patient!C2="Male",D25,E25)/1)*(Patient!C13/Patient!C17)</f>
-        <v>0.155</v>
+        <f>F23*0.475*1000</f>
+        <v>484.5</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>273</v>
+        <v>1047</v>
       </c>
       <c r="H25" s="26" t="s">
         <v>1070</v>
@@ -10285,37 +10282,41 @@
         <v>1081</v>
       </c>
       <c r="L25" s="5">
-        <v>110</v>
+        <v>730</v>
       </c>
       <c r="M25" s="5" t="s">
         <v>1072</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O25" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P25" s="14"/>
     </row>
     <row r="26" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A26" s="30" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
+      <c r="D26" s="14">
+        <v>0.155</v>
+      </c>
+      <c r="E26" s="14">
+        <v>0.13750000000000001</v>
+      </c>
       <c r="F26" s="7">
-        <f>F25*0.273*1000</f>
-        <v>42.315000000000005</v>
+        <f>(IF(Patient!C2="Male",D26,E26)/1)*(Patient!C13/Patient!C17)</f>
+        <v>0.155</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H26" s="26" t="s">
         <v>1070</v>
@@ -10334,16 +10335,16 @@
         <v>1072</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P26" s="14"/>
     </row>
     <row r="27" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A27" s="30" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>17</v>
@@ -10354,8 +10355,8 @@
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="7">
-        <f>F25*0.483*1000</f>
-        <v>74.864999999999995</v>
+        <f>F26*0.273*1000</f>
+        <v>42.315000000000005</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>1047</v>
@@ -10386,26 +10387,22 @@
     </row>
     <row r="28" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A28" s="30" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>937</v>
+        <v>17</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="14">
-        <v>0.155</v>
-      </c>
-      <c r="E28" s="14">
-        <v>0.13750000000000001</v>
-      </c>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
       <c r="F28" s="7">
-        <f>(IF(Patient!C2="Male",D28,E28)/1)*(Patient!C13/Patient!C17)</f>
-        <v>0.155</v>
+        <f>F26*0.483*1000</f>
+        <v>74.864999999999995</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>273</v>
+        <v>1047</v>
       </c>
       <c r="H28" s="26" t="s">
         <v>1070</v>
@@ -10424,31 +10421,35 @@
         <v>1072</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O28" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P28" s="14"/>
     </row>
     <row r="29" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A29" s="30" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
+      <c r="D29" s="14">
+        <v>0.155</v>
+      </c>
+      <c r="E29" s="14">
+        <v>0.13750000000000001</v>
+      </c>
       <c r="F29" s="7">
-        <f>F25*0.273*1000</f>
-        <v>42.315000000000005</v>
+        <f>(IF(Patient!C2="Male",D29,E29)/1)*(Patient!C13/Patient!C17)</f>
+        <v>0.155</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H29" s="26" t="s">
         <v>1070</v>
@@ -10467,16 +10468,16 @@
         <v>1072</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O29" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P29" s="14"/>
     </row>
     <row r="30" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A30" s="30" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>17</v>
@@ -10487,8 +10488,8 @@
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="7">
-        <f>F25*0.483*1000</f>
-        <v>74.864999999999995</v>
+        <f>F26*0.273*1000</f>
+        <v>42.315000000000005</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>1047</v>
@@ -10519,26 +10520,22 @@
     </row>
     <row r="31" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A31" s="30" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>937</v>
+        <v>17</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="14">
-        <v>1.8</v>
-      </c>
-      <c r="E31" s="14">
-        <v>1.4</v>
-      </c>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="7">
-        <f>(IF(Patient!C2="Male",D31,E31)/1)*(Patient!C13/Patient!C17)</f>
-        <v>1.8</v>
+        <f>F26*0.483*1000</f>
+        <v>74.864999999999995</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>273</v>
+        <v>1047</v>
       </c>
       <c r="H31" s="26" t="s">
         <v>1070</v>
@@ -10551,37 +10548,41 @@
         <v>1081</v>
       </c>
       <c r="L31" s="5">
-        <v>1030</v>
+        <v>110</v>
       </c>
       <c r="M31" s="5" t="s">
         <v>1072</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O31" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P31" s="14"/>
     </row>
     <row r="32" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A32" s="30" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
+      <c r="D32" s="14">
+        <v>1.8</v>
+      </c>
+      <c r="E32" s="14">
+        <v>1.4</v>
+      </c>
       <c r="F32" s="7">
-        <f>F31*0.161*1000</f>
-        <v>289.8</v>
+        <f>(IF(Patient!C2="Male",D32,E32)/1)*(Patient!C13/Patient!C17)</f>
+        <v>1.8</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H32" s="26" t="s">
         <v>1070</v>
@@ -10600,16 +10601,16 @@
         <v>1072</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O32" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P32" s="14"/>
     </row>
     <row r="33" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A33" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>17</v>
@@ -10620,8 +10621,8 @@
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="7">
-        <f>F31*0.573*1000</f>
-        <v>1031.3999999999999</v>
+        <f>F32*0.161*1000</f>
+        <v>289.8</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>1047</v>
@@ -10652,28 +10653,22 @@
     </row>
     <row r="34" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A34" s="30" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>937</v>
+        <v>17</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="14">
-        <f>0.5*Patient!C9</f>
-        <v>0.3</v>
-      </c>
-      <c r="E34" s="14">
-        <f>0.5*Patient!C9</f>
-        <v>0.3</v>
-      </c>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
       <c r="F34" s="7">
-        <f>(IF(Patient!C2="Male",D34,E34)/1)*(Patient!C13/Patient!C17)</f>
-        <v>0.3</v>
+        <f>F32*0.573*1000</f>
+        <v>1031.3999999999999</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>273</v>
+        <v>1047</v>
       </c>
       <c r="H34" s="26" t="s">
         <v>1070</v>
@@ -10686,37 +10681,43 @@
         <v>1081</v>
       </c>
       <c r="L34" s="5">
-        <v>160</v>
+        <v>1030</v>
       </c>
       <c r="M34" s="5" t="s">
         <v>1072</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O34" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P34" s="14"/>
     </row>
     <row r="35" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A35" s="30" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
+      <c r="D35" s="14">
+        <f>0.5*Patient!C9</f>
+        <v>0.3</v>
+      </c>
+      <c r="E35" s="14">
+        <f>0.5*Patient!C9</f>
+        <v>0.3</v>
+      </c>
       <c r="F35" s="7">
-        <f>F34*0.336*1000</f>
-        <v>100.8</v>
+        <f>(IF(Patient!C2="Male",D35,E35)/1)*(Patient!C13/Patient!C17)</f>
+        <v>0.3</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H35" s="26" t="s">
         <v>1070</v>
@@ -10735,16 +10736,16 @@
         <v>1072</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O35" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P35" s="14"/>
     </row>
     <row r="36" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A36" s="30" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>17</v>
@@ -10755,8 +10756,8 @@
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="7">
-        <f>F34*0.446*1000</f>
-        <v>133.80000000000001</v>
+        <f>F35*0.336*1000</f>
+        <v>100.8</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>1047</v>
@@ -10787,28 +10788,22 @@
     </row>
     <row r="37" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A37" s="30" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>937</v>
+        <v>17</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="14">
-        <f>0.5*Patient!C10</f>
-        <v>0.2</v>
-      </c>
-      <c r="E37" s="14">
-        <f>0.42*Patient!C10</f>
-        <v>0.16800000000000001</v>
-      </c>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
       <c r="F37" s="7">
-        <f>(IF(Patient!C2="Male",D37,E37)/1)*(Patient!C13/Patient!C17)</f>
-        <v>0.2</v>
+        <f>F35*0.446*1000</f>
+        <v>133.80000000000001</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>273</v>
+        <v>1047</v>
       </c>
       <c r="H37" s="26" t="s">
         <v>1070</v>
@@ -10827,31 +10822,37 @@
         <v>1072</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O37" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P37" s="14"/>
     </row>
     <row r="38" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A38" s="30" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
+      <c r="D38" s="14">
+        <f>0.5*Patient!C10</f>
+        <v>0.2</v>
+      </c>
+      <c r="E38" s="14">
+        <f>0.42*Patient!C10</f>
+        <v>0.16800000000000001</v>
+      </c>
       <c r="F38" s="7">
-        <f>F37*0.336*1000</f>
-        <v>67.2</v>
+        <f>(IF(Patient!C2="Male",D38,E38)/1)*(Patient!C13/Patient!C17)</f>
+        <v>0.2</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H38" s="26" t="s">
         <v>1070</v>
@@ -10870,16 +10871,16 @@
         <v>1072</v>
       </c>
       <c r="N38" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O38" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P38" s="14"/>
     </row>
     <row r="39" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A39" s="30" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>17</v>
@@ -10890,8 +10891,8 @@
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="7">
-        <f>F37*0.446*1000</f>
-        <v>89.2</v>
+        <f>F38*0.336*1000</f>
+        <v>67.2</v>
       </c>
       <c r="G39" s="17" t="s">
         <v>1047</v>
@@ -10922,26 +10923,22 @@
     </row>
     <row r="40" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A40" s="30" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>937</v>
+        <v>17</v>
       </c>
       <c r="C40" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="14">
-        <v>29</v>
-      </c>
-      <c r="E40" s="14">
-        <v>17.5</v>
-      </c>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
       <c r="F40" s="7">
-        <f>(IF(Patient!C2="Male",D40,E40)/1)*(Patient!C13/Patient!C17)</f>
-        <v>29</v>
+        <f>F38*0.446*1000</f>
+        <v>89.2</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>273</v>
+        <v>1047</v>
       </c>
       <c r="H40" s="26" t="s">
         <v>1070</v>
@@ -10954,37 +10951,41 @@
         <v>1081</v>
       </c>
       <c r="L40" s="5">
-        <v>13090</v>
+        <v>160</v>
       </c>
       <c r="M40" s="5" t="s">
         <v>1072</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O40" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P40" s="14"/>
     </row>
     <row r="41" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A41" s="30" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
+      <c r="D41" s="14">
+        <v>29</v>
+      </c>
+      <c r="E41" s="14">
+        <v>17.5</v>
+      </c>
       <c r="F41" s="7">
-        <f>F40*0.118*1000</f>
-        <v>3421.9999999999995</v>
+        <f>(IF(Patient!C2="Male",D41,E41)/1)*(Patient!C13/Patient!C17)</f>
+        <v>29</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H41" s="26" t="s">
         <v>1070</v>
@@ -11003,16 +11004,16 @@
         <v>1072</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O41" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P41" s="14"/>
     </row>
     <row r="42" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A42" s="30" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>17</v>
@@ -11023,8 +11024,8 @@
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="7">
-        <f>F40*0.63*1000</f>
-        <v>18270</v>
+        <f>F41*0.118*1000</f>
+        <v>3421.9999999999995</v>
       </c>
       <c r="G42" s="17" t="s">
         <v>1047</v>
@@ -11053,31 +11054,38 @@
       </c>
       <c r="P42" s="14"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A43" s="30" t="s">
-        <v>1105</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" s="8" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>46</v>
       </c>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
-      <c r="F43" s="52" t="s">
-        <v>1106</v>
+      <c r="F43" s="7">
+        <f>F41*0.63*1000</f>
+        <v>18270</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>1107</v>
-      </c>
-      <c r="H43" s="17"/>
+        <v>1047</v>
+      </c>
+      <c r="H43" s="26" t="s">
+        <v>1070</v>
+      </c>
       <c r="I43" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J43" s="17"/>
-      <c r="K43" s="33"/>
-      <c r="L43" s="21"/>
+      <c r="K43" s="33" t="s">
+        <v>1081</v>
+      </c>
+      <c r="L43" s="5">
+        <v>13090</v>
+      </c>
       <c r="M43" s="5" t="s">
         <v>1072</v>
       </c>
@@ -11091,7 +11099,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="30" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>89</v>
@@ -11101,21 +11109,19 @@
       </c>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
-      <c r="F44" s="113" t="s">
-        <v>1109</v>
+      <c r="F44" s="52" t="s">
+        <v>1106</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>548</v>
-      </c>
-      <c r="H44" s="26"/>
+        <v>1107</v>
+      </c>
+      <c r="H44" s="17"/>
       <c r="I44" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="J44" s="5"/>
-      <c r="K44" s="33" t="s">
-        <v>1110</v>
-      </c>
-      <c r="L44" s="4"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="21"/>
       <c r="M44" s="5" t="s">
         <v>1072</v>
       </c>
@@ -11127,71 +11133,66 @@
       </c>
       <c r="P44" s="14"/>
     </row>
-    <row r="45" spans="1:16" s="1" customFormat="1" ht="12">
+    <row r="45" spans="1:16">
       <c r="A45" s="30" t="s">
-        <v>1111</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>937</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D45" s="14">
-        <v>0.33</v>
-      </c>
-      <c r="E45" s="14">
-        <v>0.25</v>
-      </c>
-      <c r="F45" s="7">
-        <f>(IF(Patient!C2="Male",D45,E45)/1)*(Patient!C13/Patient!C17)</f>
-        <v>0.33</v>
+        <v>1108</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="113" t="s">
+        <v>1109</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>273</v>
-      </c>
-      <c r="H45" s="26" t="s">
-        <v>1070</v>
-      </c>
+        <v>548</v>
+      </c>
+      <c r="H45" s="26"/>
       <c r="I45" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="J45" s="17"/>
+      <c r="J45" s="5"/>
       <c r="K45" s="33" t="s">
-        <v>1081</v>
-      </c>
-      <c r="L45" s="5">
-        <v>190</v>
-      </c>
+        <v>1110</v>
+      </c>
+      <c r="L45" s="4"/>
       <c r="M45" s="5" t="s">
         <v>1072</v>
       </c>
       <c r="N45" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O45" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P45" s="14"/>
     </row>
     <row r="46" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A46" s="30" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
+      <c r="D46" s="14">
+        <v>0.33</v>
+      </c>
+      <c r="E46" s="14">
+        <v>0.25</v>
+      </c>
       <c r="F46" s="7">
-        <f>F45*0.32*1000</f>
-        <v>105.60000000000001</v>
+        <f>(IF(Patient!C2="Male",D46,E46)/1)*(Patient!C13/Patient!C17)</f>
+        <v>0.33</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H46" s="26" t="s">
         <v>1070</v>
@@ -11210,16 +11211,16 @@
         <v>1072</v>
       </c>
       <c r="N46" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O46" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P46" s="14"/>
     </row>
     <row r="47" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A47" s="30" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>17</v>
@@ -11230,8 +11231,8 @@
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="7">
-        <f>F45*0.456*1000</f>
-        <v>150.47999999999999</v>
+        <f>F46*0.32*1000</f>
+        <v>105.60000000000001</v>
       </c>
       <c r="G47" s="17" t="s">
         <v>1047</v>
@@ -11262,26 +11263,22 @@
     </row>
     <row r="48" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A48" s="30" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>937</v>
+        <v>17</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="14">
-        <v>3.3</v>
-      </c>
-      <c r="E48" s="14">
-        <v>2.2999999999999998</v>
-      </c>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
       <c r="F48" s="7">
-        <f>(IF(Patient!C2="Male",D48,E48)/1)*(Patient!C5/Patient!C15)</f>
-        <v>3.1437968084980175</v>
+        <f>F46*0.456*1000</f>
+        <v>150.47999999999999</v>
       </c>
       <c r="G48" s="17" t="s">
-        <v>273</v>
+        <v>1047</v>
       </c>
       <c r="H48" s="26" t="s">
         <v>1070</v>
@@ -11294,37 +11291,41 @@
         <v>1081</v>
       </c>
       <c r="L48" s="5">
-        <v>1550</v>
+        <v>190</v>
       </c>
       <c r="M48" s="5" t="s">
         <v>1072</v>
       </c>
       <c r="N48" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O48" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P48" s="14"/>
     </row>
     <row r="49" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A49" s="30" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
+      <c r="D49" s="14">
+        <v>3.3</v>
+      </c>
+      <c r="E49" s="14">
+        <v>2.2999999999999998</v>
+      </c>
       <c r="F49" s="7">
-        <f>F48*0.382*1000</f>
-        <v>1200.9303808462425</v>
+        <f>(IF(Patient!C2="Male",D49,E49)/1)*(Patient!C5/Patient!C15)</f>
+        <v>3.1437968084980175</v>
       </c>
       <c r="G49" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H49" s="26" t="s">
         <v>1070</v>
@@ -11343,16 +11344,16 @@
         <v>1072</v>
       </c>
       <c r="N49" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O49" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P49" s="14"/>
     </row>
     <row r="50" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A50" s="30" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>17</v>
@@ -11363,8 +11364,8 @@
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="7">
-        <f>F48*0.291*1000</f>
-        <v>914.844871272923</v>
+        <f>F49*0.382*1000</f>
+        <v>1200.9303808462425</v>
       </c>
       <c r="G50" s="17" t="s">
         <v>1047</v>
@@ -11395,26 +11396,22 @@
     </row>
     <row r="51" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A51" s="30" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>937</v>
+        <v>17</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D51" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="E51" s="14">
-        <v>0.13</v>
-      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
       <c r="F51" s="7">
-        <f>(IF(Patient!C2="Male",D51,E51)/1)*(Patient!C13/Patient!C17)</f>
-        <v>0.15</v>
+        <f>F49*0.291*1000</f>
+        <v>914.844871272923</v>
       </c>
       <c r="G51" s="17" t="s">
-        <v>273</v>
+        <v>1047</v>
       </c>
       <c r="H51" s="26" t="s">
         <v>1070</v>
@@ -11427,37 +11424,41 @@
         <v>1081</v>
       </c>
       <c r="L51" s="5">
-        <v>100</v>
+        <v>1550</v>
       </c>
       <c r="M51" s="5" t="s">
         <v>1072</v>
       </c>
       <c r="N51" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="O51" s="14" t="s">
-        <v>1073</v>
+        <v>360</v>
       </c>
       <c r="P51" s="14"/>
     </row>
     <row r="52" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A52" s="30" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>17</v>
+        <v>937</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
+      <c r="D52" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="E52" s="14">
+        <v>0.13</v>
+      </c>
       <c r="F52" s="7">
-        <f>F51*0.207*1000</f>
-        <v>31.049999999999997</v>
+        <f>(IF(Patient!C2="Male",D52,E52)/1)*(Patient!C13/Patient!C17)</f>
+        <v>0.15</v>
       </c>
       <c r="G52" s="17" t="s">
-        <v>1047</v>
+        <v>273</v>
       </c>
       <c r="H52" s="26" t="s">
         <v>1070</v>
@@ -11476,16 +11477,16 @@
         <v>1072</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O52" s="14" t="s">
-        <v>360</v>
+        <v>1073</v>
       </c>
       <c r="P52" s="14"/>
     </row>
     <row r="53" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A53" s="30" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>17</v>
@@ -11496,8 +11497,8 @@
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="7">
-        <f>F51*0.579*1000</f>
-        <v>86.85</v>
+        <f>F52*0.207*1000</f>
+        <v>31.049999999999997</v>
       </c>
       <c r="G53" s="17" t="s">
         <v>1047</v>
@@ -11526,97 +11527,102 @@
       </c>
       <c r="P53" s="14"/>
     </row>
-    <row r="54" spans="1:16" ht="24">
-      <c r="A54" s="28" t="s">
+    <row r="54" spans="1:16" s="1" customFormat="1" ht="12">
+      <c r="A54" s="30" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="7">
+        <f>F52*0.579*1000</f>
+        <v>86.85</v>
+      </c>
+      <c r="G54" s="17" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H54" s="26" t="s">
+        <v>1070</v>
+      </c>
+      <c r="I54" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="J54" s="17"/>
+      <c r="K54" s="33" t="s">
+        <v>1081</v>
+      </c>
+      <c r="L54" s="5">
+        <v>100</v>
+      </c>
+      <c r="M54" s="5" t="s">
+        <v>1072</v>
+      </c>
+      <c r="N54" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O54" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="P54" s="14"/>
+    </row>
+    <row r="55" spans="1:16" ht="24">
+      <c r="A55" s="28" t="s">
         <v>1120</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C55" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="D55" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E54" s="9" t="s">
+      <c r="E55" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F54" s="9" t="s">
+      <c r="F55" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="G54" s="29" t="s">
+      <c r="G55" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="H54" s="29" t="s">
+      <c r="H55" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="I54" s="3" t="s">
+      <c r="I55" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J54" s="3" t="s">
+      <c r="J55" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K54" s="3" t="s">
+      <c r="K55" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L54" s="29" t="s">
+      <c r="L55" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="M54" s="9" t="s">
+      <c r="M55" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N54" s="9" t="s">
+      <c r="N55" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="O54" s="9" t="s">
+      <c r="O55" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P54" s="9" t="s">
+      <c r="P55" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="24.75">
-      <c r="A55" s="30" t="s">
+    <row r="56" spans="1:16" ht="24.75">
+      <c r="A56" s="30" t="s">
         <v>1121</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="18" t="s">
-        <v>1122</v>
-      </c>
-      <c r="G55" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J55" s="18"/>
-      <c r="K55" s="114" t="s">
-        <v>1123</v>
-      </c>
-      <c r="L55" s="14"/>
-      <c r="M55" s="5" t="s">
-        <v>1124</v>
-      </c>
-      <c r="N55" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O55" s="14" t="s">
-        <v>1073</v>
-      </c>
-      <c r="P55" s="14"/>
-    </row>
-    <row r="56" spans="1:16">
-      <c r="A56" s="30" t="s">
-        <v>1125</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>89</v>
@@ -11626,19 +11632,21 @@
       </c>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
-      <c r="F56" s="8">
-        <v>0</v>
-      </c>
-      <c r="G56" s="18"/>
-      <c r="H56" s="8"/>
+      <c r="F56" s="18" t="s">
+        <v>1122</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="H56" s="18"/>
       <c r="I56" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="35" t="s">
-        <v>1049</v>
-      </c>
+      <c r="J56" s="18"/>
+      <c r="K56" s="114" t="s">
+        <v>1123</v>
+      </c>
+      <c r="L56" s="14"/>
       <c r="M56" s="5" t="s">
         <v>1124</v>
       </c>
@@ -11652,7 +11660,7 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="30" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>89</v>
@@ -11662,22 +11670,18 @@
       </c>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
-      <c r="F57" s="17">
-        <v>25</v>
-      </c>
-      <c r="G57" s="18" t="s">
-        <v>1127</v>
-      </c>
-      <c r="H57" s="17" t="s">
-        <v>1128</v>
-      </c>
+      <c r="F57" s="8">
+        <v>0</v>
+      </c>
+      <c r="G57" s="18"/>
+      <c r="H57" s="8"/>
       <c r="I57" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J57" s="17"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="12" t="s">
-        <v>1051</v>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+      <c r="L57" s="35" t="s">
+        <v>1049</v>
       </c>
       <c r="M57" s="5" t="s">
         <v>1124</v>
@@ -11692,7 +11696,7 @@
     </row>
     <row r="58" spans="1:16">
       <c r="A58" s="30" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="B58" s="18" t="s">
         <v>89</v>
@@ -11703,7 +11707,7 @@
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="17">
-        <v>1.2</v>
+        <v>25</v>
       </c>
       <c r="G58" s="18" t="s">
         <v>1127</v>
@@ -11716,8 +11720,8 @@
       </c>
       <c r="J58" s="17"/>
       <c r="K58" s="19"/>
-      <c r="L58" s="8" t="s">
-        <v>1057</v>
+      <c r="L58" s="12" t="s">
+        <v>1051</v>
       </c>
       <c r="M58" s="5" t="s">
         <v>1124</v>
@@ -11730,31 +11734,35 @@
       </c>
       <c r="P58" s="14"/>
     </row>
-    <row r="59" spans="1:16" ht="24">
+    <row r="59" spans="1:16">
       <c r="A59" s="30" t="s">
-        <v>1130</v>
-      </c>
-      <c r="B59" s="115" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B59" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C59" s="116" t="s">
-        <v>46</v>
-      </c>
-      <c r="D59" s="115"/>
-      <c r="E59" s="115"/>
-      <c r="F59" s="116" t="s">
-        <v>1131</v>
-      </c>
-      <c r="G59" s="115"/>
-      <c r="H59" s="116"/>
-      <c r="I59" s="116" t="s">
-        <v>49</v>
-      </c>
-      <c r="J59" s="116"/>
-      <c r="K59" s="116" t="s">
-        <v>1132</v>
-      </c>
-      <c r="L59" s="8"/>
+      <c r="C59" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="17">
+        <v>1.2</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H59" s="17" t="s">
+        <v>1128</v>
+      </c>
+      <c r="I59" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J59" s="17"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="8" t="s">
+        <v>1057</v>
+      </c>
       <c r="M59" s="5" t="s">
         <v>1124</v>
       </c>
@@ -11766,33 +11774,31 @@
       </c>
       <c r="P59" s="14"/>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" ht="24">
       <c r="A60" s="30" t="s">
-        <v>1133</v>
-      </c>
-      <c r="B60" s="18" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B60" s="115" t="s">
         <v>89</v>
       </c>
-      <c r="C60" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="20">
-        <v>116</v>
-      </c>
-      <c r="G60" s="18" t="s">
-        <v>1127</v>
-      </c>
-      <c r="H60" s="17" t="s">
-        <v>1128</v>
-      </c>
-      <c r="I60" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J60" s="17"/>
-      <c r="K60" s="33"/>
-      <c r="L60" s="14"/>
+      <c r="C60" s="116" t="s">
+        <v>46</v>
+      </c>
+      <c r="D60" s="115"/>
+      <c r="E60" s="115"/>
+      <c r="F60" s="116" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G60" s="115"/>
+      <c r="H60" s="116"/>
+      <c r="I60" s="116" t="s">
+        <v>49</v>
+      </c>
+      <c r="J60" s="116"/>
+      <c r="K60" s="116" t="s">
+        <v>1132</v>
+      </c>
+      <c r="L60" s="8"/>
       <c r="M60" s="5" t="s">
         <v>1124</v>
       </c>
@@ -11804,24 +11810,32 @@
       </c>
       <c r="P60" s="14"/>
     </row>
-    <row r="61" spans="1:16" ht="36.75">
+    <row r="61" spans="1:16">
       <c r="A61" s="30" t="s">
-        <v>1134</v>
-      </c>
-      <c r="B61" s="115"/>
-      <c r="C61" s="116"/>
-      <c r="D61" s="115"/>
-      <c r="E61" s="115"/>
-      <c r="F61" s="115"/>
-      <c r="G61" s="115"/>
-      <c r="H61" s="115"/>
-      <c r="I61" s="115" t="s">
-        <v>49</v>
-      </c>
-      <c r="J61" s="116"/>
-      <c r="K61" s="117" t="s">
-        <v>1135</v>
-      </c>
+        <v>1133</v>
+      </c>
+      <c r="B61" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="20">
+        <v>116</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H61" s="17" t="s">
+        <v>1128</v>
+      </c>
+      <c r="I61" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J61" s="17"/>
+      <c r="K61" s="33"/>
       <c r="L61" s="14"/>
       <c r="M61" s="5" t="s">
         <v>1124</v>
@@ -11834,35 +11848,25 @@
       </c>
       <c r="P61" s="14"/>
     </row>
-    <row r="62" spans="1:16" ht="72.75">
+    <row r="62" spans="1:16" ht="36.75">
       <c r="A62" s="30" t="s">
-        <v>1136</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="8" t="s">
-        <v>1138</v>
-      </c>
-      <c r="G62" s="17" t="s">
-        <v>1139</v>
-      </c>
-      <c r="H62" s="17" t="s">
-        <v>1140</v>
-      </c>
-      <c r="I62" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J62" s="17"/>
-      <c r="K62" s="114" t="s">
-        <v>1141</v>
-      </c>
-      <c r="L62" s="4"/>
+        <v>1134</v>
+      </c>
+      <c r="B62" s="115"/>
+      <c r="C62" s="116"/>
+      <c r="D62" s="115"/>
+      <c r="E62" s="115"/>
+      <c r="F62" s="115"/>
+      <c r="G62" s="115"/>
+      <c r="H62" s="115"/>
+      <c r="I62" s="115" t="s">
+        <v>49</v>
+      </c>
+      <c r="J62" s="116"/>
+      <c r="K62" s="117" t="s">
+        <v>1135</v>
+      </c>
+      <c r="L62" s="14"/>
       <c r="M62" s="5" t="s">
         <v>1124</v>
       </c>
@@ -11874,33 +11878,35 @@
       </c>
       <c r="P62" s="14"/>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" ht="72.75">
       <c r="A63" s="30" t="s">
-        <v>1142</v>
-      </c>
-      <c r="B63" s="18" t="s">
-        <v>89</v>
+        <v>1136</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>1137</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
-      <c r="F63" s="8">
-        <v>5.9</v>
+      <c r="F63" s="8" t="s">
+        <v>1138</v>
       </c>
       <c r="G63" s="17" t="s">
-        <v>1127</v>
+        <v>1139</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>1128</v>
+        <v>1140</v>
       </c>
       <c r="I63" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J63" s="17"/>
-      <c r="K63" s="33"/>
-      <c r="L63" s="21"/>
+      <c r="K63" s="114" t="s">
+        <v>1141</v>
+      </c>
+      <c r="L63" s="4"/>
       <c r="M63" s="5" t="s">
         <v>1124</v>
       </c>
@@ -11914,7 +11920,7 @@
     </row>
     <row r="64" spans="1:16">
       <c r="A64" s="30" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B64" s="18" t="s">
         <v>89</v>
@@ -11924,19 +11930,21 @@
       </c>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
-      <c r="F64" s="26">
-        <v>0</v>
-      </c>
-      <c r="G64" s="17"/>
-      <c r="H64" s="26"/>
+      <c r="F64" s="8">
+        <v>5.9</v>
+      </c>
+      <c r="G64" s="17" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H64" s="17" t="s">
+        <v>1128</v>
+      </c>
       <c r="I64" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J64" s="26"/>
-      <c r="K64" s="33" t="s">
-        <v>1144</v>
-      </c>
-      <c r="L64" s="4"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="33"/>
+      <c r="L64" s="21"/>
       <c r="M64" s="5" t="s">
         <v>1124</v>
       </c>
@@ -11948,33 +11956,29 @@
       </c>
       <c r="P64" s="14"/>
     </row>
-    <row r="65" spans="1:16" ht="24.75">
+    <row r="65" spans="1:16">
       <c r="A65" s="30" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B65" s="26" t="s">
-        <v>1137</v>
+        <v>1143</v>
+      </c>
+      <c r="B65" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
-      <c r="F65" s="26" t="s">
-        <v>1146</v>
-      </c>
-      <c r="G65" s="17" t="s">
-        <v>1147</v>
-      </c>
-      <c r="H65" s="26" t="s">
-        <v>1148</v>
-      </c>
+      <c r="F65" s="26">
+        <v>0</v>
+      </c>
+      <c r="G65" s="17"/>
+      <c r="H65" s="26"/>
       <c r="I65" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J65" s="5"/>
-      <c r="K65" s="114" t="s">
-        <v>1123</v>
+      <c r="J65" s="26"/>
+      <c r="K65" s="33" t="s">
+        <v>1144</v>
       </c>
       <c r="L65" s="4"/>
       <c r="M65" s="5" t="s">
@@ -11988,12 +11992,12 @@
       </c>
       <c r="P65" s="14"/>
     </row>
-    <row r="66" spans="1:16" ht="48.75">
+    <row r="66" spans="1:16" ht="24.75">
       <c r="A66" s="30" t="s">
-        <v>1149</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>89</v>
+        <v>1145</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>1137</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>46</v>
@@ -12001,20 +12005,20 @@
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
       <c r="F66" s="26" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="G66" s="17" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="H66" s="26" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="I66" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J66" s="5"/>
-      <c r="K66" s="33" t="s">
-        <v>1153</v>
+      <c r="K66" s="114" t="s">
+        <v>1123</v>
       </c>
       <c r="L66" s="4"/>
       <c r="M66" s="5" t="s">
@@ -12028,23 +12032,33 @@
       </c>
       <c r="P66" s="14"/>
     </row>
-    <row r="67" spans="1:16" ht="24">
+    <row r="67" spans="1:16" ht="48.75">
       <c r="A67" s="30" t="s">
-        <v>1154</v>
-      </c>
-      <c r="B67" s="115"/>
-      <c r="C67" s="116"/>
-      <c r="D67" s="115"/>
-      <c r="E67" s="115"/>
-      <c r="F67" s="116"/>
-      <c r="G67" s="116"/>
-      <c r="H67" s="116"/>
-      <c r="I67" s="116" t="s">
-        <v>49</v>
-      </c>
-      <c r="J67" s="116"/>
-      <c r="K67" s="115" t="s">
-        <v>1155</v>
+        <v>1149</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="26" t="s">
+        <v>1150</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>1151</v>
+      </c>
+      <c r="H67" s="26" t="s">
+        <v>1152</v>
+      </c>
+      <c r="I67" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J67" s="5"/>
+      <c r="K67" s="33" t="s">
+        <v>1153</v>
       </c>
       <c r="L67" s="4"/>
       <c r="M67" s="5" t="s">
@@ -12058,32 +12072,24 @@
       </c>
       <c r="P67" s="14"/>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" ht="24">
       <c r="A68" s="30" t="s">
-        <v>1156</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>1137</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="26" t="s">
-        <v>1157</v>
-      </c>
-      <c r="G68" s="17" t="s">
-        <v>1151</v>
-      </c>
-      <c r="H68" s="26" t="s">
-        <v>1158</v>
-      </c>
-      <c r="I68" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J68" s="8"/>
-      <c r="K68" s="26"/>
+        <v>1154</v>
+      </c>
+      <c r="B68" s="115"/>
+      <c r="C68" s="116"/>
+      <c r="D68" s="115"/>
+      <c r="E68" s="115"/>
+      <c r="F68" s="116"/>
+      <c r="G68" s="116"/>
+      <c r="H68" s="116"/>
+      <c r="I68" s="116" t="s">
+        <v>49</v>
+      </c>
+      <c r="J68" s="116"/>
+      <c r="K68" s="115" t="s">
+        <v>1155</v>
+      </c>
       <c r="L68" s="4"/>
       <c r="M68" s="5" t="s">
         <v>1124</v>
@@ -12096,30 +12102,32 @@
       </c>
       <c r="P68" s="14"/>
     </row>
-    <row r="69" spans="1:16" ht="24">
+    <row r="69" spans="1:16">
       <c r="A69" s="30" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>89</v>
+        <v>1137</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
-      <c r="F69" s="8" t="s">
-        <v>1160</v>
-      </c>
-      <c r="G69" s="17"/>
-      <c r="H69" s="8"/>
+      <c r="F69" s="26" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G69" s="17" t="s">
+        <v>1151</v>
+      </c>
+      <c r="H69" s="26" t="s">
+        <v>1158</v>
+      </c>
       <c r="I69" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J69" s="8"/>
-      <c r="K69" s="116" t="s">
-        <v>1132</v>
-      </c>
+      <c r="K69" s="26"/>
       <c r="L69" s="4"/>
       <c r="M69" s="5" t="s">
         <v>1124</v>
@@ -12132,9 +12140,9 @@
       </c>
       <c r="P69" s="14"/>
     </row>
-    <row r="70" spans="1:16">
-      <c r="A70" s="10" t="s">
-        <v>1161</v>
+    <row r="70" spans="1:16" ht="24">
+      <c r="A70" s="30" t="s">
+        <v>1159</v>
       </c>
       <c r="B70" s="18" t="s">
         <v>89</v>
@@ -12144,20 +12152,18 @@
       </c>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
-      <c r="F70" s="18">
-        <v>4.5</v>
-      </c>
-      <c r="G70" s="18" t="s">
-        <v>1127</v>
-      </c>
-      <c r="H70" s="18" t="s">
-        <v>1128</v>
-      </c>
+      <c r="F70" s="8" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G70" s="17"/>
+      <c r="H70" s="8"/>
       <c r="I70" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J70" s="26"/>
-      <c r="K70" s="33"/>
+      <c r="J70" s="8"/>
+      <c r="K70" s="116" t="s">
+        <v>1132</v>
+      </c>
       <c r="L70" s="4"/>
       <c r="M70" s="5" t="s">
         <v>1124</v>
@@ -12171,8 +12177,8 @@
       <c r="P70" s="14"/>
     </row>
     <row r="71" spans="1:16">
-      <c r="A71" s="30" t="s">
-        <v>1162</v>
+      <c r="A71" s="10" t="s">
+        <v>1161</v>
       </c>
       <c r="B71" s="18" t="s">
         <v>89</v>
@@ -12182,13 +12188,13 @@
       </c>
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
-      <c r="F71" s="26">
-        <v>145</v>
-      </c>
-      <c r="G71" s="17" t="s">
+      <c r="F71" s="18">
+        <v>4.5</v>
+      </c>
+      <c r="G71" s="18" t="s">
         <v>1127</v>
       </c>
-      <c r="H71" s="26" t="s">
+      <c r="H71" s="18" t="s">
         <v>1128</v>
       </c>
       <c r="I71" s="18" t="s">
@@ -12210,26 +12216,30 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" s="30" t="s">
-        <v>1163</v>
-      </c>
-      <c r="B72" s="36" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B72" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C72" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
-      <c r="G72" s="36"/>
-      <c r="H72" s="36"/>
-      <c r="I72" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J72" s="118"/>
-      <c r="K72" s="114" t="s">
-        <v>1164</v>
-      </c>
+      <c r="C72" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="26">
+        <v>145</v>
+      </c>
+      <c r="G72" s="17" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H72" s="26" t="s">
+        <v>1128</v>
+      </c>
+      <c r="I72" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J72" s="26"/>
+      <c r="K72" s="33"/>
       <c r="L72" s="4"/>
       <c r="M72" s="5" t="s">
         <v>1124</v>
@@ -12242,31 +12252,27 @@
       </c>
       <c r="P72" s="14"/>
     </row>
-    <row r="73" spans="1:16" ht="36">
+    <row r="73" spans="1:16">
       <c r="A73" s="30" t="s">
-        <v>1165</v>
-      </c>
-      <c r="B73" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="G73" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="H73" s="26"/>
-      <c r="I73" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J73" s="119"/>
-      <c r="K73" s="47" t="s">
-        <v>1166</v>
+        <v>1163</v>
+      </c>
+      <c r="B73" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C73" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="36"/>
+      <c r="G73" s="36"/>
+      <c r="H73" s="36"/>
+      <c r="I73" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="J73" s="118"/>
+      <c r="K73" s="114" t="s">
+        <v>1164</v>
       </c>
       <c r="L73" s="4"/>
       <c r="M73" s="5" t="s">
@@ -12280,29 +12286,31 @@
       </c>
       <c r="P73" s="14"/>
     </row>
-    <row r="74" spans="1:16" ht="24.75">
+    <row r="74" spans="1:16" ht="36">
       <c r="A74" s="30" t="s">
-        <v>1167</v>
-      </c>
-      <c r="B74" s="18" t="s">
-        <v>89</v>
+        <v>1165</v>
+      </c>
+      <c r="B74" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
-      <c r="F74" s="18" t="s">
-        <v>1122</v>
-      </c>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
+      <c r="F74" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="G74" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="H74" s="26"/>
       <c r="I74" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J74" s="18"/>
-      <c r="K74" s="114" t="s">
-        <v>1123</v>
+      <c r="J74" s="119"/>
+      <c r="K74" s="47" t="s">
+        <v>1166</v>
       </c>
       <c r="L74" s="4"/>
       <c r="M74" s="5" t="s">
@@ -12316,9 +12324,9 @@
       </c>
       <c r="P74" s="14"/>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" ht="24.75">
       <c r="A75" s="30" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B75" s="18" t="s">
         <v>89</v>
@@ -12328,17 +12336,17 @@
       </c>
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
-      <c r="F75" s="8">
-        <v>0</v>
+      <c r="F75" s="18" t="s">
+        <v>1122</v>
       </c>
       <c r="G75" s="18"/>
-      <c r="H75" s="8"/>
+      <c r="H75" s="18"/>
       <c r="I75" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J75" s="8"/>
-      <c r="K75" s="35" t="s">
-        <v>1169</v>
+      <c r="J75" s="18"/>
+      <c r="K75" s="114" t="s">
+        <v>1123</v>
       </c>
       <c r="L75" s="4"/>
       <c r="M75" s="5" t="s">
@@ -12354,7 +12362,7 @@
     </row>
     <row r="76" spans="1:16">
       <c r="A76" s="30" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="B76" s="18" t="s">
         <v>89</v>
@@ -12364,20 +12372,18 @@
       </c>
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
-      <c r="F76" s="17">
-        <v>16</v>
-      </c>
-      <c r="G76" s="18" t="s">
-        <v>1127</v>
-      </c>
-      <c r="H76" s="17" t="s">
-        <v>1128</v>
-      </c>
+      <c r="F76" s="8">
+        <v>0</v>
+      </c>
+      <c r="G76" s="18"/>
+      <c r="H76" s="8"/>
       <c r="I76" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J76" s="17"/>
-      <c r="K76" s="19"/>
+      <c r="J76" s="8"/>
+      <c r="K76" s="35" t="s">
+        <v>1169</v>
+      </c>
       <c r="L76" s="4"/>
       <c r="M76" s="5" t="s">
         <v>1124</v>
@@ -12392,7 +12398,7 @@
     </row>
     <row r="77" spans="1:16">
       <c r="A77" s="30" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="B77" s="18" t="s">
         <v>89</v>
@@ -12403,7 +12409,7 @@
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
       <c r="F77" s="17">
-        <v>1E-4</v>
+        <v>16</v>
       </c>
       <c r="G77" s="18" t="s">
         <v>1127</v>
@@ -12428,30 +12434,32 @@
       </c>
       <c r="P77" s="14"/>
     </row>
-    <row r="78" spans="1:16" ht="24">
+    <row r="78" spans="1:16">
       <c r="A78" s="30" t="s">
-        <v>1172</v>
-      </c>
-      <c r="B78" s="115" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B78" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C78" s="116" t="s">
-        <v>46</v>
-      </c>
-      <c r="D78" s="115"/>
-      <c r="E78" s="115"/>
-      <c r="F78" s="116" t="s">
-        <v>1131</v>
-      </c>
-      <c r="G78" s="115"/>
-      <c r="H78" s="116"/>
-      <c r="I78" s="116" t="s">
-        <v>49</v>
-      </c>
-      <c r="J78" s="116"/>
-      <c r="K78" s="116" t="s">
-        <v>1132</v>
-      </c>
+      <c r="C78" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="17">
+        <v>1E-4</v>
+      </c>
+      <c r="G78" s="18" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H78" s="17" t="s">
+        <v>1128</v>
+      </c>
+      <c r="I78" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J78" s="17"/>
+      <c r="K78" s="19"/>
       <c r="L78" s="4"/>
       <c r="M78" s="5" t="s">
         <v>1124</v>
@@ -12464,32 +12472,30 @@
       </c>
       <c r="P78" s="14"/>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" ht="24">
       <c r="A79" s="30" t="s">
-        <v>1173</v>
-      </c>
-      <c r="B79" s="18" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B79" s="115" t="s">
         <v>89</v>
       </c>
-      <c r="C79" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
-      <c r="F79" s="20">
-        <v>20</v>
-      </c>
-      <c r="G79" s="18" t="s">
-        <v>1127</v>
-      </c>
-      <c r="H79" s="17" t="s">
-        <v>1128</v>
-      </c>
-      <c r="I79" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J79" s="17"/>
-      <c r="K79" s="33"/>
+      <c r="C79" s="116" t="s">
+        <v>46</v>
+      </c>
+      <c r="D79" s="115"/>
+      <c r="E79" s="115"/>
+      <c r="F79" s="116" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G79" s="115"/>
+      <c r="H79" s="116"/>
+      <c r="I79" s="116" t="s">
+        <v>49</v>
+      </c>
+      <c r="J79" s="116"/>
+      <c r="K79" s="116" t="s">
+        <v>1132</v>
+      </c>
       <c r="L79" s="4"/>
       <c r="M79" s="5" t="s">
         <v>1124</v>
@@ -12502,9 +12508,9 @@
       </c>
       <c r="P79" s="14"/>
     </row>
-    <row r="80" spans="1:16" ht="36.75">
+    <row r="80" spans="1:16">
       <c r="A80" s="30" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B80" s="18" t="s">
         <v>89</v>
@@ -12514,16 +12520,20 @@
       </c>
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
-      <c r="F80" s="18"/>
-      <c r="G80" s="18"/>
-      <c r="H80" s="18"/>
+      <c r="F80" s="20">
+        <v>20</v>
+      </c>
+      <c r="G80" s="18" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H80" s="17" t="s">
+        <v>1128</v>
+      </c>
       <c r="I80" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J80" s="17"/>
-      <c r="K80" s="114" t="s">
-        <v>1175</v>
-      </c>
+      <c r="K80" s="33"/>
       <c r="L80" s="4"/>
       <c r="M80" s="5" t="s">
         <v>1124</v>
@@ -12536,33 +12546,27 @@
       </c>
       <c r="P80" s="14"/>
     </row>
-    <row r="81" spans="1:16" ht="72.75">
+    <row r="81" spans="1:16" ht="36.75">
       <c r="A81" s="30" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B81" s="17" t="s">
-        <v>1137</v>
+        <v>1174</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
-      <c r="F81" s="8" t="s">
-        <v>1138</v>
-      </c>
-      <c r="G81" s="17" t="s">
-        <v>1139</v>
-      </c>
-      <c r="H81" s="17" t="s">
-        <v>1140</v>
-      </c>
+      <c r="F81" s="18"/>
+      <c r="G81" s="18"/>
+      <c r="H81" s="18"/>
       <c r="I81" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J81" s="17"/>
       <c r="K81" s="114" t="s">
-        <v>1141</v>
+        <v>1175</v>
       </c>
       <c r="L81" s="4"/>
       <c r="M81" s="5" t="s">
@@ -12576,33 +12580,35 @@
       </c>
       <c r="P81" s="14"/>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" ht="72.75">
       <c r="A82" s="30" t="s">
-        <v>1177</v>
-      </c>
-      <c r="B82" s="18" t="s">
-        <v>89</v>
+        <v>1176</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>1137</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
-      <c r="F82" s="8">
-        <v>0</v>
+      <c r="F82" s="8" t="s">
+        <v>1138</v>
       </c>
       <c r="G82" s="17" t="s">
-        <v>1127</v>
+        <v>1139</v>
       </c>
       <c r="H82" s="17" t="s">
-        <v>1128</v>
+        <v>1140</v>
       </c>
       <c r="I82" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J82" s="17"/>
-      <c r="K82" s="33"/>
-      <c r="L82" s="21"/>
+      <c r="K82" s="114" t="s">
+        <v>1141</v>
+      </c>
+      <c r="L82" s="4"/>
       <c r="M82" s="5" t="s">
         <v>1124</v>
       </c>
@@ -12616,7 +12622,7 @@
     </row>
     <row r="83" spans="1:16">
       <c r="A83" s="30" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B83" s="18" t="s">
         <v>89</v>
@@ -12626,19 +12632,21 @@
       </c>
       <c r="D83" s="14"/>
       <c r="E83" s="14"/>
-      <c r="F83" s="26">
+      <c r="F83" s="8">
         <v>0</v>
       </c>
-      <c r="G83" s="17"/>
-      <c r="H83" s="26"/>
+      <c r="G83" s="17" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H83" s="17" t="s">
+        <v>1128</v>
+      </c>
       <c r="I83" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J83" s="26"/>
-      <c r="K83" s="33" t="s">
-        <v>1144</v>
-      </c>
-      <c r="L83" s="4"/>
+      <c r="J83" s="17"/>
+      <c r="K83" s="33"/>
+      <c r="L83" s="21"/>
       <c r="M83" s="5" t="s">
         <v>1124</v>
       </c>
@@ -12650,33 +12658,29 @@
       </c>
       <c r="P83" s="14"/>
     </row>
-    <row r="84" spans="1:16" ht="24.75">
+    <row r="84" spans="1:16">
       <c r="A84" s="30" t="s">
-        <v>1179</v>
-      </c>
-      <c r="B84" s="26" t="s">
-        <v>1137</v>
+        <v>1178</v>
+      </c>
+      <c r="B84" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
-      <c r="F84" s="26" t="s">
-        <v>1146</v>
-      </c>
-      <c r="G84" s="17" t="s">
-        <v>1147</v>
-      </c>
-      <c r="H84" s="26" t="s">
-        <v>1148</v>
-      </c>
+      <c r="F84" s="26">
+        <v>0</v>
+      </c>
+      <c r="G84" s="17"/>
+      <c r="H84" s="26"/>
       <c r="I84" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J84" s="5"/>
-      <c r="K84" s="114" t="s">
-        <v>1123</v>
+      <c r="J84" s="26"/>
+      <c r="K84" s="33" t="s">
+        <v>1144</v>
       </c>
       <c r="L84" s="4"/>
       <c r="M84" s="5" t="s">
@@ -12690,12 +12694,12 @@
       </c>
       <c r="P84" s="14"/>
     </row>
-    <row r="85" spans="1:16" ht="48.75">
+    <row r="85" spans="1:16" ht="24.75">
       <c r="A85" s="30" t="s">
-        <v>1180</v>
-      </c>
-      <c r="B85" s="18" t="s">
-        <v>89</v>
+        <v>1179</v>
+      </c>
+      <c r="B85" s="26" t="s">
+        <v>1137</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>46</v>
@@ -12703,20 +12707,20 @@
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
       <c r="F85" s="26" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="G85" s="17" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="H85" s="26" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="I85" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J85" s="5"/>
-      <c r="K85" s="33" t="s">
-        <v>1153</v>
+      <c r="K85" s="114" t="s">
+        <v>1123</v>
       </c>
       <c r="L85" s="4"/>
       <c r="M85" s="5" t="s">
@@ -12730,9 +12734,9 @@
       </c>
       <c r="P85" s="14"/>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" ht="48.75">
       <c r="A86" s="30" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B86" s="18" t="s">
         <v>89</v>
@@ -12742,14 +12746,22 @@
       </c>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
-      <c r="F86" s="8"/>
-      <c r="G86" s="17"/>
-      <c r="H86" s="8"/>
+      <c r="F86" s="26" t="s">
+        <v>1150</v>
+      </c>
+      <c r="G86" s="17" t="s">
+        <v>1151</v>
+      </c>
+      <c r="H86" s="26" t="s">
+        <v>1152</v>
+      </c>
       <c r="I86" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J86" s="8"/>
-      <c r="K86" s="26"/>
+      <c r="J86" s="5"/>
+      <c r="K86" s="33" t="s">
+        <v>1153</v>
+      </c>
       <c r="L86" s="4"/>
       <c r="M86" s="5" t="s">
         <v>1124</v>
@@ -12764,25 +12776,19 @@
     </row>
     <row r="87" spans="1:16">
       <c r="A87" s="30" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>1137</v>
+        <v>89</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
-      <c r="F87" s="26" t="s">
-        <v>1157</v>
-      </c>
-      <c r="G87" s="17" t="s">
-        <v>1151</v>
-      </c>
-      <c r="H87" s="26" t="s">
-        <v>1158</v>
-      </c>
+      <c r="F87" s="8"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="8"/>
       <c r="I87" s="18" t="s">
         <v>49</v>
       </c>
@@ -12800,30 +12806,32 @@
       </c>
       <c r="P87" s="14"/>
     </row>
-    <row r="88" spans="1:16" ht="24">
+    <row r="88" spans="1:16">
       <c r="A88" s="30" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>89</v>
+        <v>1137</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
-      <c r="F88" s="8" t="s">
-        <v>1160</v>
-      </c>
-      <c r="G88" s="17"/>
-      <c r="H88" s="8"/>
+      <c r="F88" s="26" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G88" s="17" t="s">
+        <v>1151</v>
+      </c>
+      <c r="H88" s="26" t="s">
+        <v>1158</v>
+      </c>
       <c r="I88" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J88" s="8"/>
-      <c r="K88" s="116" t="s">
-        <v>1132</v>
-      </c>
+      <c r="K88" s="26"/>
       <c r="L88" s="4"/>
       <c r="M88" s="5" t="s">
         <v>1124</v>
@@ -12836,9 +12844,9 @@
       </c>
       <c r="P88" s="14"/>
     </row>
-    <row r="89" spans="1:16">
-      <c r="A89" s="10" t="s">
-        <v>1184</v>
+    <row r="89" spans="1:16" ht="24">
+      <c r="A89" s="30" t="s">
+        <v>1183</v>
       </c>
       <c r="B89" s="18" t="s">
         <v>89</v>
@@ -12848,20 +12856,18 @@
       </c>
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
-      <c r="F89" s="18">
-        <v>120</v>
-      </c>
-      <c r="G89" s="18" t="s">
-        <v>1127</v>
-      </c>
-      <c r="H89" s="18" t="s">
-        <v>1128</v>
-      </c>
+      <c r="F89" s="8" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G89" s="17"/>
+      <c r="H89" s="8"/>
       <c r="I89" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J89" s="26"/>
-      <c r="K89" s="33"/>
+      <c r="J89" s="8"/>
+      <c r="K89" s="116" t="s">
+        <v>1132</v>
+      </c>
       <c r="L89" s="4"/>
       <c r="M89" s="5" t="s">
         <v>1124</v>
@@ -12875,8 +12881,8 @@
       <c r="P89" s="14"/>
     </row>
     <row r="90" spans="1:16">
-      <c r="A90" s="30" t="s">
-        <v>1185</v>
+      <c r="A90" s="10" t="s">
+        <v>1184</v>
       </c>
       <c r="B90" s="18" t="s">
         <v>89</v>
@@ -12886,13 +12892,13 @@
       </c>
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
-      <c r="F90" s="26">
-        <v>15</v>
-      </c>
-      <c r="G90" s="17" t="s">
+      <c r="F90" s="18">
+        <v>120</v>
+      </c>
+      <c r="G90" s="18" t="s">
         <v>1127</v>
       </c>
-      <c r="H90" s="26" t="s">
+      <c r="H90" s="18" t="s">
         <v>1128</v>
       </c>
       <c r="I90" s="18" t="s">
@@ -12914,26 +12920,30 @@
     </row>
     <row r="91" spans="1:16">
       <c r="A91" s="30" t="s">
-        <v>1186</v>
-      </c>
-      <c r="B91" s="36" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B91" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="D91" s="36"/>
-      <c r="E91" s="36"/>
-      <c r="F91" s="36"/>
-      <c r="G91" s="36"/>
-      <c r="H91" s="36"/>
-      <c r="I91" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J91" s="114"/>
-      <c r="K91" s="114" t="s">
-        <v>1164</v>
-      </c>
+      <c r="C91" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="26">
+        <v>15</v>
+      </c>
+      <c r="G91" s="17" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H91" s="26" t="s">
+        <v>1128</v>
+      </c>
+      <c r="I91" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J91" s="26"/>
+      <c r="K91" s="33"/>
       <c r="L91" s="4"/>
       <c r="M91" s="5" t="s">
         <v>1124</v>
@@ -12946,31 +12956,27 @@
       </c>
       <c r="P91" s="14"/>
     </row>
-    <row r="92" spans="1:16" ht="36">
+    <row r="92" spans="1:16">
       <c r="A92" s="30" t="s">
-        <v>1187</v>
-      </c>
-      <c r="B92" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
-      <c r="F92" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="G92" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="H92" s="26"/>
-      <c r="I92" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J92" s="19"/>
-      <c r="K92" s="33" t="s">
-        <v>1166</v>
+        <v>1186</v>
+      </c>
+      <c r="B92" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="C92" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D92" s="36"/>
+      <c r="E92" s="36"/>
+      <c r="F92" s="36"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="36"/>
+      <c r="I92" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="J92" s="114"/>
+      <c r="K92" s="114" t="s">
+        <v>1164</v>
       </c>
       <c r="L92" s="4"/>
       <c r="M92" s="5" t="s">
@@ -12983,6 +12989,44 @@
         <v>1073</v>
       </c>
       <c r="P92" s="14"/>
+    </row>
+    <row r="93" spans="1:16" ht="36">
+      <c r="A93" s="30" t="s">
+        <v>1187</v>
+      </c>
+      <c r="B93" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="G93" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="H93" s="26"/>
+      <c r="I93" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J93" s="19"/>
+      <c r="K93" s="33" t="s">
+        <v>1166</v>
+      </c>
+      <c r="L93" s="4"/>
+      <c r="M93" s="5" t="s">
+        <v>1124</v>
+      </c>
+      <c r="N93" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O93" s="14" t="s">
+        <v>1073</v>
+      </c>
+      <c r="P93" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -26313,7 +26357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G19" sqref="G19"/>
     </sheetView>

</xml_diff>

<commit_message>
Added Plasma Osmolality and Osmolarity calculation and Blood Chemistry validation.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\dehydration\source\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC967D77-C265-4B64-B878-DCF809F2D993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7D16DA-D8BF-4106-9787-AB4DAA447E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28770" yWindow="6540" windowWidth="27825" windowHeight="23535" tabRatio="500" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28770" yWindow="6540" windowWidth="27825" windowHeight="23535" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6598" uniqueCount="1194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6608" uniqueCount="1197">
   <si>
     <t>Patient Inputs</t>
   </si>
@@ -3758,6 +3758,15 @@
   </si>
   <si>
     <t>TotalFluidVolume</t>
+  </si>
+  <si>
+    <t>PlasmaOsmolality</t>
+  </si>
+  <si>
+    <t>[275,295]</t>
+  </si>
+  <si>
+    <t>PlasmaOsmolarity*</t>
   </si>
 </sst>
 </file>
@@ -9186,7 +9195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A67" sqref="A67"/>
       <selection pane="topRight" activeCell="K8" sqref="K8"/>
@@ -13036,17 +13045,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMH79"/>
+  <dimension ref="A1:AMH81"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8" style="2" customWidth="1"/>
     <col min="3" max="5" width="16.85546875" style="2" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="33.85546875" style="2" customWidth="1"/>
@@ -13576,108 +13585,87 @@
     </row>
     <row r="14" spans="1:16" ht="24">
       <c r="A14" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" s="8"/>
+        <v>1194</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>585</v>
+      </c>
       <c r="C14" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
-        <v>86</v>
+      <c r="F14" s="26" t="s">
+        <v>1195</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>87</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H14" s="26"/>
       <c r="I14" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="4"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="5"/>
       <c r="M14" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="O14" s="14" t="s">
         <v>52</v>
       </c>
       <c r="P14" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="24">
-      <c r="A15" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="22">
-        <f>(F10/0.000000000029)/(Patient!C7*1000)</f>
-        <v>5172413.793103449</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K15" s="25"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N15" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="O15" s="14" t="s">
-        <v>52</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="48" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B15" s="26"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="14"/>
       <c r="P15" s="14"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" ht="24">
       <c r="A16" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="B16" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>49</v>
       </c>
       <c r="J16" s="8"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="13"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="4"/>
       <c r="M16" s="5" t="s">
         <v>50</v>
       </c>
@@ -13688,363 +13676,358 @@
         <v>52</v>
       </c>
       <c r="P16" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="24">
       <c r="A17" s="10" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="20" t="s">
-        <v>107</v>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="22">
+        <f>(F10/0.000000000029)/(Patient!C7*1000)</f>
+        <v>5172413.793103449</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="H17" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="I17" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J17" s="8"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="13"/>
+      <c r="J17" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K17" s="25"/>
+      <c r="L17" s="21"/>
       <c r="M17" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="O17" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="P17" s="14">
-        <v>1</v>
-      </c>
+      <c r="P17" s="14"/>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="G18" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="H18" s="26" t="s">
-        <v>113</v>
+        <v>102</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>105</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="26"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="13"/>
       <c r="M18" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="O18" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="P18" s="14"/>
+      <c r="P18" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" s="12"/>
+        <v>106</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="C19" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="8">
-        <v>2.3E-3</v>
+      <c r="F19" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="H19" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="H19" s="8"/>
       <c r="I19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J19" s="12"/>
-      <c r="K19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="13"/>
       <c r="M19" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="O19" s="14" t="s">
         <v>52</v>
       </c>
       <c r="P19" s="14">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="H20" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>113</v>
+      </c>
       <c r="I20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J20" s="12"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="13"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
       <c r="M20" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="O20" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="P20" s="14">
-        <v>5</v>
-      </c>
+      <c r="P20" s="14"/>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>99</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B21" s="12"/>
       <c r="C21" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="27">
-        <v>7000</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>120</v>
-      </c>
+      <c r="F21" s="8">
+        <v>2.3E-3</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="12"/>
       <c r="I21" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J21" s="17"/>
-      <c r="K21" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="L21" s="4"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="13"/>
       <c r="M21" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="O21" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="P21" s="14"/>
-    </row>
-    <row r="22" spans="1:16" ht="24">
-      <c r="A22" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="G22" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="H22" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I22" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L22" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="O22" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="P22" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="56.25">
-      <c r="A23" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>128</v>
+      <c r="P21" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22" s="12"/>
+      <c r="I22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J22" s="12"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="P22" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J23" s="18"/>
-      <c r="K23" s="31" t="s">
-        <v>131</v>
+      <c r="F23" s="27">
+        <v>7000</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J23" s="17"/>
+      <c r="K23" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>71</v>
+        <v>122</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="P23" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="22.5">
-      <c r="A24" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="G24" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="I24" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J24" s="18"/>
-      <c r="K24" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="L24" s="4"/>
-      <c r="M24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N24" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O24" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="P24" s="14">
+        <v>52</v>
+      </c>
+      <c r="P23" s="14"/>
+    </row>
+    <row r="24" spans="1:16" ht="24">
+      <c r="A24" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="10" t="s">
-        <v>136</v>
+      <c r="C24" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I24" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L24" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N24" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O24" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="56.25">
+      <c r="A25" s="30" t="s">
+        <v>127</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="8" t="s">
-        <v>137</v>
+      <c r="F25" s="18" t="s">
+        <v>129</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>138</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="H25" s="18"/>
       <c r="I25" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8" t="s">
-        <v>139</v>
+      <c r="J25" s="18"/>
+      <c r="K25" s="31" t="s">
+        <v>131</v>
       </c>
       <c r="L25" s="4"/>
       <c r="M25" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
       <c r="O25" s="14" t="s">
         <v>132</v>
@@ -14053,33 +14036,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="10" t="s">
-        <v>141</v>
+    <row r="26" spans="1:16" ht="22.5">
+      <c r="A26" s="30" t="s">
+        <v>133</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="17" t="s">
-        <v>142</v>
+      <c r="F26" s="18" t="s">
+        <v>134</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>138</v>
+        <v>112</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>113</v>
       </c>
       <c r="I26" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J26" s="17"/>
-      <c r="K26" s="8" t="s">
-        <v>144</v>
+      <c r="J26" s="18"/>
+      <c r="K26" s="32" t="s">
+        <v>135</v>
       </c>
       <c r="L26" s="4"/>
       <c r="M26" s="5" t="s">
@@ -14092,56 +14075,56 @@
         <v>132</v>
       </c>
       <c r="P26" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="10" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
-      <c r="F27" s="17" t="s">
-        <v>147</v>
+      <c r="F27" s="8" t="s">
+        <v>137</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>149</v>
+        <v>112</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="I27" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J27" s="17"/>
+      <c r="J27" s="8"/>
       <c r="K27" s="8" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="L27" s="4"/>
       <c r="M27" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="O27" s="14" t="s">
         <v>132</v>
       </c>
       <c r="P27" s="14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="B28" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="18" t="s">
         <v>128</v>
       </c>
       <c r="C28" s="8" t="s">
@@ -14149,20 +14132,22 @@
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
-      <c r="F28" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>112</v>
+      <c r="F28" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>143</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="I28" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J28" s="17"/>
-      <c r="K28" s="4"/>
+      <c r="K28" s="8" t="s">
+        <v>144</v>
+      </c>
       <c r="L28" s="4"/>
       <c r="M28" s="5" t="s">
         <v>50</v>
@@ -14174,39 +14159,43 @@
         <v>132</v>
       </c>
       <c r="P28" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="36">
       <c r="A29" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>155</v>
+        <v>145</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>146</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="8"/>
-      <c r="F29" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G29" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="H29" s="17"/>
+      <c r="F29" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>149</v>
+      </c>
       <c r="I29" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J29" s="17"/>
-      <c r="K29" s="4"/>
+      <c r="K29" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="L29" s="4"/>
       <c r="M29" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
       <c r="O29" s="14" t="s">
         <v>132</v>
@@ -14215,26 +14204,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" ht="24">
       <c r="A30" s="10" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="G30" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="G30" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="H30" s="26" t="s">
-        <v>113</v>
+      <c r="H30" s="17" t="s">
+        <v>153</v>
       </c>
       <c r="I30" s="18" t="s">
         <v>49</v>
@@ -14255,82 +14244,71 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" ht="60">
       <c r="A31" s="10" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>66</v>
+        <v>155</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
-      <c r="F31" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>162</v>
+      <c r="F31" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="G31" s="17" t="s">
+        <v>157</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J31" s="17"/>
-      <c r="K31" s="4" t="s">
-        <v>163</v>
-      </c>
+      <c r="K31" s="4"/>
       <c r="L31" s="4"/>
       <c r="M31" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N31" s="5" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="O31" s="14" t="s">
         <v>132</v>
       </c>
       <c r="P31" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" ht="36.75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="B32" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F32" s="14" t="str">
-        <f>IF(Patient!C7&lt;&gt;"Male",D32,E32)</f>
-        <v>[13.8,17.2]</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H32" s="17" t="s">
-        <v>167</v>
+      <c r="C32" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="H32" s="26" t="s">
+        <v>113</v>
       </c>
       <c r="I32" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J32" s="17"/>
-      <c r="K32" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="L32" s="21" t="s">
-        <v>169</v>
-      </c>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
       <c r="M32" s="5" t="s">
         <v>50</v>
       </c>
@@ -14341,34 +14319,34 @@
         <v>132</v>
       </c>
       <c r="P32" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:16">
       <c r="A33" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>155</v>
+        <v>160</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>66</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
-      <c r="F33" s="26">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="G33" s="17" t="s">
+      <c r="F33" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="G33" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="H33" s="26"/>
+      <c r="H33" s="17"/>
       <c r="I33" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J33" s="26"/>
+      <c r="J33" s="17"/>
       <c r="K33" s="4" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="L33" s="4"/>
       <c r="M33" s="5" t="s">
@@ -14381,38 +14359,45 @@
         <v>132</v>
       </c>
       <c r="P33" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="36.75">
       <c r="A34" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>128</v>
+        <v>164</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="26" t="s">
-        <v>173</v>
+      <c r="D34" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F34" s="14" t="str">
+        <f>IF(Patient!C7&lt;&gt;"Male",D34,E34)</f>
+        <v>[13.8,17.2]</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="H34" s="26" t="s">
-        <v>175</v>
+        <v>15</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>167</v>
       </c>
       <c r="I34" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J34" s="5"/>
-      <c r="K34" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="L34" s="4"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="L34" s="21" t="s">
+        <v>169</v>
+      </c>
       <c r="M34" s="5" t="s">
         <v>50</v>
       </c>
@@ -14423,14 +14408,14 @@
         <v>132</v>
       </c>
       <c r="P34" s="14">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:16">
       <c r="A35" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="B35" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B35" s="18" t="s">
         <v>155</v>
       </c>
       <c r="C35" s="8" t="s">
@@ -14438,35 +14423,37 @@
       </c>
       <c r="D35" s="8"/>
       <c r="E35" s="8"/>
-      <c r="F35" s="26" t="s">
-        <v>178</v>
+      <c r="F35" s="26">
+        <v>0.40600000000000003</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J35" s="5"/>
-      <c r="K35" s="4"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="4" t="s">
+        <v>171</v>
+      </c>
       <c r="L35" s="4"/>
       <c r="M35" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
       <c r="O35" s="14" t="s">
         <v>132</v>
       </c>
       <c r="P35" s="14">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="24">
       <c r="A36" s="10" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>128</v>
@@ -14476,21 +14463,21 @@
       </c>
       <c r="D36" s="8"/>
       <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
-        <v>181</v>
+      <c r="F36" s="26" t="s">
+        <v>173</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>183</v>
+        <v>174</v>
+      </c>
+      <c r="H36" s="26" t="s">
+        <v>175</v>
       </c>
       <c r="I36" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J36" s="8"/>
+      <c r="J36" s="5"/>
       <c r="K36" s="4" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="5" t="s">
@@ -14503,37 +14490,33 @@
         <v>132</v>
       </c>
       <c r="P36" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>110</v>
+        <v>177</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>155</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="8"/>
-      <c r="F37" s="8" t="s">
-        <v>186</v>
+      <c r="F37" s="26" t="s">
+        <v>178</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>187</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="H37" s="26"/>
       <c r="I37" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J37" s="8"/>
-      <c r="K37" s="34" t="s">
-        <v>188</v>
-      </c>
+      <c r="J37" s="5"/>
+      <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="5" t="s">
         <v>50</v>
@@ -14545,36 +14528,36 @@
         <v>132</v>
       </c>
       <c r="P37" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="24">
       <c r="A38" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36" t="s">
-        <v>190</v>
-      </c>
-      <c r="G38" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="H38" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="I38" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="J38" s="36"/>
+        <v>180</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="G38" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J38" s="8"/>
       <c r="K38" s="4" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="5" t="s">
@@ -14586,129 +14569,123 @@
       <c r="O38" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="P38" s="14"/>
-    </row>
-    <row r="39" spans="1:16" ht="36">
+      <c r="P38" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="24">
       <c r="A39" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>66</v>
+        <v>185</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>110</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="8"/>
-      <c r="F39" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="G39" s="26" t="s">
-        <v>194</v>
-      </c>
-      <c r="H39" s="26"/>
+      <c r="F39" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="G39" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>187</v>
+      </c>
       <c r="I39" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J39" s="37" t="s">
-        <v>195</v>
-      </c>
-      <c r="K39" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="L39" s="39" t="s">
-        <v>197</v>
-      </c>
+      <c r="J39" s="8"/>
+      <c r="K39" s="34" t="s">
+        <v>188</v>
+      </c>
+      <c r="L39" s="4"/>
       <c r="M39" s="5" t="s">
         <v>50</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="O39" s="14" t="s">
         <v>132</v>
       </c>
       <c r="P39" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="24">
-      <c r="A40" s="28" t="s">
-        <v>198</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="G40" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="H40" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="I40" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K40" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L40" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="M40" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="N40" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="O40" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="P40" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="A40" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="36" t="s">
+        <v>190</v>
+      </c>
+      <c r="G40" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="H40" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="I40" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="J40" s="36"/>
+      <c r="K40" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="L40" s="4"/>
+      <c r="M40" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O40" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="P40" s="14"/>
+    </row>
+    <row r="41" spans="1:16" ht="36">
       <c r="A41" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>200</v>
+        <v>192</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>66</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8"/>
-      <c r="F41" s="8">
-        <v>40</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H41" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J41" s="8"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
+      <c r="F41" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="G41" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="H41" s="26"/>
+      <c r="I41" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J41" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="K41" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="L41" s="39" t="s">
+        <v>197</v>
+      </c>
       <c r="M41" s="5" t="s">
         <v>50</v>
       </c>
@@ -14716,51 +14693,65 @@
         <v>71</v>
       </c>
       <c r="O41" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="P41" s="14"/>
-    </row>
-    <row r="42" spans="1:16">
-      <c r="A42" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8">
-        <v>95</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="I42" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J42" s="8"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N42" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O42" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="P42" s="14"/>
+        <v>132</v>
+      </c>
+      <c r="P41" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="24">
+      <c r="A42" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G42" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="H42" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="I42" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L42" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="M42" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N42" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O42" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P42" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="43" spans="1:16">
       <c r="A43" s="10" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>200</v>
@@ -14770,8 +14761,8 @@
       </c>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
-      <c r="F43" s="20">
-        <v>45</v>
+      <c r="F43" s="8">
+        <v>40</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>15</v>
@@ -14798,7 +14789,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>200</v>
@@ -14808,14 +14799,14 @@
       </c>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
-      <c r="F44" s="20">
-        <v>40</v>
+      <c r="F44" s="8">
+        <v>95</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>49</v>
@@ -14836,7 +14827,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>200</v>
@@ -14847,13 +14838,13 @@
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
       <c r="F45" s="20">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>49</v>
@@ -14874,7 +14865,7 @@
     </row>
     <row r="46" spans="1:16">
       <c r="A46" s="10" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>200</v>
@@ -14885,7 +14876,7 @@
       <c r="D46" s="8"/>
       <c r="E46" s="8"/>
       <c r="F46" s="20">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>15</v>
@@ -14912,7 +14903,7 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" s="10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>200</v>
@@ -14922,14 +14913,14 @@
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="8"/>
-      <c r="F47" s="8">
+      <c r="F47" s="20">
         <v>40</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="I47" s="8" t="s">
         <v>49</v>
@@ -14950,7 +14941,7 @@
     </row>
     <row r="48" spans="1:16">
       <c r="A48" s="10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>200</v>
@@ -14960,14 +14951,14 @@
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="8"/>
-      <c r="F48" s="8">
-        <v>45</v>
+      <c r="F48" s="20">
+        <v>104</v>
       </c>
       <c r="G48" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H48" s="8" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>49</v>
@@ -14986,154 +14977,150 @@
       </c>
       <c r="P48" s="14"/>
     </row>
-    <row r="49" spans="1:16" ht="24">
-      <c r="A49" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I49" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="J49" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K49" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L49" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="M49" s="9" t="s">
+    <row r="49" spans="1:16">
+      <c r="A49" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8">
         <v>40</v>
       </c>
-      <c r="N49" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="O49" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="P49" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="24">
-      <c r="A50" s="40" t="s">
-        <v>58</v>
-      </c>
-      <c r="B50" s="8"/>
+      <c r="G49" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="I49" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J49" s="8"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="N49" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O49" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="P49" s="14"/>
+    </row>
+    <row r="50" spans="1:16">
+      <c r="A50" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>200</v>
+      </c>
       <c r="C50" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="8"/>
-      <c r="F50" s="8" t="s">
-        <v>59</v>
+      <c r="F50" s="8">
+        <v>45</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="H50" s="8" t="s">
-        <v>61</v>
+        <v>201</v>
       </c>
       <c r="I50" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="J50" s="4" t="s">
-        <v>213</v>
-      </c>
+      <c r="J50" s="8"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
       <c r="M50" s="5" t="s">
-        <v>214</v>
+        <v>50</v>
       </c>
       <c r="N50" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O50" s="14" t="s">
-        <v>215</v>
+        <v>52</v>
       </c>
       <c r="P50" s="14"/>
     </row>
-    <row r="51" spans="1:16">
-      <c r="A51" s="40" t="s">
-        <v>216</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="G51" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H51" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="I51" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J51" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="N51" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O51" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="P51" s="14"/>
-    </row>
-    <row r="52" spans="1:16">
+    <row r="51" spans="1:16" ht="24">
+      <c r="A51" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I51" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="J51" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K51" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L51" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M51" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N51" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O51" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P51" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="24">
       <c r="A52" s="40" t="s">
-        <v>219</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>200</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B52" s="8"/>
       <c r="C52" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="8"/>
-      <c r="F52" s="8">
-        <v>95</v>
+      <c r="F52" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>203</v>
+        <v>61</v>
       </c>
       <c r="I52" s="8" t="s">
         <v>49</v>
@@ -15156,30 +15143,30 @@
     </row>
     <row r="53" spans="1:16">
       <c r="A53" s="40" t="s">
-        <v>220</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>200</v>
+        <v>216</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
-      <c r="F53" s="8">
-        <v>40</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>15</v>
+      <c r="F53" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>112</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>201</v>
+        <v>138</v>
       </c>
       <c r="I53" s="8" t="s">
         <v>49</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
@@ -15194,24 +15181,26 @@
       </c>
       <c r="P53" s="14"/>
     </row>
-    <row r="54" spans="1:16" ht="24">
+    <row r="54" spans="1:16">
       <c r="A54" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="B54" s="8"/>
+        <v>219</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>200</v>
+      </c>
       <c r="C54" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="8"/>
-      <c r="F54" s="8" t="s">
-        <v>86</v>
+      <c r="F54" s="8">
+        <v>95</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>49</v>
@@ -15232,158 +15221,156 @@
       </c>
       <c r="P54" s="14"/>
     </row>
-    <row r="55" spans="1:16" ht="24">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:16">
+      <c r="A55" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8">
+        <v>40</v>
+      </c>
+      <c r="G55" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H55" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="I55" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N55" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O55" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="P55" s="14"/>
+    </row>
+    <row r="56" spans="1:16" ht="24">
+      <c r="A56" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H56" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="I56" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="N56" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O56" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="P56" s="14"/>
+    </row>
+    <row r="57" spans="1:16" ht="24">
+      <c r="A57" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B57" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C57" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9" t="s">
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G55" s="9" t="s">
+      <c r="G57" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H55" s="9" t="s">
+      <c r="H57" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I55" s="29" t="s">
+      <c r="I57" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="J55" s="9" t="s">
+      <c r="J57" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="K55" s="9" t="s">
+      <c r="K57" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L55" s="9" t="s">
+      <c r="L57" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="M55" s="9" t="s">
+      <c r="M57" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="N55" s="9" t="s">
+      <c r="N57" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="O55" s="9" t="s">
+      <c r="O57" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="P55" s="9" t="s">
+      <c r="P57" s="9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
-      <c r="A56" s="40" t="s">
+    <row r="58" spans="1:16">
+      <c r="A58" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="14" t="str">
+      <c r="B58" s="4"/>
+      <c r="C58" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="14" t="str">
         <f>F9</f>
         <v>0.42,
 [0.4,0.5]</v>
       </c>
-      <c r="G56" s="14" t="str">
+      <c r="G58" s="14" t="str">
         <f>G9</f>
         <v>guyton2006medical,
 valtin1995renal</v>
       </c>
-      <c r="H56" s="4"/>
-      <c r="I56" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J56" s="4"/>
-      <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-      <c r="M56" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="N56" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O56" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="P56" s="14"/>
-    </row>
-    <row r="57" spans="1:16">
-      <c r="A57" s="40" t="s">
-        <v>224</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F57" s="14" t="str">
-        <f>IF(Patient!C2="Male",D57,E57)</f>
-        <v>[13.8,17.2]</v>
-      </c>
-      <c r="G57" s="14" t="str">
-        <f>G32</f>
-        <v>guyton2006medical</v>
-      </c>
-      <c r="H57" s="4"/>
-      <c r="I57" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="N57" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O57" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="P57" s="14"/>
-    </row>
-    <row r="58" spans="1:16">
-      <c r="A58" s="40" t="s">
-        <v>225</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G58" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="H58" s="5"/>
+      <c r="H58" s="4"/>
       <c r="I58" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J58" s="4"/>
-      <c r="K58" s="41" t="s">
-        <v>229</v>
-      </c>
+      <c r="K58" s="4"/>
       <c r="L58" s="4"/>
       <c r="M58" s="5" t="s">
         <v>222</v>
@@ -15398,7 +15385,7 @@
     </row>
     <row r="59" spans="1:16">
       <c r="A59" s="40" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>110</v>
@@ -15406,13 +15393,19 @@
       <c r="C59" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="14" t="s">
-        <v>231</v>
-      </c>
-      <c r="G59" s="8" t="s">
-        <v>232</v>
+      <c r="D59" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F59" s="14" t="str">
+        <f>IF(Patient!C2="Male",D59,E59)</f>
+        <v>[13.8,17.2]</v>
+      </c>
+      <c r="G59" s="14" t="str">
+        <f>G34</f>
+        <v>guyton2006medical</v>
       </c>
       <c r="H59" s="4"/>
       <c r="I59" s="5" t="s">
@@ -15434,36 +15427,36 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" s="40" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D60" s="5"/>
       <c r="E60" s="5"/>
-      <c r="F60" s="42">
-        <v>8.9999999999999999E-8</v>
+      <c r="F60" s="14" t="s">
+        <v>227</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>235</v>
-      </c>
+        <v>228</v>
+      </c>
+      <c r="H60" s="5"/>
       <c r="I60" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J60" s="4"/>
-      <c r="K60" s="4"/>
+      <c r="K60" s="41" t="s">
+        <v>229</v>
+      </c>
       <c r="L60" s="4"/>
       <c r="M60" s="5" t="s">
         <v>222</v>
       </c>
       <c r="N60" s="5" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="O60" s="14" t="s">
         <v>223</v>
@@ -15472,36 +15465,34 @@
     </row>
     <row r="61" spans="1:16">
       <c r="A61" s="40" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
-      <c r="F61" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="G61" s="43" t="s">
-        <v>238</v>
+      <c r="F61" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>232</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J61" s="4"/>
-      <c r="K61" s="4" t="s">
-        <v>239</v>
-      </c>
+      <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="5" t="s">
         <v>222</v>
       </c>
       <c r="N61" s="5" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="O61" s="14" t="s">
         <v>223</v>
@@ -15510,26 +15501,25 @@
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="B62" s="14" t="str">
-        <f>B15</f>
-        <v>ct/uL</v>
+        <v>233</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>234</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
-      <c r="F62" s="14">
-        <f>F15</f>
-        <v>5172413.793103449</v>
-      </c>
-      <c r="G62" s="14" t="str">
-        <f>G15</f>
-        <v>guyton2006medical</v>
-      </c>
-      <c r="H62" s="4"/>
+      <c r="F62" s="42">
+        <v>8.9999999999999999E-8</v>
+      </c>
+      <c r="G62" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>235</v>
+      </c>
       <c r="I62" s="5" t="s">
         <v>49</v>
       </c>
@@ -15549,112 +15539,101 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="40" t="s">
-        <v>118</v>
-      </c>
-      <c r="B63" s="44" t="str">
-        <f>B21</f>
-        <v>ct/uL</v>
+        <v>236</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
-      <c r="F63" s="44">
-        <f>F21</f>
-        <v>7000</v>
-      </c>
-      <c r="G63" s="44" t="str">
-        <f>G21</f>
-        <v xml:space="preserve">guyton2006medical   </v>
+      <c r="F63" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="G63" s="43" t="s">
+        <v>238</v>
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J63" s="4"/>
-      <c r="K63" s="4"/>
+      <c r="K63" s="4" t="s">
+        <v>239</v>
+      </c>
       <c r="L63" s="4"/>
       <c r="M63" s="5" t="s">
         <v>222</v>
       </c>
       <c r="N63" s="5" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="O63" s="14" t="s">
         <v>223</v>
       </c>
       <c r="P63" s="14"/>
     </row>
-    <row r="64" spans="1:16" ht="24">
-      <c r="A64" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D64" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="H64" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I64" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="J64" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="K64" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="L64" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="M64" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="N64" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="O64" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="P64" s="9" t="s">
-        <v>43</v>
-      </c>
+    <row r="64" spans="1:16">
+      <c r="A64" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B64" s="14" t="str">
+        <f>B17</f>
+        <v>ct/uL</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="14">
+        <f>F17</f>
+        <v>5172413.793103449</v>
+      </c>
+      <c r="G64" s="14" t="str">
+        <f>G17</f>
+        <v>guyton2006medical</v>
+      </c>
+      <c r="H64" s="4"/>
+      <c r="I64" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="N64" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O64" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="P64" s="14"/>
     </row>
     <row r="65" spans="1:16">
       <c r="A65" s="40" t="s">
-        <v>241</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>110</v>
+        <v>118</v>
+      </c>
+      <c r="B65" s="44" t="str">
+        <f>B23</f>
+        <v>ct/uL</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
-      <c r="F65" s="14" t="str">
-        <f>F24</f>
-        <v>[4,5]</v>
-      </c>
-      <c r="G65" s="14" t="str">
-        <f>G24</f>
-        <v>valtin1995renal</v>
+      <c r="F65" s="44">
+        <f>F23</f>
+        <v>7000</v>
+      </c>
+      <c r="G65" s="44" t="str">
+        <f>G23</f>
+        <v xml:space="preserve">guyton2006medical   </v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="5" t="s">
@@ -15664,58 +15643,86 @@
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
       <c r="M65" s="5" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="N65" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O65" s="14" t="s">
-        <v>243</v>
+        <v>223</v>
       </c>
       <c r="P65" s="14"/>
     </row>
-    <row r="66" spans="1:16">
-      <c r="A66" s="40" t="s">
-        <v>244</v>
-      </c>
-      <c r="B66" s="4"/>
-      <c r="C66" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-      <c r="M66" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="N66" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="O66" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="P66" s="14"/>
+    <row r="66" spans="1:16" ht="24">
+      <c r="A66" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I66" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="J66" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K66" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L66" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M66" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="N66" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O66" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P66" s="9" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="67" spans="1:16">
       <c r="A67" s="40" t="s">
-        <v>245</v>
-      </c>
-      <c r="B67" s="4"/>
+        <v>241</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="C67" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="5"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="4"/>
+      <c r="F67" s="14" t="str">
+        <f>F26</f>
+        <v>[4,5]</v>
+      </c>
+      <c r="G67" s="14" t="str">
+        <f>G26</f>
+        <v>valtin1995renal</v>
+      </c>
       <c r="H67" s="4"/>
       <c r="I67" s="5" t="s">
         <v>49</v>
@@ -15736,7 +15743,7 @@
     </row>
     <row r="68" spans="1:16">
       <c r="A68" s="40" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="5" t="s">
@@ -15766,26 +15773,16 @@
     </row>
     <row r="69" spans="1:16">
       <c r="A69" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="B69" s="5" t="s">
-        <v>66</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="B69" s="4"/>
       <c r="C69" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D69" s="5"/>
       <c r="E69" s="5"/>
-      <c r="F69" s="14" t="str">
-        <f>F6</f>
-        <v>[9.0,18.0],
-[6.0,20.0]</v>
-      </c>
-      <c r="G69" s="14" t="str">
-        <f>G6</f>
-        <v>valtin1995renal,
-Deepakfirst</v>
-      </c>
+      <c r="F69" s="14"/>
+      <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="5" t="s">
         <v>49</v>
@@ -15806,24 +15803,16 @@
     </row>
     <row r="70" spans="1:16">
       <c r="A70" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>128</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="B70" s="4"/>
       <c r="C70" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
-      <c r="F70" s="14" t="str">
-        <f>F26</f>
-        <v>[44.08,52.1]</v>
-      </c>
-      <c r="G70" s="14" t="str">
-        <f>G26</f>
-        <v>cheuvront2014comparison</v>
-      </c>
+      <c r="F70" s="14"/>
+      <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="5" t="s">
         <v>49</v>
@@ -15844,16 +15833,26 @@
     </row>
     <row r="71" spans="1:16">
       <c r="A71" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="B71" s="14"/>
+        <v>247</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="C71" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="4"/>
+      <c r="F71" s="14" t="str">
+        <f>F6</f>
+        <v>[9.0,18.0],
+[6.0,20.0]</v>
+      </c>
+      <c r="G71" s="14" t="str">
+        <f>G6</f>
+        <v>valtin1995renal,
+Deepakfirst</v>
+      </c>
       <c r="H71" s="4"/>
       <c r="I71" s="5" t="s">
         <v>49</v>
@@ -15874,22 +15873,23 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" s="40" t="s">
-        <v>250</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>89</v>
+        <v>248</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
-      <c r="F72" s="14" t="s">
-        <v>251</v>
+      <c r="F72" s="14" t="str">
+        <f>F28</f>
+        <v>[44.08,52.1]</v>
       </c>
       <c r="G72" s="14" t="str">
-        <f>G25</f>
-        <v>valtin1995renal</v>
+        <f>G28</f>
+        <v>cheuvront2014comparison</v>
       </c>
       <c r="H72" s="4"/>
       <c r="I72" s="5" t="s">
@@ -15911,24 +15911,16 @@
     </row>
     <row r="73" spans="1:16">
       <c r="A73" s="40" t="s">
-        <v>252</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>128</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="B73" s="14"/>
       <c r="C73" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
-      <c r="F73" s="14" t="str">
-        <f>F28</f>
-        <v>[5.0,15.0]</v>
-      </c>
-      <c r="G73" s="14" t="str">
-        <f>G28</f>
-        <v>valtin1995renal</v>
-      </c>
+      <c r="F73" s="14"/>
+      <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="5" t="s">
         <v>49</v>
@@ -15949,10 +15941,10 @@
     </row>
     <row r="74" spans="1:16">
       <c r="A74" s="40" t="s">
-        <v>253</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>66</v>
+        <v>250</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>46</v>
@@ -15960,10 +15952,11 @@
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
       <c r="F74" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="G74" s="14" t="s">
-        <v>91</v>
+        <v>251</v>
+      </c>
+      <c r="G74" s="14" t="str">
+        <f>G27</f>
+        <v>valtin1995renal</v>
       </c>
       <c r="H74" s="4"/>
       <c r="I74" s="5" t="s">
@@ -15985,16 +15978,24 @@
     </row>
     <row r="75" spans="1:16">
       <c r="A75" s="40" t="s">
-        <v>255</v>
-      </c>
-      <c r="B75" s="4"/>
+        <v>252</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="C75" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D75" s="5"/>
       <c r="E75" s="5"/>
-      <c r="F75" s="14"/>
-      <c r="G75" s="4"/>
+      <c r="F75" s="14" t="str">
+        <f>F30</f>
+        <v>[5.0,15.0]</v>
+      </c>
+      <c r="G75" s="14" t="str">
+        <f>G30</f>
+        <v>valtin1995renal</v>
+      </c>
       <c r="H75" s="4"/>
       <c r="I75" s="5" t="s">
         <v>49</v>
@@ -16015,10 +16016,10 @@
     </row>
     <row r="76" spans="1:16">
       <c r="A76" s="40" t="s">
-        <v>256</v>
-      </c>
-      <c r="B76" s="18" t="s">
-        <v>89</v>
+        <v>253</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>46</v>
@@ -16026,12 +16027,10 @@
       <c r="D76" s="5"/>
       <c r="E76" s="5"/>
       <c r="F76" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="G76" s="14" t="str">
-        <f>G36</f>
-        <v>Leeuwen2015laboratory,
-valtin1995renal</v>
+        <v>254</v>
+      </c>
+      <c r="G76" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="H76" s="4"/>
       <c r="I76" s="5" t="s">
@@ -16053,7 +16052,7 @@
     </row>
     <row r="77" spans="1:16">
       <c r="A77" s="40" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="5" t="s">
@@ -16083,29 +16082,29 @@
     </row>
     <row r="78" spans="1:16">
       <c r="A78" s="40" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D78" s="5"/>
       <c r="E78" s="5"/>
-      <c r="F78" s="14" t="str">
-        <f>F18</f>
-        <v>[6,8]</v>
+      <c r="F78" s="14" t="s">
+        <v>257</v>
       </c>
       <c r="G78" s="14" t="str">
-        <f>G18</f>
-        <v>valtin1995renal</v>
+        <f>G38</f>
+        <v>Leeuwen2015laboratory,
+valtin1995renal</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="J78" s="14"/>
+      <c r="J78" s="4"/>
       <c r="K78" s="4"/>
       <c r="L78" s="4"/>
       <c r="M78" s="5" t="s">
@@ -16120,14 +16119,82 @@
       <c r="P78" s="14"/>
     </row>
     <row r="79" spans="1:16">
-      <c r="O79" s="45"/>
+      <c r="A79" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="B79" s="4"/>
+      <c r="C79" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="N79" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O79" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="P79" s="14"/>
+    </row>
+    <row r="80" spans="1:16">
+      <c r="A80" s="40" t="s">
+        <v>259</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D80" s="5"/>
+      <c r="E80" s="5"/>
+      <c r="F80" s="14" t="str">
+        <f>F20</f>
+        <v>[6,8]</v>
+      </c>
+      <c r="G80" s="14" t="str">
+        <f>G20</f>
+        <v>valtin1995renal</v>
+      </c>
+      <c r="H80" s="4"/>
+      <c r="I80" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J80" s="14"/>
+      <c r="K80" s="4"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="N80" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O80" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="P80" s="14"/>
+    </row>
+    <row r="81" spans="15:15">
+      <c r="O81" s="45"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="L32" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="L39" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="K58" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="L34" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="L41" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="K60" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -16140,7 +16207,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -27162,7 +27229,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fixed female total fluid volume validation.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\dehydration\source\data\human\adult\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\tissue_and_energy_updates\source\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7D16DA-D8BF-4106-9787-AB4DAA447E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264A510D-EA51-4070-8198-E4A6B6FB24A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28770" yWindow="6540" windowWidth="27825" windowHeight="23535" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20640" yWindow="2820" windowWidth="33195" windowHeight="26130" tabRatio="500" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" r:id="rId1"/>
@@ -4038,7 +4038,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4375,6 +4375,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9195,10 +9198,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A67" sqref="A67"/>
-      <selection pane="topRight" activeCell="K8" sqref="K8"/>
+      <selection pane="topRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9560,9 +9563,15 @@
       <c r="C9" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
+      <c r="D9" s="121">
+        <v>1</v>
+      </c>
+      <c r="E9" s="121">
+        <f>37/42</f>
+        <v>0.88095238095238093</v>
+      </c>
       <c r="F9" s="110">
+        <f>IF(Patient!C2="Male",D9,E9)*42</f>
         <v>42</v>
       </c>
       <c r="G9" s="111" t="s">
@@ -13047,7 +13056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMH81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="D10" sqref="D10"/>
     </sheetView>

</xml_diff>

<commit_message>
Fix Tissue IntracellularFluidPH references
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/SystemValidationData.xlsx
+++ b/data/human/adult/validation/SystemValidationData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\Pulse\tissue_and_energy_updates\source\data\human\adult\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Pulse\engine\data\human\adult\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264A510D-EA51-4070-8198-E4A6B6FB24A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA922A5F-A419-44D3-9585-65137315485B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="2820" windowWidth="33195" windowHeight="26130" tabRatio="500" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="750" windowWidth="28770" windowHeight="17250" tabRatio="500" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Respiratory" sheetId="10" r:id="rId10"/>
     <sheet name="Tissue" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3338,9 +3338,6 @@
  7.0</t>
   </si>
   <si>
-    <t>guyton2006medical,         Rodgers2005physiologically</t>
-  </si>
-  <si>
     <t>p384</t>
   </si>
   <si>
@@ -3767,6 +3764,9 @@
   </si>
   <si>
     <t>PlasmaOsmolarity*</t>
+  </si>
+  <si>
+    <t>guyton2006medical, rodgers2005physiologically</t>
   </si>
 </sst>
 </file>
@@ -9201,7 +9201,7 @@
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A67" sqref="A67"/>
-      <selection pane="topRight" activeCell="E5" sqref="E5"/>
+      <selection pane="topRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9406,17 +9406,17 @@
         <v>1054</v>
       </c>
       <c r="G5" s="8" t="s">
+        <v>1196</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>1055</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>1056</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>49</v>
       </c>
       <c r="J5" s="109"/>
       <c r="K5" s="8" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>1054</v>
@@ -9436,7 +9436,7 @@
     </row>
     <row r="6" spans="1:16" s="1" customFormat="1">
       <c r="A6" s="10" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>17</v>
@@ -9458,7 +9458,7 @@
         <v>49</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="K6" s="8"/>
       <c r="L6" s="8">
@@ -9477,7 +9477,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="67" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>14</v>
@@ -9515,7 +9515,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="67" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="8" t="s">
@@ -9527,10 +9527,10 @@
         <v>0.85</v>
       </c>
       <c r="G8" s="111" t="s">
+        <v>1061</v>
+      </c>
+      <c r="H8" s="111" t="s">
         <v>1062</v>
-      </c>
-      <c r="H8" s="111" t="s">
-        <v>1063</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>49</v>
@@ -9555,7 +9555,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="120" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>937</v>
@@ -9599,7 +9599,7 @@
     </row>
     <row r="10" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1">
       <c r="A10" s="28" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>1</v>
@@ -9649,7 +9649,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="67" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>14</v>
@@ -9666,7 +9666,7 @@
         <v>104</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="I11" s="14" t="s">
         <v>49</v>
@@ -9691,7 +9691,7 @@
     </row>
     <row r="12" spans="1:16" s="1" customFormat="1">
       <c r="A12" s="67" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>14</v>
@@ -9708,7 +9708,7 @@
         <v>104</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>49</v>
@@ -9733,7 +9733,7 @@
     </row>
     <row r="13" spans="1:16" s="1" customFormat="1" ht="26.25" customHeight="1">
       <c r="A13" s="28" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>1</v>
@@ -9783,7 +9783,7 @@
     </row>
     <row r="14" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A14" s="30" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>937</v>
@@ -9805,32 +9805,32 @@
         <v>273</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I14" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J14" s="17"/>
       <c r="K14" s="33" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="L14" s="5">
         <v>3140</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N14" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P14" s="14"/>
     </row>
     <row r="15" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A15" s="30" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>17</v>
@@ -9848,20 +9848,20 @@
         <v>1047</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I15" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J15" s="17"/>
       <c r="K15" s="33" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="L15" s="5">
         <v>3140</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N15" s="5" t="s">
         <v>71</v>
@@ -9873,7 +9873,7 @@
     </row>
     <row r="16" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A16" s="30" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>17</v>
@@ -9891,20 +9891,20 @@
         <v>1047</v>
       </c>
       <c r="H16" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I16" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J16" s="17"/>
       <c r="K16" s="33" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="L16" s="5">
         <v>3140</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N16" s="5" t="s">
         <v>71</v>
@@ -9916,7 +9916,7 @@
     </row>
     <row r="17" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A17" s="30" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>937</v>
@@ -9938,32 +9938,32 @@
         <v>273</v>
       </c>
       <c r="H17" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I17" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J17" s="17"/>
       <c r="K17" s="33" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="L17" s="5">
         <v>2680</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N17" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P17" s="14"/>
     </row>
     <row r="18" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A18" s="30" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>17</v>
@@ -9981,20 +9981,20 @@
         <v>1047</v>
       </c>
       <c r="H18" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I18" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J18" s="17"/>
       <c r="K18" s="33" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="L18" s="5">
         <v>2680</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N18" s="5" t="s">
         <v>71</v>
@@ -10006,7 +10006,7 @@
     </row>
     <row r="19" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A19" s="30" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>17</v>
@@ -10024,20 +10024,20 @@
         <v>1047</v>
       </c>
       <c r="H19" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I19" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J19" s="17"/>
       <c r="K19" s="33" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="L19" s="5">
         <v>2680</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N19" s="5" t="s">
         <v>71</v>
@@ -10049,7 +10049,7 @@
     </row>
     <row r="20" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A20" s="30" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>937</v>
@@ -10071,32 +10071,32 @@
         <v>273</v>
       </c>
       <c r="H20" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I20" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J20" s="17"/>
       <c r="K20" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L20" s="5">
         <v>1020</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N20" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P20" s="14"/>
     </row>
     <row r="21" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A21" s="30" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>17</v>
@@ -10114,20 +10114,20 @@
         <v>1047</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I21" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J21" s="17"/>
       <c r="K21" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L21" s="5">
         <v>1020</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N21" s="5" t="s">
         <v>71</v>
@@ -10139,7 +10139,7 @@
     </row>
     <row r="22" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A22" s="30" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>17</v>
@@ -10157,20 +10157,20 @@
         <v>1047</v>
       </c>
       <c r="H22" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I22" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J22" s="17"/>
       <c r="K22" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L22" s="5">
         <v>1020</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N22" s="5" t="s">
         <v>71</v>
@@ -10182,7 +10182,7 @@
     </row>
     <row r="23" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A23" s="30" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>937</v>
@@ -10204,32 +10204,32 @@
         <v>273</v>
       </c>
       <c r="H23" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I23" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J23" s="17"/>
       <c r="K23" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L23" s="5">
         <v>730</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N23" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P23" s="14"/>
     </row>
     <row r="24" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A24" s="30" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>17</v>
@@ -10247,20 +10247,20 @@
         <v>1047</v>
       </c>
       <c r="H24" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I24" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J24" s="17"/>
       <c r="K24" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L24" s="5">
         <v>730</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N24" s="5" t="s">
         <v>71</v>
@@ -10272,7 +10272,7 @@
     </row>
     <row r="25" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A25" s="30" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>17</v>
@@ -10290,20 +10290,20 @@
         <v>1047</v>
       </c>
       <c r="H25" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I25" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J25" s="17"/>
       <c r="K25" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L25" s="5">
         <v>730</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N25" s="5" t="s">
         <v>71</v>
@@ -10315,7 +10315,7 @@
     </row>
     <row r="26" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A26" s="30" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>937</v>
@@ -10337,32 +10337,32 @@
         <v>273</v>
       </c>
       <c r="H26" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I26" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J26" s="17"/>
       <c r="K26" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L26" s="5">
         <v>110</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N26" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O26" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P26" s="14"/>
     </row>
     <row r="27" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A27" s="30" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>17</v>
@@ -10380,20 +10380,20 @@
         <v>1047</v>
       </c>
       <c r="H27" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I27" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J27" s="17"/>
       <c r="K27" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L27" s="5">
         <v>110</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N27" s="5" t="s">
         <v>71</v>
@@ -10405,7 +10405,7 @@
     </row>
     <row r="28" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A28" s="30" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>17</v>
@@ -10423,20 +10423,20 @@
         <v>1047</v>
       </c>
       <c r="H28" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I28" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J28" s="17"/>
       <c r="K28" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L28" s="5">
         <v>110</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N28" s="5" t="s">
         <v>71</v>
@@ -10448,7 +10448,7 @@
     </row>
     <row r="29" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A29" s="30" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>937</v>
@@ -10470,32 +10470,32 @@
         <v>273</v>
       </c>
       <c r="H29" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I29" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J29" s="17"/>
       <c r="K29" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L29" s="5">
         <v>110</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N29" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O29" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P29" s="14"/>
     </row>
     <row r="30" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A30" s="30" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>17</v>
@@ -10513,20 +10513,20 @@
         <v>1047</v>
       </c>
       <c r="H30" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I30" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J30" s="17"/>
       <c r="K30" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L30" s="5">
         <v>110</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N30" s="5" t="s">
         <v>71</v>
@@ -10538,7 +10538,7 @@
     </row>
     <row r="31" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A31" s="30" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>17</v>
@@ -10556,20 +10556,20 @@
         <v>1047</v>
       </c>
       <c r="H31" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I31" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J31" s="17"/>
       <c r="K31" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L31" s="5">
         <v>110</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N31" s="5" t="s">
         <v>71</v>
@@ -10581,7 +10581,7 @@
     </row>
     <row r="32" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A32" s="30" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>937</v>
@@ -10603,32 +10603,32 @@
         <v>273</v>
       </c>
       <c r="H32" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I32" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J32" s="17"/>
       <c r="K32" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L32" s="5">
         <v>1030</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N32" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O32" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P32" s="14"/>
     </row>
     <row r="33" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A33" s="30" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>17</v>
@@ -10646,20 +10646,20 @@
         <v>1047</v>
       </c>
       <c r="H33" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I33" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J33" s="17"/>
       <c r="K33" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L33" s="5">
         <v>1030</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N33" s="5" t="s">
         <v>71</v>
@@ -10671,7 +10671,7 @@
     </row>
     <row r="34" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A34" s="30" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>17</v>
@@ -10689,20 +10689,20 @@
         <v>1047</v>
       </c>
       <c r="H34" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I34" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J34" s="17"/>
       <c r="K34" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L34" s="5">
         <v>1030</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N34" s="5" t="s">
         <v>71</v>
@@ -10714,7 +10714,7 @@
     </row>
     <row r="35" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A35" s="30" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>937</v>
@@ -10738,32 +10738,32 @@
         <v>273</v>
       </c>
       <c r="H35" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I35" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J35" s="17"/>
       <c r="K35" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L35" s="5">
         <v>160</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N35" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O35" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P35" s="14"/>
     </row>
     <row r="36" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A36" s="30" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>17</v>
@@ -10781,20 +10781,20 @@
         <v>1047</v>
       </c>
       <c r="H36" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I36" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J36" s="17"/>
       <c r="K36" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L36" s="5">
         <v>160</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N36" s="5" t="s">
         <v>71</v>
@@ -10806,7 +10806,7 @@
     </row>
     <row r="37" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A37" s="30" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>17</v>
@@ -10824,20 +10824,20 @@
         <v>1047</v>
       </c>
       <c r="H37" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I37" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J37" s="17"/>
       <c r="K37" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L37" s="5">
         <v>160</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N37" s="5" t="s">
         <v>71</v>
@@ -10849,7 +10849,7 @@
     </row>
     <row r="38" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A38" s="30" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>937</v>
@@ -10873,32 +10873,32 @@
         <v>273</v>
       </c>
       <c r="H38" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I38" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J38" s="17"/>
       <c r="K38" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L38" s="5">
         <v>160</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N38" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O38" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P38" s="14"/>
     </row>
     <row r="39" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A39" s="30" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>17</v>
@@ -10916,20 +10916,20 @@
         <v>1047</v>
       </c>
       <c r="H39" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I39" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J39" s="17"/>
       <c r="K39" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L39" s="5">
         <v>160</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N39" s="5" t="s">
         <v>71</v>
@@ -10941,7 +10941,7 @@
     </row>
     <row r="40" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A40" s="30" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>17</v>
@@ -10959,20 +10959,20 @@
         <v>1047</v>
       </c>
       <c r="H40" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I40" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J40" s="17"/>
       <c r="K40" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L40" s="5">
         <v>160</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N40" s="5" t="s">
         <v>71</v>
@@ -10984,7 +10984,7 @@
     </row>
     <row r="41" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A41" s="30" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>937</v>
@@ -11006,32 +11006,32 @@
         <v>273</v>
       </c>
       <c r="H41" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I41" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J41" s="17"/>
       <c r="K41" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L41" s="5">
         <v>13090</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N41" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O41" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P41" s="14"/>
     </row>
     <row r="42" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A42" s="30" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>17</v>
@@ -11049,20 +11049,20 @@
         <v>1047</v>
       </c>
       <c r="H42" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I42" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J42" s="17"/>
       <c r="K42" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L42" s="5">
         <v>13090</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N42" s="5" t="s">
         <v>71</v>
@@ -11074,7 +11074,7 @@
     </row>
     <row r="43" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A43" s="30" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>17</v>
@@ -11092,20 +11092,20 @@
         <v>1047</v>
       </c>
       <c r="H43" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I43" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J43" s="17"/>
       <c r="K43" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L43" s="5">
         <v>13090</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N43" s="5" t="s">
         <v>71</v>
@@ -11117,7 +11117,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" s="30" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B44" s="18" t="s">
         <v>89</v>
@@ -11128,10 +11128,10 @@
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="52" t="s">
+        <v>1105</v>
+      </c>
+      <c r="G44" s="17" t="s">
         <v>1106</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>1107</v>
       </c>
       <c r="H44" s="17"/>
       <c r="I44" s="26" t="s">
@@ -11141,7 +11141,7 @@
       <c r="K44" s="33"/>
       <c r="L44" s="21"/>
       <c r="M44" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N44" s="5" t="s">
         <v>71</v>
@@ -11153,7 +11153,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" s="30" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B45" s="18" t="s">
         <v>89</v>
@@ -11164,7 +11164,7 @@
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="113" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="G45" s="17" t="s">
         <v>548</v>
@@ -11175,11 +11175,11 @@
       </c>
       <c r="J45" s="5"/>
       <c r="K45" s="33" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="L45" s="4"/>
       <c r="M45" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N45" s="5" t="s">
         <v>71</v>
@@ -11191,7 +11191,7 @@
     </row>
     <row r="46" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A46" s="30" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>937</v>
@@ -11213,32 +11213,32 @@
         <v>273</v>
       </c>
       <c r="H46" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I46" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J46" s="17"/>
       <c r="K46" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L46" s="5">
         <v>190</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O46" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P46" s="14"/>
     </row>
     <row r="47" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A47" s="30" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>17</v>
@@ -11256,20 +11256,20 @@
         <v>1047</v>
       </c>
       <c r="H47" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I47" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J47" s="17"/>
       <c r="K47" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L47" s="5">
         <v>190</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N47" s="5" t="s">
         <v>71</v>
@@ -11281,7 +11281,7 @@
     </row>
     <row r="48" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A48" s="30" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>17</v>
@@ -11299,20 +11299,20 @@
         <v>1047</v>
       </c>
       <c r="H48" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I48" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J48" s="17"/>
       <c r="K48" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L48" s="5">
         <v>190</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N48" s="5" t="s">
         <v>71</v>
@@ -11324,7 +11324,7 @@
     </row>
     <row r="49" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A49" s="30" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>937</v>
@@ -11346,32 +11346,32 @@
         <v>273</v>
       </c>
       <c r="H49" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I49" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J49" s="17"/>
       <c r="K49" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L49" s="5">
         <v>1550</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N49" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O49" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P49" s="14"/>
     </row>
     <row r="50" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A50" s="30" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>17</v>
@@ -11389,20 +11389,20 @@
         <v>1047</v>
       </c>
       <c r="H50" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I50" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J50" s="17"/>
       <c r="K50" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L50" s="5">
         <v>1550</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N50" s="5" t="s">
         <v>71</v>
@@ -11414,7 +11414,7 @@
     </row>
     <row r="51" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A51" s="30" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>17</v>
@@ -11432,20 +11432,20 @@
         <v>1047</v>
       </c>
       <c r="H51" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I51" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J51" s="17"/>
       <c r="K51" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L51" s="5">
         <v>1550</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N51" s="5" t="s">
         <v>71</v>
@@ -11457,7 +11457,7 @@
     </row>
     <row r="52" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A52" s="30" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>937</v>
@@ -11479,32 +11479,32 @@
         <v>273</v>
       </c>
       <c r="H52" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I52" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J52" s="17"/>
       <c r="K52" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L52" s="5">
         <v>100</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N52" s="5" t="s">
         <v>51</v>
       </c>
       <c r="O52" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P52" s="14"/>
     </row>
     <row r="53" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A53" s="30" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>17</v>
@@ -11522,20 +11522,20 @@
         <v>1047</v>
       </c>
       <c r="H53" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I53" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J53" s="17"/>
       <c r="K53" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L53" s="5">
         <v>100</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N53" s="5" t="s">
         <v>71</v>
@@ -11547,7 +11547,7 @@
     </row>
     <row r="54" spans="1:16" s="1" customFormat="1" ht="12">
       <c r="A54" s="30" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>17</v>
@@ -11565,20 +11565,20 @@
         <v>1047</v>
       </c>
       <c r="H54" s="26" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I54" s="26" t="s">
         <v>49</v>
       </c>
       <c r="J54" s="17"/>
       <c r="K54" s="33" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="L54" s="5">
         <v>100</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="N54" s="5" t="s">
         <v>71</v>
@@ -11590,7 +11590,7 @@
     </row>
     <row r="55" spans="1:16" ht="24">
       <c r="A55" s="28" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>1</v>
@@ -11640,7 +11640,7 @@
     </row>
     <row r="56" spans="1:16" ht="24.75">
       <c r="A56" s="30" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>89</v>
@@ -11651,7 +11651,7 @@
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="18" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="G56" s="18" t="s">
         <v>143</v>
@@ -11662,23 +11662,23 @@
       </c>
       <c r="J56" s="18"/>
       <c r="K56" s="114" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="L56" s="14"/>
       <c r="M56" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N56" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O56" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P56" s="14"/>
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="30" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="B57" s="18" t="s">
         <v>89</v>
@@ -11702,19 +11702,19 @@
         <v>1049</v>
       </c>
       <c r="M57" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N57" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O57" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P57" s="14"/>
     </row>
     <row r="58" spans="1:16">
       <c r="A58" s="30" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="B58" s="18" t="s">
         <v>89</v>
@@ -11728,10 +11728,10 @@
         <v>25</v>
       </c>
       <c r="G58" s="18" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H58" s="17" t="s">
         <v>1127</v>
-      </c>
-      <c r="H58" s="17" t="s">
-        <v>1128</v>
       </c>
       <c r="I58" s="18" t="s">
         <v>49</v>
@@ -11742,19 +11742,19 @@
         <v>1051</v>
       </c>
       <c r="M58" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N58" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O58" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P58" s="14"/>
     </row>
     <row r="59" spans="1:16">
       <c r="A59" s="30" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>89</v>
@@ -11768,10 +11768,10 @@
         <v>1.2</v>
       </c>
       <c r="G59" s="18" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H59" s="17" t="s">
         <v>1127</v>
-      </c>
-      <c r="H59" s="17" t="s">
-        <v>1128</v>
       </c>
       <c r="I59" s="18" t="s">
         <v>49</v>
@@ -11779,22 +11779,22 @@
       <c r="J59" s="17"/>
       <c r="K59" s="19"/>
       <c r="L59" s="8" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="M59" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N59" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O59" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P59" s="14"/>
     </row>
     <row r="60" spans="1:16" ht="24">
       <c r="A60" s="30" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="B60" s="115" t="s">
         <v>89</v>
@@ -11805,7 +11805,7 @@
       <c r="D60" s="115"/>
       <c r="E60" s="115"/>
       <c r="F60" s="116" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="G60" s="115"/>
       <c r="H60" s="116"/>
@@ -11814,23 +11814,23 @@
       </c>
       <c r="J60" s="116"/>
       <c r="K60" s="116" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="L60" s="8"/>
       <c r="M60" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N60" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O60" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P60" s="14"/>
     </row>
     <row r="61" spans="1:16">
       <c r="A61" s="30" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B61" s="18" t="s">
         <v>89</v>
@@ -11844,10 +11844,10 @@
         <v>116</v>
       </c>
       <c r="G61" s="18" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H61" s="17" t="s">
         <v>1127</v>
-      </c>
-      <c r="H61" s="17" t="s">
-        <v>1128</v>
       </c>
       <c r="I61" s="18" t="s">
         <v>49</v>
@@ -11856,19 +11856,19 @@
       <c r="K61" s="33"/>
       <c r="L61" s="14"/>
       <c r="M61" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N61" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O61" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P61" s="14"/>
     </row>
     <row r="62" spans="1:16" ht="36.75">
       <c r="A62" s="30" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B62" s="115"/>
       <c r="C62" s="116"/>
@@ -11882,26 +11882,26 @@
       </c>
       <c r="J62" s="116"/>
       <c r="K62" s="117" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="L62" s="14"/>
       <c r="M62" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N62" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O62" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P62" s="14"/>
     </row>
     <row r="63" spans="1:16" ht="72.75">
       <c r="A63" s="30" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B63" s="17" t="s">
         <v>1136</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>1137</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>46</v>
@@ -11909,36 +11909,36 @@
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
       <c r="F63" s="8" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G63" s="17" t="s">
         <v>1138</v>
       </c>
-      <c r="G63" s="17" t="s">
+      <c r="H63" s="17" t="s">
         <v>1139</v>
-      </c>
-      <c r="H63" s="17" t="s">
-        <v>1140</v>
       </c>
       <c r="I63" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J63" s="17"/>
       <c r="K63" s="114" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="L63" s="4"/>
       <c r="M63" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N63" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O63" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P63" s="14"/>
     </row>
     <row r="64" spans="1:16">
       <c r="A64" s="30" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B64" s="18" t="s">
         <v>89</v>
@@ -11952,10 +11952,10 @@
         <v>5.9</v>
       </c>
       <c r="G64" s="17" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H64" s="17" t="s">
         <v>1127</v>
-      </c>
-      <c r="H64" s="17" t="s">
-        <v>1128</v>
       </c>
       <c r="I64" s="18" t="s">
         <v>49</v>
@@ -11964,19 +11964,19 @@
       <c r="K64" s="33"/>
       <c r="L64" s="21"/>
       <c r="M64" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N64" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O64" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P64" s="14"/>
     </row>
     <row r="65" spans="1:16">
       <c r="A65" s="30" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="B65" s="18" t="s">
         <v>89</v>
@@ -11996,26 +11996,26 @@
       </c>
       <c r="J65" s="26"/>
       <c r="K65" s="33" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="L65" s="4"/>
       <c r="M65" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N65" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O65" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P65" s="14"/>
     </row>
     <row r="66" spans="1:16" ht="24.75">
       <c r="A66" s="30" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>46</v>
@@ -12023,36 +12023,36 @@
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
       <c r="F66" s="26" t="s">
+        <v>1145</v>
+      </c>
+      <c r="G66" s="17" t="s">
         <v>1146</v>
       </c>
-      <c r="G66" s="17" t="s">
+      <c r="H66" s="26" t="s">
         <v>1147</v>
-      </c>
-      <c r="H66" s="26" t="s">
-        <v>1148</v>
       </c>
       <c r="I66" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J66" s="5"/>
       <c r="K66" s="114" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="L66" s="4"/>
       <c r="M66" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N66" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O66" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P66" s="14"/>
     </row>
     <row r="67" spans="1:16" ht="48.75">
       <c r="A67" s="30" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="B67" s="18" t="s">
         <v>89</v>
@@ -12063,36 +12063,36 @@
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
       <c r="F67" s="26" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G67" s="17" t="s">
         <v>1150</v>
       </c>
-      <c r="G67" s="17" t="s">
+      <c r="H67" s="26" t="s">
         <v>1151</v>
-      </c>
-      <c r="H67" s="26" t="s">
-        <v>1152</v>
       </c>
       <c r="I67" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J67" s="5"/>
       <c r="K67" s="33" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="L67" s="4"/>
       <c r="M67" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N67" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O67" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P67" s="14"/>
     </row>
     <row r="68" spans="1:16" ht="24">
       <c r="A68" s="30" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="B68" s="115"/>
       <c r="C68" s="116"/>
@@ -12106,26 +12106,26 @@
       </c>
       <c r="J68" s="116"/>
       <c r="K68" s="115" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="L68" s="4"/>
       <c r="M68" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N68" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O68" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P68" s="14"/>
     </row>
     <row r="69" spans="1:16">
       <c r="A69" s="30" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>46</v>
@@ -12133,13 +12133,13 @@
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="26" t="s">
+        <v>1156</v>
+      </c>
+      <c r="G69" s="17" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H69" s="26" t="s">
         <v>1157</v>
-      </c>
-      <c r="G69" s="17" t="s">
-        <v>1151</v>
-      </c>
-      <c r="H69" s="26" t="s">
-        <v>1158</v>
       </c>
       <c r="I69" s="18" t="s">
         <v>49</v>
@@ -12148,19 +12148,19 @@
       <c r="K69" s="26"/>
       <c r="L69" s="4"/>
       <c r="M69" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N69" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O69" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P69" s="14"/>
     </row>
     <row r="70" spans="1:16" ht="24">
       <c r="A70" s="30" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="B70" s="18" t="s">
         <v>89</v>
@@ -12171,7 +12171,7 @@
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="8" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="G70" s="17"/>
       <c r="H70" s="8"/>
@@ -12180,23 +12180,23 @@
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="116" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="L70" s="4"/>
       <c r="M70" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N70" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O70" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P70" s="14"/>
     </row>
     <row r="71" spans="1:16">
       <c r="A71" s="10" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="B71" s="18" t="s">
         <v>89</v>
@@ -12210,10 +12210,10 @@
         <v>4.5</v>
       </c>
       <c r="G71" s="18" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H71" s="18" t="s">
         <v>1127</v>
-      </c>
-      <c r="H71" s="18" t="s">
-        <v>1128</v>
       </c>
       <c r="I71" s="18" t="s">
         <v>49</v>
@@ -12222,19 +12222,19 @@
       <c r="K71" s="33"/>
       <c r="L71" s="4"/>
       <c r="M71" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N71" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O71" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P71" s="14"/>
     </row>
     <row r="72" spans="1:16">
       <c r="A72" s="30" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B72" s="18" t="s">
         <v>89</v>
@@ -12248,10 +12248,10 @@
         <v>145</v>
       </c>
       <c r="G72" s="17" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H72" s="26" t="s">
         <v>1127</v>
-      </c>
-      <c r="H72" s="26" t="s">
-        <v>1128</v>
       </c>
       <c r="I72" s="18" t="s">
         <v>49</v>
@@ -12260,19 +12260,19 @@
       <c r="K72" s="33"/>
       <c r="L72" s="4"/>
       <c r="M72" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N72" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O72" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P72" s="14"/>
     </row>
     <row r="73" spans="1:16">
       <c r="A73" s="30" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="B73" s="36" t="s">
         <v>89</v>
@@ -12290,23 +12290,23 @@
       </c>
       <c r="J73" s="118"/>
       <c r="K73" s="114" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="L73" s="4"/>
       <c r="M73" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N73" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O73" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P73" s="14"/>
     </row>
     <row r="74" spans="1:16" ht="36">
       <c r="A74" s="30" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="B74" s="26" t="s">
         <v>66</v>
@@ -12328,23 +12328,23 @@
       </c>
       <c r="J74" s="119"/>
       <c r="K74" s="47" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="L74" s="4"/>
       <c r="M74" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N74" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O74" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P74" s="14"/>
     </row>
     <row r="75" spans="1:16" ht="24.75">
       <c r="A75" s="30" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="B75" s="18" t="s">
         <v>89</v>
@@ -12355,7 +12355,7 @@
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
       <c r="F75" s="18" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="G75" s="18"/>
       <c r="H75" s="18"/>
@@ -12364,23 +12364,23 @@
       </c>
       <c r="J75" s="18"/>
       <c r="K75" s="114" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="L75" s="4"/>
       <c r="M75" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N75" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O75" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P75" s="14"/>
     </row>
     <row r="76" spans="1:16">
       <c r="A76" s="30" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B76" s="18" t="s">
         <v>89</v>
@@ -12400,23 +12400,23 @@
       </c>
       <c r="J76" s="8"/>
       <c r="K76" s="35" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="L76" s="4"/>
       <c r="M76" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N76" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O76" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P76" s="14"/>
     </row>
     <row r="77" spans="1:16">
       <c r="A77" s="30" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="B77" s="18" t="s">
         <v>89</v>
@@ -12430,10 +12430,10 @@
         <v>16</v>
       </c>
       <c r="G77" s="18" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H77" s="17" t="s">
         <v>1127</v>
-      </c>
-      <c r="H77" s="17" t="s">
-        <v>1128</v>
       </c>
       <c r="I77" s="18" t="s">
         <v>49</v>
@@ -12442,19 +12442,19 @@
       <c r="K77" s="19"/>
       <c r="L77" s="4"/>
       <c r="M77" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N77" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O77" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P77" s="14"/>
     </row>
     <row r="78" spans="1:16">
       <c r="A78" s="30" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="B78" s="18" t="s">
         <v>89</v>
@@ -12468,10 +12468,10 @@
         <v>1E-4</v>
       </c>
       <c r="G78" s="18" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H78" s="17" t="s">
         <v>1127</v>
-      </c>
-      <c r="H78" s="17" t="s">
-        <v>1128</v>
       </c>
       <c r="I78" s="18" t="s">
         <v>49</v>
@@ -12480,19 +12480,19 @@
       <c r="K78" s="19"/>
       <c r="L78" s="4"/>
       <c r="M78" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N78" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O78" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P78" s="14"/>
     </row>
     <row r="79" spans="1:16" ht="24">
       <c r="A79" s="30" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="B79" s="115" t="s">
         <v>89</v>
@@ -12503,7 +12503,7 @@
       <c r="D79" s="115"/>
       <c r="E79" s="115"/>
       <c r="F79" s="116" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="G79" s="115"/>
       <c r="H79" s="116"/>
@@ -12512,23 +12512,23 @@
       </c>
       <c r="J79" s="116"/>
       <c r="K79" s="116" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="L79" s="4"/>
       <c r="M79" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N79" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O79" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P79" s="14"/>
     </row>
     <row r="80" spans="1:16">
       <c r="A80" s="30" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="B80" s="18" t="s">
         <v>89</v>
@@ -12542,10 +12542,10 @@
         <v>20</v>
       </c>
       <c r="G80" s="18" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H80" s="17" t="s">
         <v>1127</v>
-      </c>
-      <c r="H80" s="17" t="s">
-        <v>1128</v>
       </c>
       <c r="I80" s="18" t="s">
         <v>49</v>
@@ -12554,19 +12554,19 @@
       <c r="K80" s="33"/>
       <c r="L80" s="4"/>
       <c r="M80" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N80" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O80" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P80" s="14"/>
     </row>
     <row r="81" spans="1:16" ht="36.75">
       <c r="A81" s="30" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B81" s="18" t="s">
         <v>89</v>
@@ -12584,26 +12584,26 @@
       </c>
       <c r="J81" s="17"/>
       <c r="K81" s="114" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="L81" s="4"/>
       <c r="M81" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N81" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O81" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P81" s="14"/>
     </row>
     <row r="82" spans="1:16" ht="72.75">
       <c r="A82" s="30" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>46</v>
@@ -12611,36 +12611,36 @@
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
       <c r="F82" s="8" t="s">
+        <v>1137</v>
+      </c>
+      <c r="G82" s="17" t="s">
         <v>1138</v>
       </c>
-      <c r="G82" s="17" t="s">
+      <c r="H82" s="17" t="s">
         <v>1139</v>
-      </c>
-      <c r="H82" s="17" t="s">
-        <v>1140</v>
       </c>
       <c r="I82" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J82" s="17"/>
       <c r="K82" s="114" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="L82" s="4"/>
       <c r="M82" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N82" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O82" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P82" s="14"/>
     </row>
     <row r="83" spans="1:16">
       <c r="A83" s="30" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="B83" s="18" t="s">
         <v>89</v>
@@ -12654,10 +12654,10 @@
         <v>0</v>
       </c>
       <c r="G83" s="17" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H83" s="17" t="s">
         <v>1127</v>
-      </c>
-      <c r="H83" s="17" t="s">
-        <v>1128</v>
       </c>
       <c r="I83" s="18" t="s">
         <v>49</v>
@@ -12666,19 +12666,19 @@
       <c r="K83" s="33"/>
       <c r="L83" s="21"/>
       <c r="M83" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N83" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O83" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P83" s="14"/>
     </row>
     <row r="84" spans="1:16">
       <c r="A84" s="30" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="B84" s="18" t="s">
         <v>89</v>
@@ -12698,26 +12698,26 @@
       </c>
       <c r="J84" s="26"/>
       <c r="K84" s="33" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="L84" s="4"/>
       <c r="M84" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N84" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O84" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P84" s="14"/>
     </row>
     <row r="85" spans="1:16" ht="24.75">
       <c r="A85" s="30" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>46</v>
@@ -12725,36 +12725,36 @@
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
       <c r="F85" s="26" t="s">
+        <v>1145</v>
+      </c>
+      <c r="G85" s="17" t="s">
         <v>1146</v>
       </c>
-      <c r="G85" s="17" t="s">
+      <c r="H85" s="26" t="s">
         <v>1147</v>
-      </c>
-      <c r="H85" s="26" t="s">
-        <v>1148</v>
       </c>
       <c r="I85" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J85" s="5"/>
       <c r="K85" s="114" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="L85" s="4"/>
       <c r="M85" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N85" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O85" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P85" s="14"/>
     </row>
     <row r="86" spans="1:16" ht="48.75">
       <c r="A86" s="30" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="B86" s="18" t="s">
         <v>89</v>
@@ -12765,36 +12765,36 @@
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
       <c r="F86" s="26" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G86" s="17" t="s">
         <v>1150</v>
       </c>
-      <c r="G86" s="17" t="s">
+      <c r="H86" s="26" t="s">
         <v>1151</v>
-      </c>
-      <c r="H86" s="26" t="s">
-        <v>1152</v>
       </c>
       <c r="I86" s="18" t="s">
         <v>49</v>
       </c>
       <c r="J86" s="5"/>
       <c r="K86" s="33" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="L86" s="4"/>
       <c r="M86" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N86" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O86" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P86" s="14"/>
     </row>
     <row r="87" spans="1:16">
       <c r="A87" s="30" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="B87" s="18" t="s">
         <v>89</v>
@@ -12814,22 +12814,22 @@
       <c r="K87" s="26"/>
       <c r="L87" s="4"/>
       <c r="M87" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N87" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O87" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P87" s="14"/>
     </row>
     <row r="88" spans="1:16">
       <c r="A88" s="30" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>46</v>
@@ -12837,13 +12837,13 @@
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
       <c r="F88" s="26" t="s">
+        <v>1156</v>
+      </c>
+      <c r="G88" s="17" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H88" s="26" t="s">
         <v>1157</v>
-      </c>
-      <c r="G88" s="17" t="s">
-        <v>1151</v>
-      </c>
-      <c r="H88" s="26" t="s">
-        <v>1158</v>
       </c>
       <c r="I88" s="18" t="s">
         <v>49</v>
@@ -12852,19 +12852,19 @@
       <c r="K88" s="26"/>
       <c r="L88" s="4"/>
       <c r="M88" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N88" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O88" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P88" s="14"/>
     </row>
     <row r="89" spans="1:16" ht="24">
       <c r="A89" s="30" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="B89" s="18" t="s">
         <v>89</v>
@@ -12875,7 +12875,7 @@
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
       <c r="F89" s="8" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="G89" s="17"/>
       <c r="H89" s="8"/>
@@ -12884,23 +12884,23 @@
       </c>
       <c r="J89" s="8"/>
       <c r="K89" s="116" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="L89" s="4"/>
       <c r="M89" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N89" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O89" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P89" s="14"/>
     </row>
     <row r="90" spans="1:16">
       <c r="A90" s="10" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="B90" s="18" t="s">
         <v>89</v>
@@ -12914,10 +12914,10 @@
         <v>120</v>
       </c>
       <c r="G90" s="18" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H90" s="18" t="s">
         <v>1127</v>
-      </c>
-      <c r="H90" s="18" t="s">
-        <v>1128</v>
       </c>
       <c r="I90" s="18" t="s">
         <v>49</v>
@@ -12926,19 +12926,19 @@
       <c r="K90" s="33"/>
       <c r="L90" s="4"/>
       <c r="M90" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N90" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O90" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P90" s="14"/>
     </row>
     <row r="91" spans="1:16">
       <c r="A91" s="30" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="B91" s="18" t="s">
         <v>89</v>
@@ -12952,10 +12952,10 @@
         <v>15</v>
       </c>
       <c r="G91" s="17" t="s">
+        <v>1126</v>
+      </c>
+      <c r="H91" s="26" t="s">
         <v>1127</v>
-      </c>
-      <c r="H91" s="26" t="s">
-        <v>1128</v>
       </c>
       <c r="I91" s="18" t="s">
         <v>49</v>
@@ -12964,19 +12964,19 @@
       <c r="K91" s="33"/>
       <c r="L91" s="4"/>
       <c r="M91" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N91" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O91" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P91" s="14"/>
     </row>
     <row r="92" spans="1:16">
       <c r="A92" s="30" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="B92" s="36" t="s">
         <v>89</v>
@@ -12994,23 +12994,23 @@
       </c>
       <c r="J92" s="114"/>
       <c r="K92" s="114" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="L92" s="4"/>
       <c r="M92" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N92" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O92" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P92" s="14"/>
     </row>
     <row r="93" spans="1:16" ht="36">
       <c r="A93" s="30" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="B93" s="26" t="s">
         <v>66</v>
@@ -13032,17 +13032,17 @@
       </c>
       <c r="J93" s="19"/>
       <c r="K93" s="33" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="L93" s="4"/>
       <c r="M93" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="N93" s="5" t="s">
         <v>71</v>
       </c>
       <c r="O93" s="14" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P93" s="14"/>
     </row>
@@ -13594,7 +13594,7 @@
     </row>
     <row r="14" spans="1:16" ht="24">
       <c r="A14" s="10" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>585</v>
@@ -13605,7 +13605,7 @@
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="26" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>15</v>
@@ -13632,7 +13632,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="48" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="8"/>
@@ -20816,7 +20816,7 @@
       <c r="I2" s="25"/>
       <c r="J2" s="49"/>
       <c r="K2" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L2" s="5"/>
       <c r="M2" s="14" t="s">
@@ -20854,7 +20854,7 @@
       </c>
       <c r="J3" s="49"/>
       <c r="K3" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L3" s="5" t="s">
         <v>57</v>
@@ -20892,7 +20892,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="49"/>
       <c r="K4" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L4" s="5" t="s">
         <v>71</v>
@@ -20930,7 +20930,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="49"/>
       <c r="K5" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>57</v>
@@ -20970,7 +20970,7 @@
       </c>
       <c r="J6" s="49"/>
       <c r="K6" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L6" s="5"/>
       <c r="M6" s="14" t="s">
@@ -21004,7 +21004,7 @@
       <c r="I7" s="17"/>
       <c r="J7" s="49"/>
       <c r="K7" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>57</v>
@@ -21040,7 +21040,7 @@
       <c r="I8" s="17"/>
       <c r="J8" s="49"/>
       <c r="K8" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L8" s="5" t="s">
         <v>71</v>
@@ -21080,7 +21080,7 @@
       </c>
       <c r="J9" s="49"/>
       <c r="K9" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>71</v>
@@ -21116,7 +21116,7 @@
       <c r="I10" s="8"/>
       <c r="J10" s="49"/>
       <c r="K10" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L10" s="5" t="s">
         <v>71</v>
@@ -21154,7 +21154,7 @@
       </c>
       <c r="J11" s="49"/>
       <c r="K11" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>71</v>
@@ -21190,7 +21190,7 @@
       </c>
       <c r="J12" s="49"/>
       <c r="K12" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L12" s="5" t="s">
         <v>51</v>
@@ -21227,7 +21227,7 @@
       <c r="I13" s="8"/>
       <c r="J13" s="49"/>
       <c r="K13" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>57</v>
@@ -21257,7 +21257,7 @@
       <c r="I14" s="8"/>
       <c r="J14" s="49"/>
       <c r="K14" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14" s="14" t="s">
@@ -21291,7 +21291,7 @@
       </c>
       <c r="J15" s="49"/>
       <c r="K15" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>71</v>
@@ -21329,7 +21329,7 @@
       <c r="I16" s="17"/>
       <c r="J16" s="49"/>
       <c r="K16" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L16" s="5" t="s">
         <v>71</v>
@@ -21369,7 +21369,7 @@
       </c>
       <c r="J17" s="49"/>
       <c r="K17" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>71</v>
@@ -21399,7 +21399,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="49"/>
       <c r="K18" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L18" s="5"/>
       <c r="M18" s="14" t="s">
@@ -21425,7 +21425,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="49"/>
       <c r="K19" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L19" s="5"/>
       <c r="M19" s="14" t="s">
@@ -21463,7 +21463,7 @@
       </c>
       <c r="J20" s="49"/>
       <c r="K20" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L20" s="5" t="s">
         <v>71</v>
@@ -21501,7 +21501,7 @@
       </c>
       <c r="J21" s="49"/>
       <c r="K21" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>71</v>
@@ -21529,7 +21529,7 @@
       <c r="I22" s="8"/>
       <c r="J22" s="49"/>
       <c r="K22" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L22" s="5"/>
       <c r="M22" s="14" t="s">
@@ -21565,7 +21565,7 @@
       </c>
       <c r="J23" s="49"/>
       <c r="K23" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L23" s="5" t="s">
         <v>71</v>
@@ -21605,7 +21605,7 @@
       </c>
       <c r="J24" s="49"/>
       <c r="K24" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L24" s="5" t="s">
         <v>71</v>
@@ -21639,7 +21639,7 @@
       <c r="I25" s="8"/>
       <c r="J25" s="49"/>
       <c r="K25" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>71</v>
@@ -21667,7 +21667,7 @@
       </c>
       <c r="J26" s="49"/>
       <c r="K26" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="14" t="s">
@@ -21693,7 +21693,7 @@
       </c>
       <c r="J27" s="49"/>
       <c r="K27" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="14" t="s">
@@ -21729,7 +21729,7 @@
       </c>
       <c r="J28" s="49"/>
       <c r="K28" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L28" s="5" t="s">
         <v>71</v>
@@ -21765,7 +21765,7 @@
       <c r="I29" s="8"/>
       <c r="J29" s="49"/>
       <c r="K29" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>140</v>
@@ -21805,7 +21805,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="49"/>
       <c r="K30" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>140</v>
@@ -21847,7 +21847,7 @@
       </c>
       <c r="J31" s="49"/>
       <c r="K31" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L31" s="5" t="s">
         <v>71</v>
@@ -21885,7 +21885,7 @@
       </c>
       <c r="J32" s="49"/>
       <c r="K32" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L32" s="5" t="s">
         <v>71</v>
@@ -21925,7 +21925,7 @@
       </c>
       <c r="J33" s="49"/>
       <c r="K33" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L33" s="5" t="s">
         <v>71</v>
@@ -21965,7 +21965,7 @@
       </c>
       <c r="J34" s="49"/>
       <c r="K34" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L34" s="5" t="s">
         <v>71</v>
@@ -22001,7 +22001,7 @@
       <c r="I35" s="8"/>
       <c r="J35" s="49"/>
       <c r="K35" s="5" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="L35" s="5" t="s">
         <v>71</v>
@@ -22083,7 +22083,7 @@
       </c>
       <c r="J37" s="49"/>
       <c r="K37" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L37" s="5" t="s">
         <v>71</v>
@@ -22117,7 +22117,7 @@
       <c r="I38" s="25"/>
       <c r="J38" s="49"/>
       <c r="K38" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>71</v>
@@ -22153,7 +22153,7 @@
       </c>
       <c r="J39" s="49"/>
       <c r="K39" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L39" s="5" t="s">
         <v>71</v>
@@ -22187,7 +22187,7 @@
       <c r="I40" s="25"/>
       <c r="J40" s="49"/>
       <c r="K40" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L40" s="5" t="s">
         <v>71</v>
@@ -22221,7 +22221,7 @@
       <c r="I41" s="25"/>
       <c r="J41" s="49"/>
       <c r="K41" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>71</v>
@@ -22255,7 +22255,7 @@
       <c r="I42" s="25"/>
       <c r="J42" s="49"/>
       <c r="K42" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>71</v>
@@ -22289,7 +22289,7 @@
       <c r="I43" s="25"/>
       <c r="J43" s="49"/>
       <c r="K43" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L43" s="5" t="s">
         <v>71</v>
@@ -22323,7 +22323,7 @@
       <c r="I44" s="25"/>
       <c r="J44" s="49"/>
       <c r="K44" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L44" s="5" t="s">
         <v>71</v>
@@ -22359,7 +22359,7 @@
       </c>
       <c r="J45" s="49"/>
       <c r="K45" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>71</v>
@@ -22393,7 +22393,7 @@
       <c r="I46" s="25"/>
       <c r="J46" s="49"/>
       <c r="K46" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L46" s="5" t="s">
         <v>71</v>
@@ -22427,7 +22427,7 @@
       <c r="I47" s="25"/>
       <c r="J47" s="49"/>
       <c r="K47" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>71</v>
@@ -22461,7 +22461,7 @@
       <c r="I48" s="25"/>
       <c r="J48" s="49"/>
       <c r="K48" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>71</v>
@@ -22497,7 +22497,7 @@
       <c r="I49" s="25"/>
       <c r="J49" s="49"/>
       <c r="K49" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>71</v>
@@ -22533,7 +22533,7 @@
       <c r="I50" s="25"/>
       <c r="J50" s="49"/>
       <c r="K50" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L50" s="5" t="s">
         <v>71</v>
@@ -22567,7 +22567,7 @@
       <c r="I51" s="25"/>
       <c r="J51" s="49"/>
       <c r="K51" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L51" s="5" t="s">
         <v>71</v>
@@ -22601,7 +22601,7 @@
       <c r="I52" s="59"/>
       <c r="J52" s="49"/>
       <c r="K52" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L52" s="5" t="s">
         <v>71</v>
@@ -22635,7 +22635,7 @@
       <c r="I53" s="25"/>
       <c r="J53" s="49"/>
       <c r="K53" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L53" s="5" t="s">
         <v>71</v>
@@ -22669,7 +22669,7 @@
       <c r="I54" s="59"/>
       <c r="J54" s="49"/>
       <c r="K54" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L54" s="5" t="s">
         <v>71</v>
@@ -22705,7 +22705,7 @@
       </c>
       <c r="J55" s="49"/>
       <c r="K55" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L55" s="5" t="s">
         <v>71</v>
@@ -22741,7 +22741,7 @@
       </c>
       <c r="J56" s="49"/>
       <c r="K56" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L56" s="5" t="s">
         <v>71</v>
@@ -22777,7 +22777,7 @@
       </c>
       <c r="J57" s="49"/>
       <c r="K57" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L57" s="5" t="s">
         <v>71</v>
@@ -22813,7 +22813,7 @@
       </c>
       <c r="J58" s="49"/>
       <c r="K58" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L58" s="5" t="s">
         <v>71</v>
@@ -22849,7 +22849,7 @@
       </c>
       <c r="J59" s="49"/>
       <c r="K59" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L59" s="5" t="s">
         <v>71</v>
@@ -22885,7 +22885,7 @@
       </c>
       <c r="J60" s="49"/>
       <c r="K60" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L60" s="5" t="s">
         <v>71</v>
@@ -22921,7 +22921,7 @@
       </c>
       <c r="J61" s="49"/>
       <c r="K61" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L61" s="5" t="s">
         <v>71</v>
@@ -22957,7 +22957,7 @@
       </c>
       <c r="J62" s="49"/>
       <c r="K62" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L62" s="5" t="s">
         <v>71</v>
@@ -22993,7 +22993,7 @@
       </c>
       <c r="J63" s="49"/>
       <c r="K63" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L63" s="5" t="s">
         <v>71</v>
@@ -23027,7 +23027,7 @@
       <c r="I64" s="25"/>
       <c r="J64" s="49"/>
       <c r="K64" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L64" s="5" t="s">
         <v>71</v>
@@ -23063,7 +23063,7 @@
       <c r="I65" s="25"/>
       <c r="J65" s="49"/>
       <c r="K65" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L65" s="5" t="s">
         <v>71</v>
@@ -23099,7 +23099,7 @@
       <c r="I66" s="25"/>
       <c r="J66" s="49"/>
       <c r="K66" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L66" s="5" t="s">
         <v>71</v>
@@ -23139,7 +23139,7 @@
       </c>
       <c r="J67" s="49"/>
       <c r="K67" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L67" s="5" t="s">
         <v>71</v>
@@ -23175,7 +23175,7 @@
       <c r="I68" s="25"/>
       <c r="J68" s="49"/>
       <c r="K68" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L68" s="5" t="s">
         <v>71</v>
@@ -23211,7 +23211,7 @@
       </c>
       <c r="J69" s="49"/>
       <c r="K69" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L69" s="5" t="s">
         <v>71</v>
@@ -23247,7 +23247,7 @@
       </c>
       <c r="J70" s="49"/>
       <c r="K70" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L70" s="5" t="s">
         <v>71</v>
@@ -23283,7 +23283,7 @@
       </c>
       <c r="J71" s="49"/>
       <c r="K71" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L71" s="5" t="s">
         <v>71</v>
@@ -23319,7 +23319,7 @@
       </c>
       <c r="J72" s="49"/>
       <c r="K72" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L72" s="5" t="s">
         <v>71</v>
@@ -23355,7 +23355,7 @@
       </c>
       <c r="J73" s="49"/>
       <c r="K73" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L73" s="5" t="s">
         <v>71</v>
@@ -23391,7 +23391,7 @@
       </c>
       <c r="J74" s="49"/>
       <c r="K74" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L74" s="5" t="s">
         <v>71</v>
@@ -23427,7 +23427,7 @@
       </c>
       <c r="J75" s="49"/>
       <c r="K75" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L75" s="5" t="s">
         <v>71</v>
@@ -23463,7 +23463,7 @@
       </c>
       <c r="J76" s="49"/>
       <c r="K76" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L76" s="5" t="s">
         <v>71</v>
@@ -23499,7 +23499,7 @@
       </c>
       <c r="J77" s="49"/>
       <c r="K77" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L77" s="5" t="s">
         <v>71</v>
@@ -23535,7 +23535,7 @@
       </c>
       <c r="J78" s="49"/>
       <c r="K78" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L78" s="5" t="s">
         <v>71</v>
@@ -23571,7 +23571,7 @@
       </c>
       <c r="J79" s="49"/>
       <c r="K79" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L79" s="5" t="s">
         <v>71</v>
@@ -23607,7 +23607,7 @@
       </c>
       <c r="J80" s="49"/>
       <c r="K80" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L80" s="5" t="s">
         <v>71</v>
@@ -23643,7 +23643,7 @@
       </c>
       <c r="J81" s="49"/>
       <c r="K81" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L81" s="5" t="s">
         <v>71</v>
@@ -23679,7 +23679,7 @@
       <c r="I82" s="25"/>
       <c r="J82" s="49"/>
       <c r="K82" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L82" s="5" t="s">
         <v>71</v>
@@ -23715,7 +23715,7 @@
       </c>
       <c r="J83" s="49"/>
       <c r="K83" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L83" s="5" t="s">
         <v>71</v>
@@ -23751,7 +23751,7 @@
       <c r="I84" s="25"/>
       <c r="J84" s="49"/>
       <c r="K84" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L84" s="5" t="s">
         <v>71</v>
@@ -23787,7 +23787,7 @@
       </c>
       <c r="J85" s="49"/>
       <c r="K85" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L85" s="5" t="s">
         <v>71</v>
@@ -23823,7 +23823,7 @@
       <c r="I86" s="25"/>
       <c r="J86" s="49"/>
       <c r="K86" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L86" s="5" t="s">
         <v>71</v>
@@ -23857,7 +23857,7 @@
       <c r="I87" s="59"/>
       <c r="J87" s="49"/>
       <c r="K87" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L87" s="5" t="s">
         <v>71</v>
@@ -23895,7 +23895,7 @@
       </c>
       <c r="J88" s="49"/>
       <c r="K88" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L88" s="5" t="s">
         <v>71</v>
@@ -23931,7 +23931,7 @@
       </c>
       <c r="J89" s="49"/>
       <c r="K89" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L89" s="5" t="s">
         <v>71</v>
@@ -23965,7 +23965,7 @@
       <c r="I90" s="25"/>
       <c r="J90" s="49"/>
       <c r="K90" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L90" s="5" t="s">
         <v>71</v>
@@ -24001,7 +24001,7 @@
       </c>
       <c r="J91" s="49"/>
       <c r="K91" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L91" s="5" t="s">
         <v>71</v>
@@ -24035,7 +24035,7 @@
       <c r="I92" s="25"/>
       <c r="J92" s="49"/>
       <c r="K92" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L92" s="5" t="s">
         <v>71</v>
@@ -24071,7 +24071,7 @@
       </c>
       <c r="J93" s="49"/>
       <c r="K93" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L93" s="5" t="s">
         <v>71</v>
@@ -24105,7 +24105,7 @@
       <c r="I94" s="25"/>
       <c r="J94" s="49"/>
       <c r="K94" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L94" s="5" t="s">
         <v>71</v>
@@ -24141,7 +24141,7 @@
       <c r="I95" s="25"/>
       <c r="J95" s="49"/>
       <c r="K95" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L95" s="5" t="s">
         <v>71</v>
@@ -24177,7 +24177,7 @@
       <c r="I96" s="25"/>
       <c r="J96" s="49"/>
       <c r="K96" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L96" s="5" t="s">
         <v>71</v>
@@ -24213,7 +24213,7 @@
       </c>
       <c r="J97" s="49"/>
       <c r="K97" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L97" s="5" t="s">
         <v>71</v>
@@ -24247,7 +24247,7 @@
       <c r="I98" s="25"/>
       <c r="J98" s="49"/>
       <c r="K98" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L98" s="5" t="s">
         <v>71</v>
@@ -24285,7 +24285,7 @@
       </c>
       <c r="J99" s="49"/>
       <c r="K99" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L99" s="5" t="s">
         <v>71</v>
@@ -24323,7 +24323,7 @@
       </c>
       <c r="J100" s="49"/>
       <c r="K100" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L100" s="5" t="s">
         <v>71</v>
@@ -24357,7 +24357,7 @@
       <c r="I101" s="25"/>
       <c r="J101" s="49"/>
       <c r="K101" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L101" s="5" t="s">
         <v>71</v>
@@ -24395,7 +24395,7 @@
       </c>
       <c r="J102" s="49"/>
       <c r="K102" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L102" s="5" t="s">
         <v>71</v>
@@ -24431,7 +24431,7 @@
       <c r="I103" s="59"/>
       <c r="J103" s="49"/>
       <c r="K103" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L103" s="5" t="s">
         <v>71</v>
@@ -24467,7 +24467,7 @@
       </c>
       <c r="J104" s="49"/>
       <c r="K104" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L104" s="5" t="s">
         <v>71</v>
@@ -24503,7 +24503,7 @@
       </c>
       <c r="J105" s="49"/>
       <c r="K105" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L105" s="5" t="s">
         <v>71</v>
@@ -24539,7 +24539,7 @@
       </c>
       <c r="J106" s="49"/>
       <c r="K106" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L106" s="5" t="s">
         <v>71</v>
@@ -24575,7 +24575,7 @@
       </c>
       <c r="J107" s="49"/>
       <c r="K107" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L107" s="5" t="s">
         <v>71</v>
@@ -24611,7 +24611,7 @@
       </c>
       <c r="J108" s="49"/>
       <c r="K108" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L108" s="5" t="s">
         <v>71</v>
@@ -24647,7 +24647,7 @@
       </c>
       <c r="J109" s="49"/>
       <c r="K109" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L109" s="5" t="s">
         <v>71</v>
@@ -24683,7 +24683,7 @@
       </c>
       <c r="J110" s="49"/>
       <c r="K110" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L110" s="5" t="s">
         <v>71</v>
@@ -24719,7 +24719,7 @@
       </c>
       <c r="J111" s="49"/>
       <c r="K111" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L111" s="5" t="s">
         <v>71</v>
@@ -24755,7 +24755,7 @@
       </c>
       <c r="J112" s="49"/>
       <c r="K112" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L112" s="5" t="s">
         <v>71</v>
@@ -24791,7 +24791,7 @@
       </c>
       <c r="J113" s="49"/>
       <c r="K113" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L113" s="5" t="s">
         <v>71</v>
@@ -24825,7 +24825,7 @@
       <c r="I114" s="25"/>
       <c r="J114" s="49"/>
       <c r="K114" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L114" s="5" t="s">
         <v>71</v>
@@ -24861,7 +24861,7 @@
       </c>
       <c r="J115" s="49"/>
       <c r="K115" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L115" s="5" t="s">
         <v>71</v>
@@ -24895,7 +24895,7 @@
       <c r="I116" s="25"/>
       <c r="J116" s="49"/>
       <c r="K116" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L116" s="5" t="s">
         <v>71</v>
@@ -24929,7 +24929,7 @@
       <c r="I117" s="25"/>
       <c r="J117" s="49"/>
       <c r="K117" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L117" s="5" t="s">
         <v>71</v>
@@ -24965,7 +24965,7 @@
       </c>
       <c r="J118" s="49"/>
       <c r="K118" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L118" s="5" t="s">
         <v>71</v>
@@ -25001,7 +25001,7 @@
       </c>
       <c r="J119" s="49"/>
       <c r="K119" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L119" s="5" t="s">
         <v>71</v>
@@ -25035,7 +25035,7 @@
       <c r="I120" s="59"/>
       <c r="J120" s="49"/>
       <c r="K120" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L120" s="5" t="s">
         <v>71</v>
@@ -25071,7 +25071,7 @@
       </c>
       <c r="J121" s="49"/>
       <c r="K121" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L121" s="5" t="s">
         <v>71</v>
@@ -25107,7 +25107,7 @@
       </c>
       <c r="J122" s="49"/>
       <c r="K122" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L122" s="5" t="s">
         <v>71</v>
@@ -25143,7 +25143,7 @@
       </c>
       <c r="J123" s="49"/>
       <c r="K123" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L123" s="5" t="s">
         <v>71</v>
@@ -25179,7 +25179,7 @@
       </c>
       <c r="J124" s="49"/>
       <c r="K124" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L124" s="5" t="s">
         <v>71</v>
@@ -25215,7 +25215,7 @@
       </c>
       <c r="J125" s="49"/>
       <c r="K125" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L125" s="5" t="s">
         <v>71</v>
@@ -25251,7 +25251,7 @@
       </c>
       <c r="J126" s="49"/>
       <c r="K126" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L126" s="5" t="s">
         <v>71</v>
@@ -25287,7 +25287,7 @@
       </c>
       <c r="J127" s="49"/>
       <c r="K127" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L127" s="5" t="s">
         <v>71</v>
@@ -25323,7 +25323,7 @@
       </c>
       <c r="J128" s="49"/>
       <c r="K128" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L128" s="5" t="s">
         <v>71</v>
@@ -25359,7 +25359,7 @@
       </c>
       <c r="J129" s="49"/>
       <c r="K129" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L129" s="5" t="s">
         <v>71</v>
@@ -25395,7 +25395,7 @@
       </c>
       <c r="J130" s="49"/>
       <c r="K130" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L130" s="5" t="s">
         <v>71</v>
@@ -25431,7 +25431,7 @@
       <c r="I131" s="25"/>
       <c r="J131" s="49"/>
       <c r="K131" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L131" s="5" t="s">
         <v>71</v>
@@ -25467,7 +25467,7 @@
       </c>
       <c r="J132" s="49"/>
       <c r="K132" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L132" s="5" t="s">
         <v>71</v>
@@ -25503,7 +25503,7 @@
       <c r="I133" s="25"/>
       <c r="J133" s="49"/>
       <c r="K133" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L133" s="5" t="s">
         <v>71</v>
@@ -25539,7 +25539,7 @@
       </c>
       <c r="J134" s="49"/>
       <c r="K134" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L134" s="5" t="s">
         <v>71</v>
@@ -25575,7 +25575,7 @@
       <c r="I135" s="25"/>
       <c r="J135" s="49"/>
       <c r="K135" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L135" s="5" t="s">
         <v>71</v>
@@ -25609,7 +25609,7 @@
       <c r="I136" s="59"/>
       <c r="J136" s="49"/>
       <c r="K136" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L136" s="5" t="s">
         <v>71</v>
@@ -25643,7 +25643,7 @@
       <c r="I137" s="25"/>
       <c r="J137" s="49"/>
       <c r="K137" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L137" s="5" t="s">
         <v>71</v>
@@ -25677,7 +25677,7 @@
       <c r="I138" s="25"/>
       <c r="J138" s="49"/>
       <c r="K138" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L138" s="5" t="s">
         <v>71</v>
@@ -25711,7 +25711,7 @@
       <c r="I139" s="25"/>
       <c r="J139" s="49"/>
       <c r="K139" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L139" s="5" t="s">
         <v>71</v>
@@ -25745,7 +25745,7 @@
       <c r="I140" s="25"/>
       <c r="J140" s="49"/>
       <c r="K140" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L140" s="5" t="s">
         <v>71</v>
@@ -25781,7 +25781,7 @@
       </c>
       <c r="J141" s="49"/>
       <c r="K141" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L141" s="5" t="s">
         <v>71</v>
@@ -25815,7 +25815,7 @@
       <c r="I142" s="25"/>
       <c r="J142" s="49"/>
       <c r="K142" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L142" s="5" t="s">
         <v>71</v>
@@ -25849,7 +25849,7 @@
       <c r="I143" s="25"/>
       <c r="J143" s="49"/>
       <c r="K143" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L143" s="5" t="s">
         <v>71</v>
@@ -25885,7 +25885,7 @@
       </c>
       <c r="J144" s="49"/>
       <c r="K144" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L144" s="5" t="s">
         <v>71</v>
@@ -25921,7 +25921,7 @@
       </c>
       <c r="J145" s="49"/>
       <c r="K145" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L145" s="5" t="s">
         <v>71</v>
@@ -25957,7 +25957,7 @@
       </c>
       <c r="J146" s="49"/>
       <c r="K146" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L146" s="5" t="s">
         <v>71</v>
@@ -25993,7 +25993,7 @@
       </c>
       <c r="J147" s="49"/>
       <c r="K147" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L147" s="5" t="s">
         <v>71</v>
@@ -26029,7 +26029,7 @@
       </c>
       <c r="J148" s="49"/>
       <c r="K148" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L148" s="5" t="s">
         <v>71</v>
@@ -26065,7 +26065,7 @@
       </c>
       <c r="J149" s="49"/>
       <c r="K149" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L149" s="5" t="s">
         <v>71</v>
@@ -26101,7 +26101,7 @@
       </c>
       <c r="J150" s="49"/>
       <c r="K150" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L150" s="5" t="s">
         <v>71</v>
@@ -26137,7 +26137,7 @@
       </c>
       <c r="J151" s="49"/>
       <c r="K151" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L151" s="5" t="s">
         <v>71</v>
@@ -26173,7 +26173,7 @@
       </c>
       <c r="J152" s="49"/>
       <c r="K152" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L152" s="5" t="s">
         <v>71</v>
@@ -26209,7 +26209,7 @@
       </c>
       <c r="J153" s="49"/>
       <c r="K153" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L153" s="5" t="s">
         <v>71</v>
@@ -26243,7 +26243,7 @@
       <c r="I154" s="59"/>
       <c r="J154" s="56"/>
       <c r="K154" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L154" s="5" t="s">
         <v>71</v>
@@ -26277,7 +26277,7 @@
       <c r="I155" s="33"/>
       <c r="J155" s="56"/>
       <c r="K155" s="5" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L155" s="5" t="s">
         <v>71</v>
@@ -26775,7 +26775,7 @@
     </row>
     <row r="10" spans="1:16" ht="24">
       <c r="A10" s="67" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>787</v>
@@ -26789,14 +26789,14 @@
         <v>347</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="5" t="s">
         <v>49</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="K10" s="13"/>
       <c r="L10" s="59"/>

</xml_diff>